<commit_message>
extract excel document automatically(2)
"-" 문자 넣었고, 왼쪽 위 병합했고, 테두리 다 잡았음
그리고 원하는 연도만 골라 추출할 수 있게 함.
</commit_message>
<xml_diff>
--- a/data/output/연결 손익계산서.xlsx
+++ b/data/output/연결 손익계산서.xlsx
@@ -34,15 +34,15 @@
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
-      <patternFill patternType="solid"/>
-    </fill>
-    <fill>
       <patternFill patternType="solid">
         <fgColor rgb="00C0C0C0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid"/>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -50,19 +50,59 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -454,1673 +494,2210 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="D1" s="1" t="inlineStr">
+      <c r="A1" s="1" t="n"/>
+      <c r="B1" s="2" t="n"/>
+      <c r="C1" s="3" t="n"/>
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>Samsung</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="n"/>
+      <c r="F1" s="1" t="n"/>
+      <c r="G1" s="4" t="inlineStr">
         <is>
           <t>Hyundai</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="n"/>
+      <c r="I1" s="1" t="n"/>
+      <c r="J1" s="4" t="inlineStr">
         <is>
           <t>Sum</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="n"/>
+      <c r="L1" s="1" t="n"/>
+      <c r="M1" s="4" t="inlineStr">
         <is>
           <t>Average</t>
         </is>
       </c>
+      <c r="N1" s="1" t="n"/>
+      <c r="O1" s="1" t="n"/>
     </row>
     <row r="2">
-      <c r="D2" s="2" t="inlineStr">
+      <c r="A2" s="1" t="n"/>
+      <c r="B2" s="2" t="n"/>
+      <c r="C2" s="3" t="n"/>
+      <c r="D2" s="5" t="inlineStr">
         <is>
           <t>2023년</t>
         </is>
       </c>
-      <c r="E2" s="2" t="inlineStr">
+      <c r="E2" s="5" t="inlineStr">
         <is>
           <t>2022년</t>
         </is>
       </c>
-      <c r="F2" s="2" t="inlineStr">
+      <c r="F2" s="5" t="inlineStr">
         <is>
           <t>2021년</t>
         </is>
       </c>
-      <c r="G2" s="2" t="inlineStr">
+      <c r="G2" s="5" t="inlineStr">
         <is>
           <t>2023년</t>
         </is>
       </c>
-      <c r="H2" s="2" t="inlineStr">
+      <c r="H2" s="5" t="inlineStr">
         <is>
           <t>2022년</t>
         </is>
       </c>
-      <c r="I2" s="2" t="inlineStr">
+      <c r="I2" s="5" t="inlineStr">
         <is>
           <t>2021년</t>
         </is>
       </c>
-      <c r="J2" s="2" t="inlineStr">
+      <c r="J2" s="5" t="inlineStr">
         <is>
           <t>2023년</t>
         </is>
       </c>
-      <c r="K2" s="2" t="inlineStr">
+      <c r="K2" s="5" t="inlineStr">
         <is>
           <t>2022년</t>
         </is>
       </c>
-      <c r="L2" s="2" t="inlineStr">
+      <c r="L2" s="5" t="inlineStr">
         <is>
           <t>2021년</t>
         </is>
       </c>
-      <c r="M2" s="2" t="inlineStr">
+      <c r="M2" s="5" t="inlineStr">
         <is>
           <t>2023년</t>
         </is>
       </c>
-      <c r="N2" s="2" t="inlineStr">
+      <c r="N2" s="5" t="inlineStr">
         <is>
           <t>2022년</t>
         </is>
       </c>
-      <c r="O2" s="2" t="inlineStr">
+      <c r="O2" s="5" t="inlineStr">
         <is>
           <t>2021년</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="n"/>
-      <c r="B3" s="3" t="n"/>
-      <c r="C3" s="3" t="n"/>
-      <c r="D3" s="3" t="n"/>
-      <c r="E3" s="3" t="n"/>
-      <c r="F3" s="3" t="n"/>
-      <c r="G3" s="3" t="n"/>
-      <c r="H3" s="3" t="n"/>
-      <c r="I3" s="3" t="n"/>
-      <c r="J3" s="3" t="n"/>
-      <c r="K3" s="3" t="n"/>
-      <c r="L3" s="3" t="n"/>
-      <c r="M3" s="3" t="n"/>
-      <c r="N3" s="3" t="n"/>
-      <c r="O3" s="3" t="n"/>
+      <c r="A3" s="6" t="n"/>
+      <c r="B3" s="6" t="n"/>
+      <c r="C3" s="6" t="n"/>
+      <c r="D3" s="6" t="n"/>
+      <c r="E3" s="6" t="n"/>
+      <c r="F3" s="6" t="n"/>
+      <c r="G3" s="6" t="n"/>
+      <c r="H3" s="6" t="n"/>
+      <c r="I3" s="6" t="n"/>
+      <c r="J3" s="6" t="n"/>
+      <c r="K3" s="6" t="n"/>
+      <c r="L3" s="6" t="n"/>
+      <c r="M3" s="6" t="n"/>
+      <c r="N3" s="6" t="n"/>
+      <c r="O3" s="6" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="1" t="inlineStr">
         <is>
           <t>영업수익</t>
         </is>
       </c>
-      <c r="D4" t="n">
+      <c r="B4" s="1" t="n"/>
+      <c r="C4" s="1" t="n"/>
+      <c r="D4" s="1" t="n">
         <v>258935494</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4" s="1" t="n">
         <v>302231360</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F4" s="1" t="n">
         <v>279604799</v>
       </c>
-      <c r="J4" t="n">
+      <c r="G4" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H4" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I4" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J4" s="1" t="n">
         <v>258935494</v>
       </c>
-      <c r="K4" t="n">
+      <c r="K4" s="1" t="n">
         <v>302231360</v>
       </c>
-      <c r="L4" t="n">
+      <c r="L4" s="1" t="n">
         <v>279604799</v>
       </c>
-      <c r="M4" t="n">
+      <c r="M4" s="1" t="n">
         <v>258935494</v>
       </c>
-      <c r="N4" t="n">
+      <c r="N4" s="1" t="n">
         <v>302231360</v>
       </c>
-      <c r="O4" t="n">
+      <c r="O4" s="1" t="n">
         <v>279604799</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="1" t="inlineStr">
         <is>
           <t>매출원가</t>
         </is>
       </c>
-      <c r="D5" t="n">
+      <c r="B5" s="1" t="n"/>
+      <c r="C5" s="1" t="n"/>
+      <c r="D5" s="1" t="n">
         <v>180388580</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E5" s="1" t="n">
         <v>190041770</v>
       </c>
-      <c r="F5" t="n">
+      <c r="F5" s="1" t="n">
         <v>166411342</v>
       </c>
-      <c r="G5" t="n">
+      <c r="G5" s="1" t="n">
         <v>129179183</v>
       </c>
-      <c r="H5" t="n">
+      <c r="H5" s="1" t="n">
         <v>113879569</v>
       </c>
-      <c r="I5" t="n">
+      <c r="I5" s="1" t="n">
         <v>94721313</v>
       </c>
-      <c r="J5" t="n">
+      <c r="J5" s="1" t="n">
         <v>309567763</v>
       </c>
-      <c r="K5" t="n">
+      <c r="K5" s="1" t="n">
         <v>303921339</v>
       </c>
-      <c r="L5" t="n">
+      <c r="L5" s="1" t="n">
         <v>261132655</v>
       </c>
-      <c r="M5" t="n">
+      <c r="M5" s="1" t="n">
         <v>154783881.5</v>
       </c>
-      <c r="N5" t="n">
+      <c r="N5" s="1" t="n">
         <v>151960669.5</v>
       </c>
-      <c r="O5" t="n">
+      <c r="O5" s="1" t="n">
         <v>130566327.5</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="1" t="inlineStr">
         <is>
           <t>매출총이익</t>
         </is>
       </c>
-      <c r="D6" t="n">
+      <c r="B6" s="1" t="n"/>
+      <c r="C6" s="1" t="n"/>
+      <c r="D6" s="1" t="n">
         <v>78546914</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E6" s="1" t="n">
         <v>112189590</v>
       </c>
-      <c r="F6" t="n">
+      <c r="F6" s="1" t="n">
         <v>113193457</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G6" s="1" t="n">
         <v>33484396</v>
       </c>
-      <c r="H6" t="n">
+      <c r="H6" s="1" t="n">
         <v>28271900</v>
       </c>
-      <c r="I6" t="n">
+      <c r="I6" s="1" t="n">
         <v>21726846</v>
       </c>
-      <c r="J6" t="n">
+      <c r="J6" s="1" t="n">
         <v>112031310</v>
       </c>
-      <c r="K6" t="n">
+      <c r="K6" s="1" t="n">
         <v>140461490</v>
       </c>
-      <c r="L6" t="n">
+      <c r="L6" s="1" t="n">
         <v>134920303</v>
       </c>
-      <c r="M6" t="n">
+      <c r="M6" s="1" t="n">
         <v>56015655</v>
       </c>
-      <c r="N6" t="n">
+      <c r="N6" s="1" t="n">
         <v>70230745</v>
       </c>
-      <c r="O6" t="n">
+      <c r="O6" s="1" t="n">
         <v>67460151.5</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="1" t="inlineStr">
         <is>
           <t>판매비와관리비</t>
         </is>
       </c>
-      <c r="D7" t="n">
+      <c r="B7" s="1" t="n"/>
+      <c r="C7" s="1" t="n"/>
+      <c r="D7" s="1" t="n">
         <v>71979938</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E7" s="1" t="n">
         <v>68812960</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F7" s="1" t="n">
         <v>61559601</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G7" s="1" t="n">
         <v>18357495</v>
       </c>
-      <c r="H7" t="n">
+      <c r="H7" s="1" t="n">
         <v>18446972</v>
       </c>
-      <c r="I7" t="n">
+      <c r="I7" s="1" t="n">
         <v>15200325</v>
       </c>
-      <c r="J7" t="n">
+      <c r="J7" s="1" t="n">
         <v>90337433</v>
       </c>
-      <c r="K7" t="n">
+      <c r="K7" s="1" t="n">
         <v>87259932</v>
       </c>
-      <c r="L7" t="n">
+      <c r="L7" s="1" t="n">
         <v>76759926</v>
       </c>
-      <c r="M7" t="n">
+      <c r="M7" s="1" t="n">
         <v>45168716.5</v>
       </c>
-      <c r="N7" t="n">
+      <c r="N7" s="1" t="n">
         <v>43629966</v>
       </c>
-      <c r="O7" t="n">
+      <c r="O7" s="1" t="n">
         <v>38379963</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="1" t="inlineStr">
         <is>
           <t>영업이익</t>
         </is>
       </c>
-      <c r="D8" t="n">
+      <c r="B8" s="1" t="n"/>
+      <c r="C8" s="1" t="n"/>
+      <c r="D8" s="1" t="n">
         <v>6566976</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E8" s="1" t="n">
         <v>43376630</v>
       </c>
-      <c r="F8" t="n">
+      <c r="F8" s="1" t="n">
         <v>51633856</v>
       </c>
-      <c r="G8" t="n">
+      <c r="G8" s="1" t="n">
         <v>15126901</v>
       </c>
-      <c r="H8" t="n">
+      <c r="H8" s="1" t="n">
         <v>9824928</v>
       </c>
-      <c r="I8" t="n">
+      <c r="I8" s="1" t="n">
         <v>6526521</v>
       </c>
-      <c r="J8" t="n">
+      <c r="J8" s="1" t="n">
         <v>21693877</v>
       </c>
-      <c r="K8" t="n">
+      <c r="K8" s="1" t="n">
         <v>53201558</v>
       </c>
-      <c r="L8" t="n">
+      <c r="L8" s="1" t="n">
         <v>58160377</v>
       </c>
-      <c r="M8" t="n">
+      <c r="M8" s="1" t="n">
         <v>10846938.5</v>
       </c>
-      <c r="N8" t="n">
+      <c r="N8" s="1" t="n">
         <v>26600779</v>
       </c>
-      <c r="O8" t="n">
+      <c r="O8" s="1" t="n">
         <v>29080188.5</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="1" t="inlineStr">
         <is>
           <t>기타이익</t>
         </is>
       </c>
-      <c r="D9" t="n">
+      <c r="B9" s="1" t="n"/>
+      <c r="C9" s="1" t="n"/>
+      <c r="D9" s="1" t="n">
         <v>1180448</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E9" s="1" t="n">
         <v>1962071</v>
       </c>
-      <c r="F9" t="n">
+      <c r="F9" s="1" t="n">
         <v>2205695</v>
       </c>
-      <c r="J9" t="n">
+      <c r="G9" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H9" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I9" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J9" s="1" t="n">
         <v>1180448</v>
       </c>
-      <c r="K9" t="n">
+      <c r="K9" s="1" t="n">
         <v>1962071</v>
       </c>
-      <c r="L9" t="n">
+      <c r="L9" s="1" t="n">
         <v>2205695</v>
       </c>
-      <c r="M9" t="n">
+      <c r="M9" s="1" t="n">
         <v>1180448</v>
       </c>
-      <c r="N9" t="n">
+      <c r="N9" s="1" t="n">
         <v>1962071</v>
       </c>
-      <c r="O9" t="n">
+      <c r="O9" s="1" t="n">
         <v>2205695</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="1" t="inlineStr">
         <is>
           <t>기타손실</t>
         </is>
       </c>
-      <c r="D10" t="n">
+      <c r="B10" s="1" t="n"/>
+      <c r="C10" s="1" t="n"/>
+      <c r="D10" s="1" t="n">
         <v>1083327</v>
       </c>
-      <c r="E10" t="n">
+      <c r="E10" s="1" t="n">
         <v>1790176</v>
       </c>
-      <c r="F10" t="n">
+      <c r="F10" s="1" t="n">
         <v>2055971</v>
       </c>
-      <c r="J10" t="n">
+      <c r="G10" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H10" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I10" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J10" s="1" t="n">
         <v>1083327</v>
       </c>
-      <c r="K10" t="n">
+      <c r="K10" s="1" t="n">
         <v>1790176</v>
       </c>
-      <c r="L10" t="n">
+      <c r="L10" s="1" t="n">
         <v>2055971</v>
       </c>
-      <c r="M10" t="n">
+      <c r="M10" s="1" t="n">
         <v>1083327</v>
       </c>
-      <c r="N10" t="n">
+      <c r="N10" s="1" t="n">
         <v>1790176</v>
       </c>
-      <c r="O10" t="n">
+      <c r="O10" s="1" t="n">
         <v>2055971</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" s="1" t="inlineStr">
         <is>
           <t>지분법이익</t>
         </is>
       </c>
-      <c r="D11" t="n">
+      <c r="B11" s="1" t="n"/>
+      <c r="C11" s="1" t="n"/>
+      <c r="D11" s="1" t="n">
         <v>887550</v>
       </c>
-      <c r="E11" t="n">
+      <c r="E11" s="1" t="n">
         <v>1090643</v>
       </c>
-      <c r="F11" t="n">
+      <c r="F11" s="1" t="n">
         <v>729614</v>
       </c>
-      <c r="J11" t="n">
+      <c r="G11" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H11" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I11" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J11" s="1" t="n">
         <v>887550</v>
       </c>
-      <c r="K11" t="n">
+      <c r="K11" s="1" t="n">
         <v>1090643</v>
       </c>
-      <c r="L11" t="n">
+      <c r="L11" s="1" t="n">
         <v>729614</v>
       </c>
-      <c r="M11" t="n">
+      <c r="M11" s="1" t="n">
         <v>887550</v>
       </c>
-      <c r="N11" t="n">
+      <c r="N11" s="1" t="n">
         <v>1090643</v>
       </c>
-      <c r="O11" t="n">
+      <c r="O11" s="1" t="n">
         <v>729614</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" s="1" t="inlineStr">
         <is>
           <t>금융수익</t>
         </is>
       </c>
-      <c r="D12" t="n">
+      <c r="B12" s="1" t="n"/>
+      <c r="C12" s="1" t="n"/>
+      <c r="D12" s="1" t="n">
         <v>16100148</v>
       </c>
-      <c r="E12" t="n">
+      <c r="E12" s="1" t="n">
         <v>20828995</v>
       </c>
-      <c r="F12" t="n">
+      <c r="F12" s="1" t="n">
         <v>8543187</v>
       </c>
-      <c r="G12" t="n">
+      <c r="G12" s="1" t="n">
         <v>1559538</v>
       </c>
-      <c r="H12" t="n">
+      <c r="H12" s="1" t="n">
         <v>985893</v>
       </c>
-      <c r="I12" t="n">
+      <c r="I12" s="1" t="n">
         <v>841196</v>
       </c>
-      <c r="J12" t="n">
+      <c r="J12" s="1" t="n">
         <v>17659686</v>
       </c>
-      <c r="K12" t="n">
+      <c r="K12" s="1" t="n">
         <v>21814888</v>
       </c>
-      <c r="L12" t="n">
+      <c r="L12" s="1" t="n">
         <v>9384383</v>
       </c>
-      <c r="M12" t="n">
+      <c r="M12" s="1" t="n">
         <v>8829843</v>
       </c>
-      <c r="N12" t="n">
+      <c r="N12" s="1" t="n">
         <v>10907444</v>
       </c>
-      <c r="O12" t="n">
+      <c r="O12" s="1" t="n">
         <v>4692191.5</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" s="1" t="inlineStr">
         <is>
           <t>금융비용</t>
         </is>
       </c>
-      <c r="D13" t="n">
+      <c r="B13" s="1" t="n"/>
+      <c r="C13" s="1" t="n"/>
+      <c r="D13" s="1" t="n">
         <v>12645530</v>
       </c>
-      <c r="E13" t="n">
+      <c r="E13" s="1" t="n">
         <v>19027689</v>
       </c>
-      <c r="F13" t="n">
+      <c r="F13" s="1" t="n">
         <v>7704554</v>
       </c>
-      <c r="G13" t="n">
+      <c r="G13" s="1" t="n">
         <v>970700</v>
       </c>
-      <c r="H13" t="n">
+      <c r="H13" s="1" t="n">
         <v>879638</v>
       </c>
-      <c r="I13" t="n">
+      <c r="I13" s="1" t="n">
         <v>512836</v>
       </c>
-      <c r="J13" t="n">
+      <c r="J13" s="1" t="n">
         <v>13616230</v>
       </c>
-      <c r="K13" t="n">
+      <c r="K13" s="1" t="n">
         <v>19907327</v>
       </c>
-      <c r="L13" t="n">
+      <c r="L13" s="1" t="n">
         <v>8217390</v>
       </c>
-      <c r="M13" t="n">
+      <c r="M13" s="1" t="n">
         <v>6808115</v>
       </c>
-      <c r="N13" t="n">
+      <c r="N13" s="1" t="n">
         <v>9953663.5</v>
       </c>
-      <c r="O13" t="n">
+      <c r="O13" s="1" t="n">
         <v>4108695</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" s="1" t="inlineStr">
         <is>
           <t>법인세비용차감전순이익(손실)</t>
         </is>
       </c>
-      <c r="D14" t="n">
+      <c r="B14" s="1" t="n"/>
+      <c r="C14" s="1" t="n"/>
+      <c r="D14" s="1" t="n">
         <v>11006265</v>
       </c>
-      <c r="E14" t="n">
+      <c r="E14" s="1" t="n">
         <v>46440474</v>
       </c>
-      <c r="F14" t="n">
+      <c r="F14" s="1" t="n">
         <v>53351827</v>
       </c>
-      <c r="J14" t="n">
+      <c r="G14" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H14" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I14" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J14" s="1" t="n">
         <v>11006265</v>
       </c>
-      <c r="K14" t="n">
+      <c r="K14" s="1" t="n">
         <v>46440474</v>
       </c>
-      <c r="L14" t="n">
+      <c r="L14" s="1" t="n">
         <v>53351827</v>
       </c>
-      <c r="M14" t="n">
+      <c r="M14" s="1" t="n">
         <v>11006265</v>
       </c>
-      <c r="N14" t="n">
+      <c r="N14" s="1" t="n">
         <v>46440474</v>
       </c>
-      <c r="O14" t="n">
+      <c r="O14" s="1" t="n">
         <v>53351827</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
+      <c r="A15" s="1" t="inlineStr">
         <is>
           <t>법인세비용(수익)</t>
         </is>
       </c>
-      <c r="D15" t="n">
+      <c r="B15" s="1" t="n"/>
+      <c r="C15" s="1" t="n"/>
+      <c r="D15" s="1" t="n">
         <v>-4480835</v>
       </c>
-      <c r="E15" t="n">
+      <c r="E15" s="1" t="n">
         <v>-9213603</v>
       </c>
-      <c r="F15" t="n">
+      <c r="F15" s="1" t="n">
         <v>13444377</v>
       </c>
-      <c r="G15" t="n">
+      <c r="G15" s="1" t="n">
         <v>4626640</v>
       </c>
-      <c r="H15" t="n">
+      <c r="H15" s="1" t="n">
         <v>2979168</v>
       </c>
-      <c r="I15" t="n">
+      <c r="I15" s="1" t="n">
         <v>2266823</v>
       </c>
-      <c r="J15" t="n">
+      <c r="J15" s="1" t="n">
         <v>145805</v>
       </c>
-      <c r="K15" t="n">
+      <c r="K15" s="1" t="n">
         <v>-6234435</v>
       </c>
-      <c r="L15" t="n">
+      <c r="L15" s="1" t="n">
         <v>15711200</v>
       </c>
-      <c r="M15" t="n">
+      <c r="M15" s="1" t="n">
         <v>72902.5</v>
       </c>
-      <c r="N15" t="n">
+      <c r="N15" s="1" t="n">
         <v>-3117217.5</v>
       </c>
-      <c r="O15" t="n">
+      <c r="O15" s="1" t="n">
         <v>7855600</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
+      <c r="A16" s="1" t="inlineStr">
         <is>
           <t>계속영업이익(손실)</t>
         </is>
       </c>
-      <c r="D16" t="n">
+      <c r="B16" s="1" t="n"/>
+      <c r="C16" s="1" t="n"/>
+      <c r="D16" s="1" t="n">
         <v>15487100</v>
       </c>
-      <c r="E16" t="n">
+      <c r="E16" s="1" t="n">
         <v>55654077</v>
       </c>
-      <c r="F16" t="n">
+      <c r="F16" s="1" t="n">
         <v>39907450</v>
       </c>
-      <c r="J16" t="n">
+      <c r="G16" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H16" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I16" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J16" s="1" t="n">
         <v>15487100</v>
       </c>
-      <c r="K16" t="n">
+      <c r="K16" s="1" t="n">
         <v>55654077</v>
       </c>
-      <c r="L16" t="n">
+      <c r="L16" s="1" t="n">
         <v>39907450</v>
       </c>
-      <c r="M16" t="n">
+      <c r="M16" s="1" t="n">
         <v>15487100</v>
       </c>
-      <c r="N16" t="n">
+      <c r="N16" s="1" t="n">
         <v>55654077</v>
       </c>
-      <c r="O16" t="n">
+      <c r="O16" s="1" t="n">
         <v>39907450</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
+      <c r="A17" s="1" t="inlineStr">
         <is>
           <t>당기순이익(손실)</t>
         </is>
       </c>
-      <c r="D17" t="n">
+      <c r="B17" s="1" t="n"/>
+      <c r="C17" s="1" t="n"/>
+      <c r="D17" s="1" t="n">
         <v>15487100</v>
       </c>
-      <c r="E17" t="n">
+      <c r="E17" s="1" t="n">
         <v>55654077</v>
       </c>
-      <c r="F17" t="n">
+      <c r="F17" s="1" t="n">
         <v>39907450</v>
       </c>
-      <c r="J17" t="n">
+      <c r="G17" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H17" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I17" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J17" s="1" t="n">
         <v>15487100</v>
       </c>
-      <c r="K17" t="n">
+      <c r="K17" s="1" t="n">
         <v>55654077</v>
       </c>
-      <c r="L17" t="n">
+      <c r="L17" s="1" t="n">
         <v>39907450</v>
       </c>
-      <c r="M17" t="n">
+      <c r="M17" s="1" t="n">
         <v>15487100</v>
       </c>
-      <c r="N17" t="n">
+      <c r="N17" s="1" t="n">
         <v>55654077</v>
       </c>
-      <c r="O17" t="n">
+      <c r="O17" s="1" t="n">
         <v>39907450</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
+      <c r="A18" s="1" t="inlineStr">
         <is>
           <t>당기순이익(손실)의 귀속</t>
         </is>
       </c>
-      <c r="D18" t="n">
-        <v/>
-      </c>
-      <c r="E18" t="n">
-        <v/>
-      </c>
-      <c r="F18" t="n">
-        <v/>
-      </c>
-      <c r="G18" t="n">
-        <v/>
-      </c>
-      <c r="H18" t="n">
-        <v/>
-      </c>
-      <c r="I18" t="n">
-        <v/>
-      </c>
-      <c r="J18" t="n">
-        <v/>
-      </c>
-      <c r="K18" t="n">
-        <v/>
-      </c>
-      <c r="L18" t="n">
-        <v/>
-      </c>
-      <c r="M18" t="n">
-        <v/>
-      </c>
-      <c r="N18" t="n">
-        <v/>
-      </c>
-      <c r="O18" t="n">
+      <c r="B18" s="1" t="n"/>
+      <c r="C18" s="1" t="n"/>
+      <c r="D18" s="1" t="n">
+        <v/>
+      </c>
+      <c r="E18" s="1" t="n">
+        <v/>
+      </c>
+      <c r="F18" s="1" t="n">
+        <v/>
+      </c>
+      <c r="G18" s="1" t="n">
+        <v/>
+      </c>
+      <c r="H18" s="1" t="n">
+        <v/>
+      </c>
+      <c r="I18" s="1" t="n">
+        <v/>
+      </c>
+      <c r="J18" s="1" t="n">
+        <v/>
+      </c>
+      <c r="K18" s="1" t="n">
+        <v/>
+      </c>
+      <c r="L18" s="1" t="n">
+        <v/>
+      </c>
+      <c r="M18" s="1" t="n">
+        <v/>
+      </c>
+      <c r="N18" s="1" t="n">
+        <v/>
+      </c>
+      <c r="O18" s="1" t="n">
         <v/>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
+      <c r="A19" s="1" t="inlineStr">
         <is>
           <t>당기순이익(손실)의 귀속</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="B19" s="1" t="inlineStr">
         <is>
           <t>지배기업의 소유주에게 귀속되는 당기순이익(손실)</t>
         </is>
       </c>
-      <c r="D19" t="n">
+      <c r="C19" s="1" t="n"/>
+      <c r="D19" s="1" t="n">
         <v>14473401</v>
       </c>
-      <c r="E19" t="n">
+      <c r="E19" s="1" t="n">
         <v>54730018</v>
       </c>
-      <c r="F19" t="n">
+      <c r="F19" s="1" t="n">
         <v>39243791</v>
       </c>
-      <c r="J19" t="n">
+      <c r="G19" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H19" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I19" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J19" s="1" t="n">
         <v>14473401</v>
       </c>
-      <c r="K19" t="n">
+      <c r="K19" s="1" t="n">
         <v>54730018</v>
       </c>
-      <c r="L19" t="n">
+      <c r="L19" s="1" t="n">
         <v>39243791</v>
       </c>
-      <c r="M19" t="n">
+      <c r="M19" s="1" t="n">
         <v>14473401</v>
       </c>
-      <c r="N19" t="n">
+      <c r="N19" s="1" t="n">
         <v>54730018</v>
       </c>
-      <c r="O19" t="n">
+      <c r="O19" s="1" t="n">
         <v>39243791</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
+      <c r="A20" s="1" t="inlineStr">
         <is>
           <t>당기순이익(손실)의 귀속</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="B20" s="1" t="inlineStr">
         <is>
           <t>비지배지분에 귀속되는 당기순이익(손실)</t>
         </is>
       </c>
-      <c r="D20" t="n">
+      <c r="C20" s="1" t="n"/>
+      <c r="D20" s="1" t="n">
         <v>1013699</v>
       </c>
-      <c r="E20" t="n">
+      <c r="E20" s="1" t="n">
         <v>924059</v>
       </c>
-      <c r="F20" t="n">
+      <c r="F20" s="1" t="n">
         <v>663659</v>
       </c>
-      <c r="J20" t="n">
+      <c r="G20" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H20" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I20" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J20" s="1" t="n">
         <v>1013699</v>
       </c>
-      <c r="K20" t="n">
+      <c r="K20" s="1" t="n">
         <v>924059</v>
       </c>
-      <c r="L20" t="n">
+      <c r="L20" s="1" t="n">
         <v>663659</v>
       </c>
-      <c r="M20" t="n">
+      <c r="M20" s="1" t="n">
         <v>1013699</v>
       </c>
-      <c r="N20" t="n">
+      <c r="N20" s="1" t="n">
         <v>924059</v>
       </c>
-      <c r="O20" t="n">
+      <c r="O20" s="1" t="n">
         <v>663659</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
+      <c r="A21" s="1" t="inlineStr">
         <is>
           <t>당기순이익(손실)의 귀속</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="B21" s="1" t="inlineStr">
         <is>
           <t>지배기업소유주지분</t>
         </is>
       </c>
-      <c r="G21" t="n">
+      <c r="C21" s="1" t="n"/>
+      <c r="D21" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E21" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F21" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G21" s="1" t="n">
         <v>11961717</v>
       </c>
-      <c r="H21" t="n">
+      <c r="H21" s="1" t="n">
         <v>7364364</v>
       </c>
-      <c r="I21" t="n">
+      <c r="I21" s="1" t="n">
         <v>4942356</v>
       </c>
-      <c r="J21" t="n">
+      <c r="J21" s="1" t="n">
         <v>11961717</v>
       </c>
-      <c r="K21" t="n">
+      <c r="K21" s="1" t="n">
         <v>7364364</v>
       </c>
-      <c r="L21" t="n">
+      <c r="L21" s="1" t="n">
         <v>4942356</v>
       </c>
-      <c r="M21" t="n">
+      <c r="M21" s="1" t="n">
         <v>11961717</v>
       </c>
-      <c r="N21" t="n">
+      <c r="N21" s="1" t="n">
         <v>7364364</v>
       </c>
-      <c r="O21" t="n">
+      <c r="O21" s="1" t="n">
         <v>4942356</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
+      <c r="A22" s="1" t="inlineStr">
         <is>
           <t>당기순이익(손실)의 귀속</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="B22" s="1" t="inlineStr">
         <is>
           <t>비지배지분</t>
         </is>
       </c>
-      <c r="G22" t="n">
+      <c r="C22" s="1" t="n"/>
+      <c r="D22" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E22" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F22" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G22" s="1" t="n">
         <v>310584</v>
       </c>
-      <c r="H22" t="n">
+      <c r="H22" s="1" t="n">
         <v>619250</v>
       </c>
-      <c r="I22" t="n">
+      <c r="I22" s="1" t="n">
         <v>750721</v>
       </c>
-      <c r="J22" t="n">
+      <c r="J22" s="1" t="n">
         <v>310584</v>
       </c>
-      <c r="K22" t="n">
+      <c r="K22" s="1" t="n">
         <v>619250</v>
       </c>
-      <c r="L22" t="n">
+      <c r="L22" s="1" t="n">
         <v>750721</v>
       </c>
-      <c r="M22" t="n">
+      <c r="M22" s="1" t="n">
         <v>310584</v>
       </c>
-      <c r="N22" t="n">
+      <c r="N22" s="1" t="n">
         <v>619250</v>
       </c>
-      <c r="O22" t="n">
+      <c r="O22" s="1" t="n">
         <v>750721</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
+      <c r="A23" s="1" t="inlineStr">
         <is>
           <t>주당이익</t>
         </is>
       </c>
-      <c r="D23" t="n">
-        <v/>
-      </c>
-      <c r="E23" t="n">
-        <v/>
-      </c>
-      <c r="F23" t="n">
-        <v/>
-      </c>
-      <c r="G23" t="n">
-        <v/>
-      </c>
-      <c r="H23" t="n">
-        <v/>
-      </c>
-      <c r="I23" t="n">
-        <v/>
-      </c>
-      <c r="J23" t="n">
-        <v/>
-      </c>
-      <c r="K23" t="n">
-        <v/>
-      </c>
-      <c r="L23" t="n">
-        <v/>
-      </c>
-      <c r="M23" t="n">
-        <v/>
-      </c>
-      <c r="N23" t="n">
-        <v/>
-      </c>
-      <c r="O23" t="n">
+      <c r="B23" s="1" t="n"/>
+      <c r="C23" s="1" t="n"/>
+      <c r="D23" s="1" t="n">
+        <v/>
+      </c>
+      <c r="E23" s="1" t="n">
+        <v/>
+      </c>
+      <c r="F23" s="1" t="n">
+        <v/>
+      </c>
+      <c r="G23" s="1" t="n">
+        <v/>
+      </c>
+      <c r="H23" s="1" t="n">
+        <v/>
+      </c>
+      <c r="I23" s="1" t="n">
+        <v/>
+      </c>
+      <c r="J23" s="1" t="n">
+        <v/>
+      </c>
+      <c r="K23" s="1" t="n">
+        <v/>
+      </c>
+      <c r="L23" s="1" t="n">
+        <v/>
+      </c>
+      <c r="M23" s="1" t="n">
+        <v/>
+      </c>
+      <c r="N23" s="1" t="n">
+        <v/>
+      </c>
+      <c r="O23" s="1" t="n">
         <v/>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
+      <c r="A24" s="1" t="inlineStr">
         <is>
           <t>주당이익</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="B24" s="1" t="inlineStr">
         <is>
           <t>기본주당이익(손실) (단위 : 원)</t>
         </is>
       </c>
-      <c r="D24" t="n">
+      <c r="C24" s="1" t="n"/>
+      <c r="D24" s="1" t="n">
         <v>2131</v>
       </c>
-      <c r="E24" t="n">
+      <c r="E24" s="1" t="n">
         <v>8057</v>
       </c>
-      <c r="F24" t="n">
+      <c r="F24" s="1" t="n">
         <v>5777</v>
       </c>
-      <c r="J24" t="n">
+      <c r="G24" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H24" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I24" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J24" s="1" t="n">
         <v>2131</v>
       </c>
-      <c r="K24" t="n">
+      <c r="K24" s="1" t="n">
         <v>8057</v>
       </c>
-      <c r="L24" t="n">
+      <c r="L24" s="1" t="n">
         <v>5777</v>
       </c>
-      <c r="M24" t="n">
+      <c r="M24" s="1" t="n">
         <v>2131</v>
       </c>
-      <c r="N24" t="n">
+      <c r="N24" s="1" t="n">
         <v>8057</v>
       </c>
-      <c r="O24" t="n">
+      <c r="O24" s="1" t="n">
         <v>5777</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
+      <c r="A25" s="1" t="inlineStr">
         <is>
           <t>주당이익</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="B25" s="1" t="inlineStr">
         <is>
           <t>희석주당이익(손실) (단위 : 원)</t>
         </is>
       </c>
-      <c r="D25" t="n">
+      <c r="C25" s="1" t="n"/>
+      <c r="D25" s="1" t="n">
         <v>2131</v>
       </c>
-      <c r="E25" t="n">
+      <c r="E25" s="1" t="n">
         <v>8057</v>
       </c>
-      <c r="F25" t="n">
+      <c r="F25" s="1" t="n">
         <v>5777</v>
       </c>
-      <c r="J25" t="n">
+      <c r="G25" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H25" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I25" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J25" s="1" t="n">
         <v>2131</v>
       </c>
-      <c r="K25" t="n">
+      <c r="K25" s="1" t="n">
         <v>8057</v>
       </c>
-      <c r="L25" t="n">
+      <c r="L25" s="1" t="n">
         <v>5777</v>
       </c>
-      <c r="M25" t="n">
+      <c r="M25" s="1" t="n">
         <v>2131</v>
       </c>
-      <c r="N25" t="n">
+      <c r="N25" s="1" t="n">
         <v>8057</v>
       </c>
-      <c r="O25" t="n">
+      <c r="O25" s="1" t="n">
         <v>5777</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
+      <c r="A26" s="1" t="inlineStr">
         <is>
           <t>주당이익</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
+      <c r="B26" s="1" t="inlineStr">
         <is>
           <t>기본주당이익 (단위 :원)</t>
         </is>
       </c>
-      <c r="G26" t="n">
-        <v/>
-      </c>
-      <c r="H26" t="n">
-        <v/>
-      </c>
-      <c r="I26" t="n">
-        <v/>
-      </c>
-      <c r="J26" t="n">
-        <v/>
-      </c>
-      <c r="K26" t="n">
-        <v/>
-      </c>
-      <c r="L26" t="n">
-        <v/>
-      </c>
-      <c r="M26" t="n">
-        <v/>
-      </c>
-      <c r="N26" t="n">
-        <v/>
-      </c>
-      <c r="O26" t="n">
+      <c r="C26" s="1" t="n"/>
+      <c r="D26" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E26" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F26" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G26" s="1" t="n">
+        <v/>
+      </c>
+      <c r="H26" s="1" t="n">
+        <v/>
+      </c>
+      <c r="I26" s="1" t="n">
+        <v/>
+      </c>
+      <c r="J26" s="1" t="n">
+        <v/>
+      </c>
+      <c r="K26" s="1" t="n">
+        <v/>
+      </c>
+      <c r="L26" s="1" t="n">
+        <v/>
+      </c>
+      <c r="M26" s="1" t="n">
+        <v/>
+      </c>
+      <c r="N26" s="1" t="n">
+        <v/>
+      </c>
+      <c r="O26" s="1" t="n">
         <v/>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
+      <c r="A27" s="1" t="inlineStr">
         <is>
           <t>주당이익</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
+      <c r="B27" s="1" t="inlineStr">
         <is>
           <t>기본주당이익 (단위 :원)</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="C27" s="1" t="inlineStr">
         <is>
           <t>보통주기본주당이익(손실) (단위 : 원)</t>
         </is>
       </c>
-      <c r="G27" t="n">
+      <c r="D27" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E27" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F27" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G27" s="1" t="n">
         <v>45703</v>
       </c>
-      <c r="H27" t="n">
+      <c r="H27" s="1" t="n">
         <v>28521</v>
       </c>
-      <c r="I27" t="n">
+      <c r="I27" s="1" t="n">
         <v>18979</v>
       </c>
-      <c r="J27" t="n">
+      <c r="J27" s="1" t="n">
         <v>45703</v>
       </c>
-      <c r="K27" t="n">
+      <c r="K27" s="1" t="n">
         <v>28521</v>
       </c>
-      <c r="L27" t="n">
+      <c r="L27" s="1" t="n">
         <v>18979</v>
       </c>
-      <c r="M27" t="n">
+      <c r="M27" s="1" t="n">
         <v>45703</v>
       </c>
-      <c r="N27" t="n">
+      <c r="N27" s="1" t="n">
         <v>28521</v>
       </c>
-      <c r="O27" t="n">
+      <c r="O27" s="1" t="n">
         <v>18979</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
+      <c r="A28" s="1" t="inlineStr">
         <is>
           <t>주당이익</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="B28" s="1" t="inlineStr">
         <is>
           <t>기본주당이익 (단위 :원)</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="C28" s="1" t="inlineStr">
         <is>
           <t>계속영업 보통주기본주당이익(손실) (단위: 원)</t>
         </is>
       </c>
-      <c r="G28" t="n">
+      <c r="D28" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E28" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F28" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G28" s="1" t="n">
         <v>47622</v>
       </c>
-      <c r="H28" t="n">
+      <c r="H28" s="1" t="n">
         <v>29105</v>
       </c>
-      <c r="I28" t="n">
+      <c r="I28" s="1" t="n">
         <v>18521</v>
       </c>
-      <c r="J28" t="n">
+      <c r="J28" s="1" t="n">
         <v>47622</v>
       </c>
-      <c r="K28" t="n">
+      <c r="K28" s="1" t="n">
         <v>29105</v>
       </c>
-      <c r="L28" t="n">
+      <c r="L28" s="1" t="n">
         <v>18521</v>
       </c>
-      <c r="M28" t="n">
+      <c r="M28" s="1" t="n">
         <v>47622</v>
       </c>
-      <c r="N28" t="n">
+      <c r="N28" s="1" t="n">
         <v>29105</v>
       </c>
-      <c r="O28" t="n">
+      <c r="O28" s="1" t="n">
         <v>18521</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
+      <c r="A29" s="1" t="inlineStr">
         <is>
           <t>주당이익</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="B29" s="1" t="inlineStr">
         <is>
           <t>기본주당이익 (단위 :원)</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="C29" s="1" t="inlineStr">
         <is>
           <t>중단영업 보통주기본주당이익(손실) (단위: 원)</t>
         </is>
       </c>
-      <c r="G29" t="n">
+      <c r="D29" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E29" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F29" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G29" s="1" t="n">
         <v>-1919</v>
       </c>
-      <c r="H29" t="n">
+      <c r="H29" s="1" t="n">
         <v>-584</v>
       </c>
-      <c r="I29" t="n">
+      <c r="I29" s="1" t="n">
         <v>458</v>
       </c>
-      <c r="J29" t="n">
+      <c r="J29" s="1" t="n">
         <v>-1919</v>
       </c>
-      <c r="K29" t="n">
+      <c r="K29" s="1" t="n">
         <v>-584</v>
       </c>
-      <c r="L29" t="n">
+      <c r="L29" s="1" t="n">
         <v>458</v>
       </c>
-      <c r="M29" t="n">
+      <c r="M29" s="1" t="n">
         <v>-1919</v>
       </c>
-      <c r="N29" t="n">
+      <c r="N29" s="1" t="n">
         <v>-584</v>
       </c>
-      <c r="O29" t="n">
+      <c r="O29" s="1" t="n">
         <v>458</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
+      <c r="A30" s="1" t="inlineStr">
         <is>
           <t>주당이익</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
+      <c r="B30" s="1" t="inlineStr">
         <is>
           <t>기본주당이익 (단위 :원)</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
+      <c r="C30" s="1" t="inlineStr">
         <is>
           <t>1우선주 기본주당이익(손실) (단위 : 원)</t>
         </is>
       </c>
-      <c r="G30" t="n">
+      <c r="D30" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E30" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F30" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G30" s="1" t="n">
         <v>45535</v>
       </c>
-      <c r="H30" t="n">
+      <c r="H30" s="1" t="n">
         <v>28207</v>
       </c>
-      <c r="I30" t="n">
+      <c r="I30" s="1" t="n">
         <v>19002</v>
       </c>
-      <c r="J30" t="n">
+      <c r="J30" s="1" t="n">
         <v>45535</v>
       </c>
-      <c r="K30" t="n">
+      <c r="K30" s="1" t="n">
         <v>28207</v>
       </c>
-      <c r="L30" t="n">
+      <c r="L30" s="1" t="n">
         <v>19002</v>
       </c>
-      <c r="M30" t="n">
+      <c r="M30" s="1" t="n">
         <v>45535</v>
       </c>
-      <c r="N30" t="n">
+      <c r="N30" s="1" t="n">
         <v>28207</v>
       </c>
-      <c r="O30" t="n">
+      <c r="O30" s="1" t="n">
         <v>19002</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
+      <c r="A31" s="1" t="inlineStr">
         <is>
           <t>주당이익</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
+      <c r="B31" s="1" t="inlineStr">
         <is>
           <t>기본주당이익 (단위 :원)</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
+      <c r="C31" s="1" t="inlineStr">
         <is>
           <t>계속영업 1우선주기본주당이익(손실) (단위 : 원)</t>
         </is>
       </c>
-      <c r="G31" t="n">
+      <c r="D31" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E31" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F31" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G31" s="1" t="n">
         <v>47445</v>
       </c>
-      <c r="H31" t="n">
+      <c r="H31" s="1" t="n">
         <v>28783</v>
       </c>
-      <c r="I31" t="n">
+      <c r="I31" s="1" t="n">
         <v>18545</v>
       </c>
-      <c r="J31" t="n">
+      <c r="J31" s="1" t="n">
         <v>47445</v>
       </c>
-      <c r="K31" t="n">
+      <c r="K31" s="1" t="n">
         <v>28783</v>
       </c>
-      <c r="L31" t="n">
+      <c r="L31" s="1" t="n">
         <v>18545</v>
       </c>
-      <c r="M31" t="n">
+      <c r="M31" s="1" t="n">
         <v>47445</v>
       </c>
-      <c r="N31" t="n">
+      <c r="N31" s="1" t="n">
         <v>28783</v>
       </c>
-      <c r="O31" t="n">
+      <c r="O31" s="1" t="n">
         <v>18545</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
+      <c r="A32" s="1" t="inlineStr">
         <is>
           <t>주당이익</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
+      <c r="B32" s="1" t="inlineStr">
         <is>
           <t>기본주당이익 (단위 :원)</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="C32" s="1" t="inlineStr">
         <is>
           <t>중단영업 1우선주기본주당이익(손실) (단위 : 원)</t>
         </is>
       </c>
-      <c r="G32" t="n">
+      <c r="D32" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E32" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F32" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G32" s="1" t="n">
         <v>-1910</v>
       </c>
-      <c r="H32" t="n">
+      <c r="H32" s="1" t="n">
         <v>-576</v>
       </c>
-      <c r="I32" t="n">
+      <c r="I32" s="1" t="n">
         <v>457</v>
       </c>
-      <c r="J32" t="n">
+      <c r="J32" s="1" t="n">
         <v>-1910</v>
       </c>
-      <c r="K32" t="n">
+      <c r="K32" s="1" t="n">
         <v>-576</v>
       </c>
-      <c r="L32" t="n">
+      <c r="L32" s="1" t="n">
         <v>457</v>
       </c>
-      <c r="M32" t="n">
+      <c r="M32" s="1" t="n">
         <v>-1910</v>
       </c>
-      <c r="N32" t="n">
+      <c r="N32" s="1" t="n">
         <v>-576</v>
       </c>
-      <c r="O32" t="n">
+      <c r="O32" s="1" t="n">
         <v>457</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
+      <c r="A33" s="1" t="inlineStr">
         <is>
           <t>주당이익</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
+      <c r="B33" s="1" t="inlineStr">
         <is>
           <t>희석주당이익(손실)(단위 : 원)</t>
         </is>
       </c>
-      <c r="G33" t="n">
-        <v/>
-      </c>
-      <c r="H33" t="n">
-        <v/>
-      </c>
-      <c r="I33" t="n">
-        <v/>
-      </c>
-      <c r="J33" t="n">
-        <v/>
-      </c>
-      <c r="K33" t="n">
-        <v/>
-      </c>
-      <c r="L33" t="n">
-        <v/>
-      </c>
-      <c r="M33" t="n">
-        <v/>
-      </c>
-      <c r="N33" t="n">
-        <v/>
-      </c>
-      <c r="O33" t="n">
+      <c r="C33" s="1" t="n"/>
+      <c r="D33" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E33" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F33" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G33" s="1" t="n">
+        <v/>
+      </c>
+      <c r="H33" s="1" t="n">
+        <v/>
+      </c>
+      <c r="I33" s="1" t="n">
+        <v/>
+      </c>
+      <c r="J33" s="1" t="n">
+        <v/>
+      </c>
+      <c r="K33" s="1" t="n">
+        <v/>
+      </c>
+      <c r="L33" s="1" t="n">
+        <v/>
+      </c>
+      <c r="M33" s="1" t="n">
+        <v/>
+      </c>
+      <c r="N33" s="1" t="n">
+        <v/>
+      </c>
+      <c r="O33" s="1" t="n">
         <v/>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
+      <c r="A34" s="1" t="inlineStr">
         <is>
           <t>주당이익</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="B34" s="1" t="inlineStr">
         <is>
           <t>희석주당이익(손실)(단위 : 원)</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="C34" s="1" t="inlineStr">
         <is>
           <t>보통주 희석주당이익 (단위 : 원)</t>
         </is>
       </c>
-      <c r="G34" t="n">
+      <c r="D34" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E34" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F34" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G34" s="1" t="n">
         <v>45703</v>
       </c>
-      <c r="H34" t="n">
+      <c r="H34" s="1" t="n">
         <v>28521</v>
       </c>
-      <c r="I34" t="n">
+      <c r="I34" s="1" t="n">
         <v>18979</v>
       </c>
-      <c r="J34" t="n">
+      <c r="J34" s="1" t="n">
         <v>45703</v>
       </c>
-      <c r="K34" t="n">
+      <c r="K34" s="1" t="n">
         <v>28521</v>
       </c>
-      <c r="L34" t="n">
+      <c r="L34" s="1" t="n">
         <v>18979</v>
       </c>
-      <c r="M34" t="n">
+      <c r="M34" s="1" t="n">
         <v>45703</v>
       </c>
-      <c r="N34" t="n">
+      <c r="N34" s="1" t="n">
         <v>28521</v>
       </c>
-      <c r="O34" t="n">
+      <c r="O34" s="1" t="n">
         <v>18979</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
+      <c r="A35" s="1" t="inlineStr">
         <is>
           <t>주당이익</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr">
+      <c r="B35" s="1" t="inlineStr">
         <is>
           <t>희석주당이익(손실)(단위 : 원)</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
+      <c r="C35" s="1" t="inlineStr">
         <is>
           <t>1우선주 희석주당이익 (단위 : 원)</t>
         </is>
       </c>
-      <c r="G35" t="n">
+      <c r="D35" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E35" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F35" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G35" s="1" t="n">
         <v>45535</v>
       </c>
-      <c r="H35" t="n">
+      <c r="H35" s="1" t="n">
         <v>28207</v>
       </c>
-      <c r="I35" t="n">
+      <c r="I35" s="1" t="n">
         <v>19002</v>
       </c>
-      <c r="J35" t="n">
+      <c r="J35" s="1" t="n">
         <v>45535</v>
       </c>
-      <c r="K35" t="n">
+      <c r="K35" s="1" t="n">
         <v>28207</v>
       </c>
-      <c r="L35" t="n">
+      <c r="L35" s="1" t="n">
         <v>19002</v>
       </c>
-      <c r="M35" t="n">
+      <c r="M35" s="1" t="n">
         <v>45535</v>
       </c>
-      <c r="N35" t="n">
+      <c r="N35" s="1" t="n">
         <v>28207</v>
       </c>
-      <c r="O35" t="n">
+      <c r="O35" s="1" t="n">
         <v>19002</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
+      <c r="A36" s="1" t="inlineStr">
         <is>
           <t>매출액</t>
         </is>
       </c>
-      <c r="G36" t="n">
+      <c r="B36" s="1" t="n"/>
+      <c r="C36" s="1" t="n"/>
+      <c r="D36" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E36" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F36" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G36" s="1" t="n">
         <v>162663579</v>
       </c>
-      <c r="H36" t="n">
+      <c r="H36" s="1" t="n">
         <v>142151469</v>
       </c>
-      <c r="I36" t="n">
+      <c r="I36" s="1" t="n">
         <v>116448159</v>
       </c>
-      <c r="J36" t="n">
+      <c r="J36" s="1" t="n">
         <v>162663579</v>
       </c>
-      <c r="K36" t="n">
+      <c r="K36" s="1" t="n">
         <v>142151469</v>
       </c>
-      <c r="L36" t="n">
+      <c r="L36" s="1" t="n">
         <v>116448159</v>
       </c>
-      <c r="M36" t="n">
+      <c r="M36" s="1" t="n">
         <v>162663579</v>
       </c>
-      <c r="N36" t="n">
+      <c r="N36" s="1" t="n">
         <v>142151469</v>
       </c>
-      <c r="O36" t="n">
+      <c r="O36" s="1" t="n">
         <v>116448159</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
+      <c r="A37" s="1" t="inlineStr">
         <is>
           <t>공동기업및관계기업투자손익</t>
         </is>
       </c>
-      <c r="G37" t="n">
+      <c r="B37" s="1" t="n"/>
+      <c r="C37" s="1" t="n"/>
+      <c r="D37" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E37" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F37" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G37" s="1" t="n">
         <v>2470933</v>
       </c>
-      <c r="H37" t="n">
+      <c r="H37" s="1" t="n">
         <v>1557630</v>
       </c>
-      <c r="I37" t="n">
+      <c r="I37" s="1" t="n">
         <v>1302150</v>
       </c>
-      <c r="J37" t="n">
+      <c r="J37" s="1" t="n">
         <v>2470933</v>
       </c>
-      <c r="K37" t="n">
+      <c r="K37" s="1" t="n">
         <v>1557630</v>
       </c>
-      <c r="L37" t="n">
+      <c r="L37" s="1" t="n">
         <v>1302150</v>
       </c>
-      <c r="M37" t="n">
+      <c r="M37" s="1" t="n">
         <v>2470933</v>
       </c>
-      <c r="N37" t="n">
+      <c r="N37" s="1" t="n">
         <v>1557630</v>
       </c>
-      <c r="O37" t="n">
+      <c r="O37" s="1" t="n">
         <v>1302150</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
+      <c r="A38" s="1" t="inlineStr">
         <is>
           <t>기타수익</t>
         </is>
       </c>
-      <c r="G38" t="n">
+      <c r="B38" s="1" t="n"/>
+      <c r="C38" s="1" t="n"/>
+      <c r="D38" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E38" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F38" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G38" s="1" t="n">
         <v>1782333</v>
       </c>
-      <c r="H38" t="n">
+      <c r="H38" s="1" t="n">
         <v>1930914</v>
       </c>
-      <c r="I38" t="n">
+      <c r="I38" s="1" t="n">
         <v>1377997</v>
       </c>
-      <c r="J38" t="n">
+      <c r="J38" s="1" t="n">
         <v>1782333</v>
       </c>
-      <c r="K38" t="n">
+      <c r="K38" s="1" t="n">
         <v>1930914</v>
       </c>
-      <c r="L38" t="n">
+      <c r="L38" s="1" t="n">
         <v>1377997</v>
       </c>
-      <c r="M38" t="n">
+      <c r="M38" s="1" t="n">
         <v>1782333</v>
       </c>
-      <c r="N38" t="n">
+      <c r="N38" s="1" t="n">
         <v>1930914</v>
       </c>
-      <c r="O38" t="n">
+      <c r="O38" s="1" t="n">
         <v>1377997</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
+      <c r="A39" s="1" t="inlineStr">
         <is>
           <t>기타비용</t>
         </is>
       </c>
-      <c r="G39" t="n">
+      <c r="B39" s="1" t="n"/>
+      <c r="C39" s="1" t="n"/>
+      <c r="D39" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E39" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F39" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G39" s="1" t="n">
         <v>2350343</v>
       </c>
-      <c r="H39" t="n">
+      <c r="H39" s="1" t="n">
         <v>2238256</v>
       </c>
-      <c r="I39" t="n">
+      <c r="I39" s="1" t="n">
         <v>1745985</v>
       </c>
-      <c r="J39" t="n">
+      <c r="J39" s="1" t="n">
         <v>2350343</v>
       </c>
-      <c r="K39" t="n">
+      <c r="K39" s="1" t="n">
         <v>2238256</v>
       </c>
-      <c r="L39" t="n">
+      <c r="L39" s="1" t="n">
         <v>1745985</v>
       </c>
-      <c r="M39" t="n">
+      <c r="M39" s="1" t="n">
         <v>2350343</v>
       </c>
-      <c r="N39" t="n">
+      <c r="N39" s="1" t="n">
         <v>2238256</v>
       </c>
-      <c r="O39" t="n">
+      <c r="O39" s="1" t="n">
         <v>1745985</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
+      <c r="A40" s="1" t="inlineStr">
         <is>
           <t>법인세비용차감전순이익</t>
         </is>
       </c>
-      <c r="G40" t="n">
+      <c r="B40" s="1" t="n"/>
+      <c r="C40" s="1" t="n"/>
+      <c r="D40" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E40" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F40" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G40" s="1" t="n">
         <v>17618662</v>
       </c>
-      <c r="H40" t="n">
+      <c r="H40" s="1" t="n">
         <v>11181471</v>
       </c>
-      <c r="I40" t="n">
+      <c r="I40" s="1" t="n">
         <v>7789043</v>
       </c>
-      <c r="J40" t="n">
+      <c r="J40" s="1" t="n">
         <v>17618662</v>
       </c>
-      <c r="K40" t="n">
+      <c r="K40" s="1" t="n">
         <v>11181471</v>
       </c>
-      <c r="L40" t="n">
+      <c r="L40" s="1" t="n">
         <v>7789043</v>
       </c>
-      <c r="M40" t="n">
+      <c r="M40" s="1" t="n">
         <v>17618662</v>
       </c>
-      <c r="N40" t="n">
+      <c r="N40" s="1" t="n">
         <v>11181471</v>
       </c>
-      <c r="O40" t="n">
+      <c r="O40" s="1" t="n">
         <v>7789043</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
+      <c r="A41" s="1" t="inlineStr">
         <is>
           <t>계속영업연결당기순이익</t>
         </is>
       </c>
-      <c r="G41" t="n">
+      <c r="B41" s="1" t="n"/>
+      <c r="C41" s="1" t="n"/>
+      <c r="D41" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E41" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F41" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G41" s="1" t="n">
         <v>12992022</v>
       </c>
-      <c r="H41" t="n">
+      <c r="H41" s="1" t="n">
         <v>8202303</v>
       </c>
-      <c r="I41" t="n">
+      <c r="I41" s="1" t="n">
         <v>5522220</v>
       </c>
-      <c r="J41" t="n">
+      <c r="J41" s="1" t="n">
         <v>12992022</v>
       </c>
-      <c r="K41" t="n">
+      <c r="K41" s="1" t="n">
         <v>8202303</v>
       </c>
-      <c r="L41" t="n">
+      <c r="L41" s="1" t="n">
         <v>5522220</v>
       </c>
-      <c r="M41" t="n">
+      <c r="M41" s="1" t="n">
         <v>12992022</v>
       </c>
-      <c r="N41" t="n">
+      <c r="N41" s="1" t="n">
         <v>8202303</v>
       </c>
-      <c r="O41" t="n">
+      <c r="O41" s="1" t="n">
         <v>5522220</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
+      <c r="A42" s="1" t="inlineStr">
         <is>
           <t>중단영업당기순이익(손실)</t>
         </is>
       </c>
-      <c r="G42" t="n">
+      <c r="B42" s="1" t="n"/>
+      <c r="C42" s="1" t="n"/>
+      <c r="D42" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E42" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F42" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G42" s="1" t="n">
         <v>-719721</v>
       </c>
-      <c r="H42" t="n">
+      <c r="H42" s="1" t="n">
         <v>-218689</v>
       </c>
-      <c r="I42" t="n">
+      <c r="I42" s="1" t="n">
         <v>170857</v>
       </c>
-      <c r="J42" t="n">
+      <c r="J42" s="1" t="n">
         <v>-719721</v>
       </c>
-      <c r="K42" t="n">
+      <c r="K42" s="1" t="n">
         <v>-218689</v>
       </c>
-      <c r="L42" t="n">
+      <c r="L42" s="1" t="n">
         <v>170857</v>
       </c>
-      <c r="M42" t="n">
+      <c r="M42" s="1" t="n">
         <v>-719721</v>
       </c>
-      <c r="N42" t="n">
+      <c r="N42" s="1" t="n">
         <v>-218689</v>
       </c>
-      <c r="O42" t="n">
+      <c r="O42" s="1" t="n">
         <v>170857</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
+      <c r="A43" s="1" t="inlineStr">
         <is>
           <t>연결당기순이익</t>
         </is>
       </c>
-      <c r="G43" t="n">
+      <c r="B43" s="1" t="n"/>
+      <c r="C43" s="1" t="n"/>
+      <c r="D43" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E43" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F43" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G43" s="1" t="n">
         <v>12272301</v>
       </c>
-      <c r="H43" t="n">
+      <c r="H43" s="1" t="n">
         <v>7983614</v>
       </c>
-      <c r="I43" t="n">
+      <c r="I43" s="1" t="n">
         <v>5693077</v>
       </c>
-      <c r="J43" t="n">
+      <c r="J43" s="1" t="n">
         <v>12272301</v>
       </c>
-      <c r="K43" t="n">
+      <c r="K43" s="1" t="n">
         <v>7983614</v>
       </c>
-      <c r="L43" t="n">
+      <c r="L43" s="1" t="n">
         <v>5693077</v>
       </c>
-      <c r="M43" t="n">
+      <c r="M43" s="1" t="n">
         <v>12272301</v>
       </c>
-      <c r="N43" t="n">
+      <c r="N43" s="1" t="n">
         <v>7983614</v>
       </c>
-      <c r="O43" t="n">
+      <c r="O43" s="1" t="n">
         <v>5693077</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="J1:L1"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="M1:O1"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="G1:I1"/>
-    <mergeCell ref="M1:O1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
bugfixed, .bat for home
</commit_message>
<xml_diff>
--- a/data/output/연결 손익계산서.xlsx
+++ b/data/output/연결 손익계산서.xlsx
@@ -1288,41 +1288,65 @@
       </c>
       <c r="B18" s="1" t="n"/>
       <c r="C18" s="1" t="n"/>
-      <c r="D18" s="1" t="n">
-        <v/>
-      </c>
-      <c r="E18" s="1" t="n">
-        <v/>
-      </c>
-      <c r="F18" s="1" t="n">
-        <v/>
-      </c>
-      <c r="G18" s="1" t="n">
-        <v/>
-      </c>
-      <c r="H18" s="1" t="n">
-        <v/>
-      </c>
-      <c r="I18" s="1" t="n">
-        <v/>
-      </c>
-      <c r="J18" s="1" t="n">
-        <v/>
-      </c>
-      <c r="K18" s="1" t="n">
-        <v/>
-      </c>
-      <c r="L18" s="1" t="n">
-        <v/>
-      </c>
-      <c r="M18" s="1" t="n">
-        <v/>
-      </c>
-      <c r="N18" s="1" t="n">
-        <v/>
-      </c>
-      <c r="O18" s="1" t="n">
-        <v/>
+      <c r="D18" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E18" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F18" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G18" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H18" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I18" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J18" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K18" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L18" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M18" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N18" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O18" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
     </row>
     <row r="19">
@@ -1553,41 +1577,65 @@
       </c>
       <c r="B23" s="1" t="n"/>
       <c r="C23" s="1" t="n"/>
-      <c r="D23" s="1" t="n">
-        <v/>
-      </c>
-      <c r="E23" s="1" t="n">
-        <v/>
-      </c>
-      <c r="F23" s="1" t="n">
-        <v/>
-      </c>
-      <c r="G23" s="1" t="n">
-        <v/>
-      </c>
-      <c r="H23" s="1" t="n">
-        <v/>
-      </c>
-      <c r="I23" s="1" t="n">
-        <v/>
-      </c>
-      <c r="J23" s="1" t="n">
-        <v/>
-      </c>
-      <c r="K23" s="1" t="n">
-        <v/>
-      </c>
-      <c r="L23" s="1" t="n">
-        <v/>
-      </c>
-      <c r="M23" s="1" t="n">
-        <v/>
-      </c>
-      <c r="N23" s="1" t="n">
-        <v/>
-      </c>
-      <c r="O23" s="1" t="n">
-        <v/>
+      <c r="D23" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E23" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F23" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G23" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H23" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I23" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J23" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K23" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L23" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M23" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N23" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O23" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
     </row>
     <row r="24">
@@ -1727,32 +1775,50 @@
           <t>-</t>
         </is>
       </c>
-      <c r="G26" s="1" t="n">
-        <v/>
-      </c>
-      <c r="H26" s="1" t="n">
-        <v/>
-      </c>
-      <c r="I26" s="1" t="n">
-        <v/>
-      </c>
-      <c r="J26" s="1" t="n">
-        <v/>
-      </c>
-      <c r="K26" s="1" t="n">
-        <v/>
-      </c>
-      <c r="L26" s="1" t="n">
-        <v/>
-      </c>
-      <c r="M26" s="1" t="n">
-        <v/>
-      </c>
-      <c r="N26" s="1" t="n">
-        <v/>
-      </c>
-      <c r="O26" s="1" t="n">
-        <v/>
+      <c r="G26" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H26" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I26" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J26" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K26" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L26" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M26" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N26" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O26" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
     </row>
     <row r="27">
@@ -2136,32 +2202,50 @@
           <t>-</t>
         </is>
       </c>
-      <c r="G33" s="1" t="n">
-        <v/>
-      </c>
-      <c r="H33" s="1" t="n">
-        <v/>
-      </c>
-      <c r="I33" s="1" t="n">
-        <v/>
-      </c>
-      <c r="J33" s="1" t="n">
-        <v/>
-      </c>
-      <c r="K33" s="1" t="n">
-        <v/>
-      </c>
-      <c r="L33" s="1" t="n">
-        <v/>
-      </c>
-      <c r="M33" s="1" t="n">
-        <v/>
-      </c>
-      <c r="N33" s="1" t="n">
-        <v/>
-      </c>
-      <c r="O33" s="1" t="n">
-        <v/>
+      <c r="G33" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H33" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I33" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J33" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K33" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L33" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M33" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N33" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O33" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
     </row>
     <row r="34">

</xml_diff>

<commit_message>
added interfaces to upload pdf files
원하는 pdf파일을 업로드 하고, 거기에 맞춘 답변을 받을 수 있다.
아직 연도 선택 작업이 남았다. 연도를 바꿀때마다 db도 같이 바뀌게 해야하나? 그럼 임베딩이 너무 자주 일어나지 않을까 하는 걱정이 있다.
</commit_message>
<xml_diff>
--- a/data/output/연결 손익계산서.xlsx
+++ b/data/output/연결 손익계산서.xlsx
@@ -499,14 +499,14 @@
       <c r="C1" s="3" t="n"/>
       <c r="D1" s="4" t="inlineStr">
         <is>
-          <t>Samsung</t>
+          <t>Hyundai</t>
         </is>
       </c>
       <c r="E1" s="1" t="n"/>
       <c r="F1" s="1" t="n"/>
       <c r="G1" s="4" t="inlineStr">
         <is>
-          <t>Hyundai</t>
+          <t>Samsung</t>
         </is>
       </c>
       <c r="H1" s="1" t="n"/>
@@ -611,19 +611,19 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>영업수익</t>
+          <t>매출액</t>
         </is>
       </c>
       <c r="B4" s="1" t="n"/>
       <c r="C4" s="1" t="n"/>
       <c r="D4" s="1" t="n">
-        <v>258935494</v>
+        <v>162663579</v>
       </c>
       <c r="E4" s="1" t="n">
-        <v>302231360</v>
+        <v>142151469</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>279604799</v>
+        <v>116448159</v>
       </c>
       <c r="G4" s="7" t="inlineStr">
         <is>
@@ -641,22 +641,22 @@
         </is>
       </c>
       <c r="J4" s="1" t="n">
-        <v>258935494</v>
+        <v>162663579</v>
       </c>
       <c r="K4" s="1" t="n">
-        <v>302231360</v>
+        <v>142151469</v>
       </c>
       <c r="L4" s="1" t="n">
-        <v>279604799</v>
+        <v>116448159</v>
       </c>
       <c r="M4" s="1" t="n">
-        <v>258935494</v>
+        <v>162663579</v>
       </c>
       <c r="N4" s="1" t="n">
-        <v>302231360</v>
+        <v>142151469</v>
       </c>
       <c r="O4" s="1" t="n">
-        <v>279604799</v>
+        <v>116448159</v>
       </c>
     </row>
     <row r="5">
@@ -668,22 +668,22 @@
       <c r="B5" s="1" t="n"/>
       <c r="C5" s="1" t="n"/>
       <c r="D5" s="1" t="n">
+        <v>129179183</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>113879569</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>94721313</v>
+      </c>
+      <c r="G5" s="1" t="n">
         <v>180388580</v>
       </c>
-      <c r="E5" s="1" t="n">
+      <c r="H5" s="1" t="n">
         <v>190041770</v>
       </c>
-      <c r="F5" s="1" t="n">
+      <c r="I5" s="1" t="n">
         <v>166411342</v>
-      </c>
-      <c r="G5" s="1" t="n">
-        <v>129179183</v>
-      </c>
-      <c r="H5" s="1" t="n">
-        <v>113879569</v>
-      </c>
-      <c r="I5" s="1" t="n">
-        <v>94721313</v>
       </c>
       <c r="J5" s="1" t="n">
         <v>309567763</v>
@@ -713,22 +713,22 @@
       <c r="B6" s="1" t="n"/>
       <c r="C6" s="1" t="n"/>
       <c r="D6" s="1" t="n">
+        <v>33484396</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>28271900</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>21726846</v>
+      </c>
+      <c r="G6" s="1" t="n">
         <v>78546914</v>
       </c>
-      <c r="E6" s="1" t="n">
+      <c r="H6" s="1" t="n">
         <v>112189590</v>
       </c>
-      <c r="F6" s="1" t="n">
+      <c r="I6" s="1" t="n">
         <v>113193457</v>
-      </c>
-      <c r="G6" s="1" t="n">
-        <v>33484396</v>
-      </c>
-      <c r="H6" s="1" t="n">
-        <v>28271900</v>
-      </c>
-      <c r="I6" s="1" t="n">
-        <v>21726846</v>
       </c>
       <c r="J6" s="1" t="n">
         <v>112031310</v>
@@ -758,22 +758,22 @@
       <c r="B7" s="1" t="n"/>
       <c r="C7" s="1" t="n"/>
       <c r="D7" s="1" t="n">
+        <v>18357495</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>18446972</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>15200325</v>
+      </c>
+      <c r="G7" s="1" t="n">
         <v>71979938</v>
       </c>
-      <c r="E7" s="1" t="n">
+      <c r="H7" s="1" t="n">
         <v>68812960</v>
       </c>
-      <c r="F7" s="1" t="n">
+      <c r="I7" s="1" t="n">
         <v>61559601</v>
-      </c>
-      <c r="G7" s="1" t="n">
-        <v>18357495</v>
-      </c>
-      <c r="H7" s="1" t="n">
-        <v>18446972</v>
-      </c>
-      <c r="I7" s="1" t="n">
-        <v>15200325</v>
       </c>
       <c r="J7" s="1" t="n">
         <v>90337433</v>
@@ -803,22 +803,22 @@
       <c r="B8" s="1" t="n"/>
       <c r="C8" s="1" t="n"/>
       <c r="D8" s="1" t="n">
+        <v>15126901</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>9824928</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>6526521</v>
+      </c>
+      <c r="G8" s="1" t="n">
         <v>6566976</v>
       </c>
-      <c r="E8" s="1" t="n">
+      <c r="H8" s="1" t="n">
         <v>43376630</v>
       </c>
-      <c r="F8" s="1" t="n">
+      <c r="I8" s="1" t="n">
         <v>51633856</v>
-      </c>
-      <c r="G8" s="1" t="n">
-        <v>15126901</v>
-      </c>
-      <c r="H8" s="1" t="n">
-        <v>9824928</v>
-      </c>
-      <c r="I8" s="1" t="n">
-        <v>6526521</v>
       </c>
       <c r="J8" s="1" t="n">
         <v>21693877</v>
@@ -842,19 +842,19 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>기타이익</t>
+          <t>공동기업및관계기업투자손익</t>
         </is>
       </c>
       <c r="B9" s="1" t="n"/>
       <c r="C9" s="1" t="n"/>
       <c r="D9" s="1" t="n">
-        <v>1180448</v>
+        <v>2470933</v>
       </c>
       <c r="E9" s="1" t="n">
-        <v>1962071</v>
+        <v>1557630</v>
       </c>
       <c r="F9" s="1" t="n">
-        <v>2205695</v>
+        <v>1302150</v>
       </c>
       <c r="G9" s="7" t="inlineStr">
         <is>
@@ -872,232 +872,232 @@
         </is>
       </c>
       <c r="J9" s="1" t="n">
-        <v>1180448</v>
+        <v>2470933</v>
       </c>
       <c r="K9" s="1" t="n">
-        <v>1962071</v>
+        <v>1557630</v>
       </c>
       <c r="L9" s="1" t="n">
-        <v>2205695</v>
+        <v>1302150</v>
       </c>
       <c r="M9" s="1" t="n">
-        <v>1180448</v>
+        <v>2470933</v>
       </c>
       <c r="N9" s="1" t="n">
-        <v>1962071</v>
+        <v>1557630</v>
       </c>
       <c r="O9" s="1" t="n">
-        <v>2205695</v>
+        <v>1302150</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>기타손실</t>
+          <t>금융수익</t>
         </is>
       </c>
       <c r="B10" s="1" t="n"/>
       <c r="C10" s="1" t="n"/>
       <c r="D10" s="1" t="n">
-        <v>1083327</v>
+        <v>1559538</v>
       </c>
       <c r="E10" s="1" t="n">
-        <v>1790176</v>
+        <v>985893</v>
       </c>
       <c r="F10" s="1" t="n">
-        <v>2055971</v>
-      </c>
-      <c r="G10" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H10" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I10" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>841196</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <v>16100148</v>
+      </c>
+      <c r="H10" s="1" t="n">
+        <v>20828995</v>
+      </c>
+      <c r="I10" s="1" t="n">
+        <v>8543187</v>
       </c>
       <c r="J10" s="1" t="n">
-        <v>1083327</v>
+        <v>17659686</v>
       </c>
       <c r="K10" s="1" t="n">
-        <v>1790176</v>
+        <v>21814888</v>
       </c>
       <c r="L10" s="1" t="n">
-        <v>2055971</v>
+        <v>9384383</v>
       </c>
       <c r="M10" s="1" t="n">
-        <v>1083327</v>
+        <v>8829843</v>
       </c>
       <c r="N10" s="1" t="n">
-        <v>1790176</v>
+        <v>10907444</v>
       </c>
       <c r="O10" s="1" t="n">
-        <v>2055971</v>
+        <v>4692191.5</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>지분법이익</t>
+          <t>금융비용</t>
         </is>
       </c>
       <c r="B11" s="1" t="n"/>
       <c r="C11" s="1" t="n"/>
       <c r="D11" s="1" t="n">
-        <v>887550</v>
+        <v>970700</v>
       </c>
       <c r="E11" s="1" t="n">
-        <v>1090643</v>
+        <v>879638</v>
       </c>
       <c r="F11" s="1" t="n">
-        <v>729614</v>
-      </c>
-      <c r="G11" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H11" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I11" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>512836</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>12645530</v>
+      </c>
+      <c r="H11" s="1" t="n">
+        <v>19027689</v>
+      </c>
+      <c r="I11" s="1" t="n">
+        <v>7704554</v>
       </c>
       <c r="J11" s="1" t="n">
-        <v>887550</v>
+        <v>13616230</v>
       </c>
       <c r="K11" s="1" t="n">
-        <v>1090643</v>
+        <v>19907327</v>
       </c>
       <c r="L11" s="1" t="n">
-        <v>729614</v>
+        <v>8217390</v>
       </c>
       <c r="M11" s="1" t="n">
-        <v>887550</v>
+        <v>6808115</v>
       </c>
       <c r="N11" s="1" t="n">
-        <v>1090643</v>
+        <v>9953663.5</v>
       </c>
       <c r="O11" s="1" t="n">
-        <v>729614</v>
+        <v>4108695</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>금융수익</t>
+          <t>기타수익</t>
         </is>
       </c>
       <c r="B12" s="1" t="n"/>
       <c r="C12" s="1" t="n"/>
       <c r="D12" s="1" t="n">
-        <v>16100148</v>
+        <v>1782333</v>
       </c>
       <c r="E12" s="1" t="n">
-        <v>20828995</v>
+        <v>1930914</v>
       </c>
       <c r="F12" s="1" t="n">
-        <v>8543187</v>
-      </c>
-      <c r="G12" s="1" t="n">
-        <v>1559538</v>
-      </c>
-      <c r="H12" s="1" t="n">
-        <v>985893</v>
-      </c>
-      <c r="I12" s="1" t="n">
-        <v>841196</v>
+        <v>1377997</v>
+      </c>
+      <c r="G12" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H12" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I12" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="J12" s="1" t="n">
-        <v>17659686</v>
+        <v>1782333</v>
       </c>
       <c r="K12" s="1" t="n">
-        <v>21814888</v>
+        <v>1930914</v>
       </c>
       <c r="L12" s="1" t="n">
-        <v>9384383</v>
+        <v>1377997</v>
       </c>
       <c r="M12" s="1" t="n">
-        <v>8829843</v>
+        <v>1782333</v>
       </c>
       <c r="N12" s="1" t="n">
-        <v>10907444</v>
+        <v>1930914</v>
       </c>
       <c r="O12" s="1" t="n">
-        <v>4692191.5</v>
+        <v>1377997</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>금융비용</t>
+          <t>기타비용</t>
         </is>
       </c>
       <c r="B13" s="1" t="n"/>
       <c r="C13" s="1" t="n"/>
       <c r="D13" s="1" t="n">
-        <v>12645530</v>
+        <v>2350343</v>
       </c>
       <c r="E13" s="1" t="n">
-        <v>19027689</v>
+        <v>2238256</v>
       </c>
       <c r="F13" s="1" t="n">
-        <v>7704554</v>
-      </c>
-      <c r="G13" s="1" t="n">
-        <v>970700</v>
-      </c>
-      <c r="H13" s="1" t="n">
-        <v>879638</v>
-      </c>
-      <c r="I13" s="1" t="n">
-        <v>512836</v>
+        <v>1745985</v>
+      </c>
+      <c r="G13" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H13" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I13" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="J13" s="1" t="n">
-        <v>13616230</v>
+        <v>2350343</v>
       </c>
       <c r="K13" s="1" t="n">
-        <v>19907327</v>
+        <v>2238256</v>
       </c>
       <c r="L13" s="1" t="n">
-        <v>8217390</v>
+        <v>1745985</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>6808115</v>
+        <v>2350343</v>
       </c>
       <c r="N13" s="1" t="n">
-        <v>9953663.5</v>
+        <v>2238256</v>
       </c>
       <c r="O13" s="1" t="n">
-        <v>4108695</v>
+        <v>1745985</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>법인세비용차감전순이익(손실)</t>
+          <t>법인세비용차감전순이익</t>
         </is>
       </c>
       <c r="B14" s="1" t="n"/>
       <c r="C14" s="1" t="n"/>
       <c r="D14" s="1" t="n">
-        <v>11006265</v>
+        <v>17618662</v>
       </c>
       <c r="E14" s="1" t="n">
-        <v>46440474</v>
+        <v>11181471</v>
       </c>
       <c r="F14" s="1" t="n">
-        <v>53351827</v>
+        <v>7789043</v>
       </c>
       <c r="G14" s="7" t="inlineStr">
         <is>
@@ -1115,22 +1115,22 @@
         </is>
       </c>
       <c r="J14" s="1" t="n">
-        <v>11006265</v>
+        <v>17618662</v>
       </c>
       <c r="K14" s="1" t="n">
-        <v>46440474</v>
+        <v>11181471</v>
       </c>
       <c r="L14" s="1" t="n">
-        <v>53351827</v>
+        <v>7789043</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>11006265</v>
+        <v>17618662</v>
       </c>
       <c r="N14" s="1" t="n">
-        <v>46440474</v>
+        <v>11181471</v>
       </c>
       <c r="O14" s="1" t="n">
-        <v>53351827</v>
+        <v>7789043</v>
       </c>
     </row>
     <row r="15">
@@ -1142,22 +1142,22 @@
       <c r="B15" s="1" t="n"/>
       <c r="C15" s="1" t="n"/>
       <c r="D15" s="1" t="n">
+        <v>4626640</v>
+      </c>
+      <c r="E15" s="1" t="n">
+        <v>2979168</v>
+      </c>
+      <c r="F15" s="1" t="n">
+        <v>2266823</v>
+      </c>
+      <c r="G15" s="1" t="n">
         <v>-4480835</v>
       </c>
-      <c r="E15" s="1" t="n">
+      <c r="H15" s="1" t="n">
         <v>-9213603</v>
       </c>
-      <c r="F15" s="1" t="n">
+      <c r="I15" s="1" t="n">
         <v>13444377</v>
-      </c>
-      <c r="G15" s="1" t="n">
-        <v>4626640</v>
-      </c>
-      <c r="H15" s="1" t="n">
-        <v>2979168</v>
-      </c>
-      <c r="I15" s="1" t="n">
-        <v>2266823</v>
       </c>
       <c r="J15" s="1" t="n">
         <v>145805</v>
@@ -1181,19 +1181,19 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>계속영업이익(손실)</t>
+          <t>계속영업연결당기순이익</t>
         </is>
       </c>
       <c r="B16" s="1" t="n"/>
       <c r="C16" s="1" t="n"/>
       <c r="D16" s="1" t="n">
-        <v>15487100</v>
+        <v>12992022</v>
       </c>
       <c r="E16" s="1" t="n">
-        <v>55654077</v>
+        <v>8202303</v>
       </c>
       <c r="F16" s="1" t="n">
-        <v>39907450</v>
+        <v>5522220</v>
       </c>
       <c r="G16" s="7" t="inlineStr">
         <is>
@@ -1211,40 +1211,40 @@
         </is>
       </c>
       <c r="J16" s="1" t="n">
-        <v>15487100</v>
+        <v>12992022</v>
       </c>
       <c r="K16" s="1" t="n">
-        <v>55654077</v>
+        <v>8202303</v>
       </c>
       <c r="L16" s="1" t="n">
-        <v>39907450</v>
+        <v>5522220</v>
       </c>
       <c r="M16" s="1" t="n">
-        <v>15487100</v>
+        <v>12992022</v>
       </c>
       <c r="N16" s="1" t="n">
-        <v>55654077</v>
+        <v>8202303</v>
       </c>
       <c r="O16" s="1" t="n">
-        <v>39907450</v>
+        <v>5522220</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>당기순이익(손실)</t>
+          <t>중단영업당기순이익(손실)</t>
         </is>
       </c>
       <c r="B17" s="1" t="n"/>
       <c r="C17" s="1" t="n"/>
       <c r="D17" s="1" t="n">
-        <v>15487100</v>
+        <v>-719721</v>
       </c>
       <c r="E17" s="1" t="n">
-        <v>55654077</v>
+        <v>-218689</v>
       </c>
       <c r="F17" s="1" t="n">
-        <v>39907450</v>
+        <v>170857</v>
       </c>
       <c r="G17" s="7" t="inlineStr">
         <is>
@@ -1262,46 +1262,40 @@
         </is>
       </c>
       <c r="J17" s="1" t="n">
-        <v>15487100</v>
+        <v>-719721</v>
       </c>
       <c r="K17" s="1" t="n">
-        <v>55654077</v>
+        <v>-218689</v>
       </c>
       <c r="L17" s="1" t="n">
-        <v>39907450</v>
+        <v>170857</v>
       </c>
       <c r="M17" s="1" t="n">
-        <v>15487100</v>
+        <v>-719721</v>
       </c>
       <c r="N17" s="1" t="n">
-        <v>55654077</v>
+        <v>-218689</v>
       </c>
       <c r="O17" s="1" t="n">
-        <v>39907450</v>
+        <v>170857</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>당기순이익(손실)의 귀속</t>
+          <t>연결당기순이익</t>
         </is>
       </c>
       <c r="B18" s="1" t="n"/>
       <c r="C18" s="1" t="n"/>
-      <c r="D18" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E18" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F18" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D18" s="1" t="n">
+        <v>12272301</v>
+      </c>
+      <c r="E18" s="1" t="n">
+        <v>7983614</v>
+      </c>
+      <c r="F18" s="1" t="n">
+        <v>5693077</v>
       </c>
       <c r="G18" s="7" t="inlineStr">
         <is>
@@ -1318,35 +1312,23 @@
           <t>-</t>
         </is>
       </c>
-      <c r="J18" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K18" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L18" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M18" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N18" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O18" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="J18" s="1" t="n">
+        <v>12272301</v>
+      </c>
+      <c r="K18" s="1" t="n">
+        <v>7983614</v>
+      </c>
+      <c r="L18" s="1" t="n">
+        <v>5693077</v>
+      </c>
+      <c r="M18" s="1" t="n">
+        <v>12272301</v>
+      </c>
+      <c r="N18" s="1" t="n">
+        <v>7983614</v>
+      </c>
+      <c r="O18" s="1" t="n">
+        <v>5693077</v>
       </c>
     </row>
     <row r="19">
@@ -1355,20 +1337,22 @@
           <t>당기순이익(손실)의 귀속</t>
         </is>
       </c>
-      <c r="B19" s="1" t="inlineStr">
-        <is>
-          <t>지배기업의 소유주에게 귀속되는 당기순이익(손실)</t>
-        </is>
-      </c>
+      <c r="B19" s="1" t="n"/>
       <c r="C19" s="1" t="n"/>
-      <c r="D19" s="1" t="n">
-        <v>14473401</v>
-      </c>
-      <c r="E19" s="1" t="n">
-        <v>54730018</v>
-      </c>
-      <c r="F19" s="1" t="n">
-        <v>39243791</v>
+      <c r="D19" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E19" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F19" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="G19" s="7" t="inlineStr">
         <is>
@@ -1385,23 +1369,35 @@
           <t>-</t>
         </is>
       </c>
-      <c r="J19" s="1" t="n">
-        <v>14473401</v>
-      </c>
-      <c r="K19" s="1" t="n">
-        <v>54730018</v>
-      </c>
-      <c r="L19" s="1" t="n">
-        <v>39243791</v>
-      </c>
-      <c r="M19" s="1" t="n">
-        <v>14473401</v>
-      </c>
-      <c r="N19" s="1" t="n">
-        <v>54730018</v>
-      </c>
-      <c r="O19" s="1" t="n">
-        <v>39243791</v>
+      <c r="J19" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K19" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L19" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M19" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N19" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O19" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
     </row>
     <row r="20">
@@ -1412,18 +1408,18 @@
       </c>
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>비지배지분에 귀속되는 당기순이익(손실)</t>
+          <t>지배기업소유주지분</t>
         </is>
       </c>
       <c r="C20" s="1" t="n"/>
       <c r="D20" s="1" t="n">
-        <v>1013699</v>
+        <v>11961717</v>
       </c>
       <c r="E20" s="1" t="n">
-        <v>924059</v>
+        <v>7364364</v>
       </c>
       <c r="F20" s="1" t="n">
-        <v>663659</v>
+        <v>4942356</v>
       </c>
       <c r="G20" s="7" t="inlineStr">
         <is>
@@ -1441,22 +1437,22 @@
         </is>
       </c>
       <c r="J20" s="1" t="n">
-        <v>1013699</v>
+        <v>11961717</v>
       </c>
       <c r="K20" s="1" t="n">
-        <v>924059</v>
+        <v>7364364</v>
       </c>
       <c r="L20" s="1" t="n">
-        <v>663659</v>
+        <v>4942356</v>
       </c>
       <c r="M20" s="1" t="n">
-        <v>1013699</v>
+        <v>11961717</v>
       </c>
       <c r="N20" s="1" t="n">
-        <v>924059</v>
+        <v>7364364</v>
       </c>
       <c r="O20" s="1" t="n">
-        <v>663659</v>
+        <v>4942356</v>
       </c>
     </row>
     <row r="21">
@@ -1467,51 +1463,51 @@
       </c>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>지배기업소유주지분</t>
+          <t>비지배지분</t>
         </is>
       </c>
       <c r="C21" s="1" t="n"/>
-      <c r="D21" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E21" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F21" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G21" s="1" t="n">
-        <v>11961717</v>
-      </c>
-      <c r="H21" s="1" t="n">
-        <v>7364364</v>
-      </c>
-      <c r="I21" s="1" t="n">
-        <v>4942356</v>
+      <c r="D21" s="1" t="n">
+        <v>310584</v>
+      </c>
+      <c r="E21" s="1" t="n">
+        <v>619250</v>
+      </c>
+      <c r="F21" s="1" t="n">
+        <v>750721</v>
+      </c>
+      <c r="G21" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H21" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I21" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="J21" s="1" t="n">
-        <v>11961717</v>
+        <v>310584</v>
       </c>
       <c r="K21" s="1" t="n">
-        <v>7364364</v>
+        <v>619250</v>
       </c>
       <c r="L21" s="1" t="n">
-        <v>4942356</v>
+        <v>750721</v>
       </c>
       <c r="M21" s="1" t="n">
-        <v>11961717</v>
+        <v>310584</v>
       </c>
       <c r="N21" s="1" t="n">
-        <v>7364364</v>
+        <v>619250</v>
       </c>
       <c r="O21" s="1" t="n">
-        <v>4942356</v>
+        <v>750721</v>
       </c>
     </row>
     <row r="22">
@@ -1522,7 +1518,7 @@
       </c>
       <c r="B22" s="1" t="inlineStr">
         <is>
-          <t>비지배지분</t>
+          <t>지배기업의 소유주에게 귀속되는 당기순이익(손실)</t>
         </is>
       </c>
       <c r="C22" s="1" t="n"/>
@@ -1542,40 +1538,44 @@
         </is>
       </c>
       <c r="G22" s="1" t="n">
-        <v>310584</v>
+        <v>14473401</v>
       </c>
       <c r="H22" s="1" t="n">
-        <v>619250</v>
+        <v>54730018</v>
       </c>
       <c r="I22" s="1" t="n">
-        <v>750721</v>
+        <v>39243791</v>
       </c>
       <c r="J22" s="1" t="n">
-        <v>310584</v>
+        <v>14473401</v>
       </c>
       <c r="K22" s="1" t="n">
-        <v>619250</v>
+        <v>54730018</v>
       </c>
       <c r="L22" s="1" t="n">
-        <v>750721</v>
+        <v>39243791</v>
       </c>
       <c r="M22" s="1" t="n">
-        <v>310584</v>
+        <v>14473401</v>
       </c>
       <c r="N22" s="1" t="n">
-        <v>619250</v>
+        <v>54730018</v>
       </c>
       <c r="O22" s="1" t="n">
-        <v>750721</v>
+        <v>39243791</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>주당이익</t>
-        </is>
-      </c>
-      <c r="B23" s="1" t="n"/>
+          <t>당기순이익(손실)의 귀속</t>
+        </is>
+      </c>
+      <c r="B23" s="1" t="inlineStr">
+        <is>
+          <t>비지배지분에 귀속되는 당기순이익(손실)</t>
+        </is>
+      </c>
       <c r="C23" s="1" t="n"/>
       <c r="D23" s="7" t="inlineStr">
         <is>
@@ -1592,50 +1592,32 @@
           <t>-</t>
         </is>
       </c>
-      <c r="G23" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H23" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I23" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J23" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K23" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L23" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M23" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N23" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O23" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="G23" s="1" t="n">
+        <v>1013699</v>
+      </c>
+      <c r="H23" s="1" t="n">
+        <v>924059</v>
+      </c>
+      <c r="I23" s="1" t="n">
+        <v>663659</v>
+      </c>
+      <c r="J23" s="1" t="n">
+        <v>1013699</v>
+      </c>
+      <c r="K23" s="1" t="n">
+        <v>924059</v>
+      </c>
+      <c r="L23" s="1" t="n">
+        <v>663659</v>
+      </c>
+      <c r="M23" s="1" t="n">
+        <v>1013699</v>
+      </c>
+      <c r="N23" s="1" t="n">
+        <v>924059</v>
+      </c>
+      <c r="O23" s="1" t="n">
+        <v>663659</v>
       </c>
     </row>
     <row r="24">
@@ -1644,20 +1626,22 @@
           <t>주당이익</t>
         </is>
       </c>
-      <c r="B24" s="1" t="inlineStr">
-        <is>
-          <t>기본주당이익(손실) (단위 : 원)</t>
-        </is>
-      </c>
+      <c r="B24" s="1" t="n"/>
       <c r="C24" s="1" t="n"/>
-      <c r="D24" s="1" t="n">
-        <v>2131</v>
-      </c>
-      <c r="E24" s="1" t="n">
-        <v>8057</v>
-      </c>
-      <c r="F24" s="1" t="n">
-        <v>5777</v>
+      <c r="D24" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E24" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F24" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="G24" s="7" t="inlineStr">
         <is>
@@ -1674,23 +1658,35 @@
           <t>-</t>
         </is>
       </c>
-      <c r="J24" s="1" t="n">
-        <v>2131</v>
-      </c>
-      <c r="K24" s="1" t="n">
-        <v>8057</v>
-      </c>
-      <c r="L24" s="1" t="n">
-        <v>5777</v>
-      </c>
-      <c r="M24" s="1" t="n">
-        <v>2131</v>
-      </c>
-      <c r="N24" s="1" t="n">
-        <v>8057</v>
-      </c>
-      <c r="O24" s="1" t="n">
-        <v>5777</v>
+      <c r="J24" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K24" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L24" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M24" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N24" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O24" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
     </row>
     <row r="25">
@@ -1701,18 +1697,24 @@
       </c>
       <c r="B25" s="1" t="inlineStr">
         <is>
-          <t>희석주당이익(손실) (단위 : 원)</t>
+          <t>기본주당이익 (단위 :원)</t>
         </is>
       </c>
       <c r="C25" s="1" t="n"/>
-      <c r="D25" s="1" t="n">
-        <v>2131</v>
-      </c>
-      <c r="E25" s="1" t="n">
-        <v>8057</v>
-      </c>
-      <c r="F25" s="1" t="n">
-        <v>5777</v>
+      <c r="D25" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E25" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F25" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="G25" s="7" t="inlineStr">
         <is>
@@ -1729,23 +1731,35 @@
           <t>-</t>
         </is>
       </c>
-      <c r="J25" s="1" t="n">
-        <v>2131</v>
-      </c>
-      <c r="K25" s="1" t="n">
-        <v>8057</v>
-      </c>
-      <c r="L25" s="1" t="n">
-        <v>5777</v>
-      </c>
-      <c r="M25" s="1" t="n">
-        <v>2131</v>
-      </c>
-      <c r="N25" s="1" t="n">
-        <v>8057</v>
-      </c>
-      <c r="O25" s="1" t="n">
-        <v>5777</v>
+      <c r="J25" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K25" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L25" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M25" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N25" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O25" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
     </row>
     <row r="26">
@@ -1759,21 +1773,19 @@
           <t>기본주당이익 (단위 :원)</t>
         </is>
       </c>
-      <c r="C26" s="1" t="n"/>
-      <c r="D26" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E26" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F26" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="C26" s="1" t="inlineStr">
+        <is>
+          <t>보통주기본주당이익(손실) (단위 : 원)</t>
+        </is>
+      </c>
+      <c r="D26" s="1" t="n">
+        <v>45703</v>
+      </c>
+      <c r="E26" s="1" t="n">
+        <v>28521</v>
+      </c>
+      <c r="F26" s="1" t="n">
+        <v>18979</v>
       </c>
       <c r="G26" s="7" t="inlineStr">
         <is>
@@ -1790,35 +1802,23 @@
           <t>-</t>
         </is>
       </c>
-      <c r="J26" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K26" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L26" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M26" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N26" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O26" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="J26" s="1" t="n">
+        <v>45703</v>
+      </c>
+      <c r="K26" s="1" t="n">
+        <v>28521</v>
+      </c>
+      <c r="L26" s="1" t="n">
+        <v>18979</v>
+      </c>
+      <c r="M26" s="1" t="n">
+        <v>45703</v>
+      </c>
+      <c r="N26" s="1" t="n">
+        <v>28521</v>
+      </c>
+      <c r="O26" s="1" t="n">
+        <v>18979</v>
       </c>
     </row>
     <row r="27">
@@ -1834,50 +1834,50 @@
       </c>
       <c r="C27" s="1" t="inlineStr">
         <is>
-          <t>보통주기본주당이익(손실) (단위 : 원)</t>
-        </is>
-      </c>
-      <c r="D27" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E27" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F27" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G27" s="1" t="n">
-        <v>45703</v>
-      </c>
-      <c r="H27" s="1" t="n">
-        <v>28521</v>
-      </c>
-      <c r="I27" s="1" t="n">
-        <v>18979</v>
+          <t>계속영업 보통주기본주당이익(손실) (단위: 원)</t>
+        </is>
+      </c>
+      <c r="D27" s="1" t="n">
+        <v>47622</v>
+      </c>
+      <c r="E27" s="1" t="n">
+        <v>29105</v>
+      </c>
+      <c r="F27" s="1" t="n">
+        <v>18521</v>
+      </c>
+      <c r="G27" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H27" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I27" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="J27" s="1" t="n">
-        <v>45703</v>
+        <v>47622</v>
       </c>
       <c r="K27" s="1" t="n">
-        <v>28521</v>
+        <v>29105</v>
       </c>
       <c r="L27" s="1" t="n">
-        <v>18979</v>
+        <v>18521</v>
       </c>
       <c r="M27" s="1" t="n">
-        <v>45703</v>
+        <v>47622</v>
       </c>
       <c r="N27" s="1" t="n">
-        <v>28521</v>
+        <v>29105</v>
       </c>
       <c r="O27" s="1" t="n">
-        <v>18979</v>
+        <v>18521</v>
       </c>
     </row>
     <row r="28">
@@ -1893,50 +1893,50 @@
       </c>
       <c r="C28" s="1" t="inlineStr">
         <is>
-          <t>계속영업 보통주기본주당이익(손실) (단위: 원)</t>
-        </is>
-      </c>
-      <c r="D28" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E28" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F28" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G28" s="1" t="n">
-        <v>47622</v>
-      </c>
-      <c r="H28" s="1" t="n">
-        <v>29105</v>
-      </c>
-      <c r="I28" s="1" t="n">
-        <v>18521</v>
+          <t>중단영업 보통주기본주당이익(손실) (단위: 원)</t>
+        </is>
+      </c>
+      <c r="D28" s="1" t="n">
+        <v>-1919</v>
+      </c>
+      <c r="E28" s="1" t="n">
+        <v>-584</v>
+      </c>
+      <c r="F28" s="1" t="n">
+        <v>458</v>
+      </c>
+      <c r="G28" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H28" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I28" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="J28" s="1" t="n">
-        <v>47622</v>
+        <v>-1919</v>
       </c>
       <c r="K28" s="1" t="n">
-        <v>29105</v>
+        <v>-584</v>
       </c>
       <c r="L28" s="1" t="n">
-        <v>18521</v>
+        <v>458</v>
       </c>
       <c r="M28" s="1" t="n">
-        <v>47622</v>
+        <v>-1919</v>
       </c>
       <c r="N28" s="1" t="n">
-        <v>29105</v>
+        <v>-584</v>
       </c>
       <c r="O28" s="1" t="n">
-        <v>18521</v>
+        <v>458</v>
       </c>
     </row>
     <row r="29">
@@ -1952,50 +1952,50 @@
       </c>
       <c r="C29" s="1" t="inlineStr">
         <is>
-          <t>중단영업 보통주기본주당이익(손실) (단위: 원)</t>
-        </is>
-      </c>
-      <c r="D29" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E29" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F29" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G29" s="1" t="n">
-        <v>-1919</v>
-      </c>
-      <c r="H29" s="1" t="n">
-        <v>-584</v>
-      </c>
-      <c r="I29" s="1" t="n">
-        <v>458</v>
+          <t>1우선주 기본주당이익(손실) (단위 : 원)</t>
+        </is>
+      </c>
+      <c r="D29" s="1" t="n">
+        <v>45535</v>
+      </c>
+      <c r="E29" s="1" t="n">
+        <v>28207</v>
+      </c>
+      <c r="F29" s="1" t="n">
+        <v>19002</v>
+      </c>
+      <c r="G29" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H29" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I29" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="J29" s="1" t="n">
-        <v>-1919</v>
+        <v>45535</v>
       </c>
       <c r="K29" s="1" t="n">
-        <v>-584</v>
+        <v>28207</v>
       </c>
       <c r="L29" s="1" t="n">
-        <v>458</v>
+        <v>19002</v>
       </c>
       <c r="M29" s="1" t="n">
-        <v>-1919</v>
+        <v>45535</v>
       </c>
       <c r="N29" s="1" t="n">
-        <v>-584</v>
+        <v>28207</v>
       </c>
       <c r="O29" s="1" t="n">
-        <v>458</v>
+        <v>19002</v>
       </c>
     </row>
     <row r="30">
@@ -2011,50 +2011,50 @@
       </c>
       <c r="C30" s="1" t="inlineStr">
         <is>
-          <t>1우선주 기본주당이익(손실) (단위 : 원)</t>
-        </is>
-      </c>
-      <c r="D30" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E30" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F30" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G30" s="1" t="n">
-        <v>45535</v>
-      </c>
-      <c r="H30" s="1" t="n">
-        <v>28207</v>
-      </c>
-      <c r="I30" s="1" t="n">
-        <v>19002</v>
+          <t>계속영업 1우선주기본주당이익(손실) (단위 : 원)</t>
+        </is>
+      </c>
+      <c r="D30" s="1" t="n">
+        <v>47445</v>
+      </c>
+      <c r="E30" s="1" t="n">
+        <v>28783</v>
+      </c>
+      <c r="F30" s="1" t="n">
+        <v>18545</v>
+      </c>
+      <c r="G30" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H30" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I30" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="J30" s="1" t="n">
-        <v>45535</v>
+        <v>47445</v>
       </c>
       <c r="K30" s="1" t="n">
-        <v>28207</v>
+        <v>28783</v>
       </c>
       <c r="L30" s="1" t="n">
-        <v>19002</v>
+        <v>18545</v>
       </c>
       <c r="M30" s="1" t="n">
-        <v>45535</v>
+        <v>47445</v>
       </c>
       <c r="N30" s="1" t="n">
-        <v>28207</v>
+        <v>28783</v>
       </c>
       <c r="O30" s="1" t="n">
-        <v>19002</v>
+        <v>18545</v>
       </c>
     </row>
     <row r="31">
@@ -2070,50 +2070,50 @@
       </c>
       <c r="C31" s="1" t="inlineStr">
         <is>
-          <t>계속영업 1우선주기본주당이익(손실) (단위 : 원)</t>
-        </is>
-      </c>
-      <c r="D31" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E31" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F31" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G31" s="1" t="n">
-        <v>47445</v>
-      </c>
-      <c r="H31" s="1" t="n">
-        <v>28783</v>
-      </c>
-      <c r="I31" s="1" t="n">
-        <v>18545</v>
+          <t>중단영업 1우선주기본주당이익(손실) (단위 : 원)</t>
+        </is>
+      </c>
+      <c r="D31" s="1" t="n">
+        <v>-1910</v>
+      </c>
+      <c r="E31" s="1" t="n">
+        <v>-576</v>
+      </c>
+      <c r="F31" s="1" t="n">
+        <v>457</v>
+      </c>
+      <c r="G31" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H31" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I31" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="J31" s="1" t="n">
-        <v>47445</v>
+        <v>-1910</v>
       </c>
       <c r="K31" s="1" t="n">
-        <v>28783</v>
+        <v>-576</v>
       </c>
       <c r="L31" s="1" t="n">
-        <v>18545</v>
+        <v>457</v>
       </c>
       <c r="M31" s="1" t="n">
-        <v>47445</v>
+        <v>-1910</v>
       </c>
       <c r="N31" s="1" t="n">
-        <v>28783</v>
+        <v>-576</v>
       </c>
       <c r="O31" s="1" t="n">
-        <v>18545</v>
+        <v>457</v>
       </c>
     </row>
     <row r="32">
@@ -2124,14 +2124,10 @@
       </c>
       <c r="B32" s="1" t="inlineStr">
         <is>
-          <t>기본주당이익 (단위 :원)</t>
-        </is>
-      </c>
-      <c r="C32" s="1" t="inlineStr">
-        <is>
-          <t>중단영업 1우선주기본주당이익(손실) (단위 : 원)</t>
-        </is>
-      </c>
+          <t>희석주당이익(손실)(단위 : 원)</t>
+        </is>
+      </c>
+      <c r="C32" s="1" t="n"/>
       <c r="D32" s="7" t="inlineStr">
         <is>
           <t>-</t>
@@ -2147,32 +2143,50 @@
           <t>-</t>
         </is>
       </c>
-      <c r="G32" s="1" t="n">
-        <v>-1910</v>
-      </c>
-      <c r="H32" s="1" t="n">
-        <v>-576</v>
-      </c>
-      <c r="I32" s="1" t="n">
-        <v>457</v>
-      </c>
-      <c r="J32" s="1" t="n">
-        <v>-1910</v>
-      </c>
-      <c r="K32" s="1" t="n">
-        <v>-576</v>
-      </c>
-      <c r="L32" s="1" t="n">
-        <v>457</v>
-      </c>
-      <c r="M32" s="1" t="n">
-        <v>-1910</v>
-      </c>
-      <c r="N32" s="1" t="n">
-        <v>-576</v>
-      </c>
-      <c r="O32" s="1" t="n">
-        <v>457</v>
+      <c r="G32" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H32" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I32" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J32" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K32" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L32" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M32" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N32" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O32" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
     </row>
     <row r="33">
@@ -2186,21 +2200,19 @@
           <t>희석주당이익(손실)(단위 : 원)</t>
         </is>
       </c>
-      <c r="C33" s="1" t="n"/>
-      <c r="D33" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E33" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F33" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="C33" s="1" t="inlineStr">
+        <is>
+          <t>보통주 희석주당이익 (단위 : 원)</t>
+        </is>
+      </c>
+      <c r="D33" s="1" t="n">
+        <v>45703</v>
+      </c>
+      <c r="E33" s="1" t="n">
+        <v>28521</v>
+      </c>
+      <c r="F33" s="1" t="n">
+        <v>18979</v>
       </c>
       <c r="G33" s="7" t="inlineStr">
         <is>
@@ -2217,35 +2229,23 @@
           <t>-</t>
         </is>
       </c>
-      <c r="J33" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K33" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L33" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M33" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N33" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O33" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="J33" s="1" t="n">
+        <v>45703</v>
+      </c>
+      <c r="K33" s="1" t="n">
+        <v>28521</v>
+      </c>
+      <c r="L33" s="1" t="n">
+        <v>18979</v>
+      </c>
+      <c r="M33" s="1" t="n">
+        <v>45703</v>
+      </c>
+      <c r="N33" s="1" t="n">
+        <v>28521</v>
+      </c>
+      <c r="O33" s="1" t="n">
+        <v>18979</v>
       </c>
     </row>
     <row r="34">
@@ -2261,50 +2261,50 @@
       </c>
       <c r="C34" s="1" t="inlineStr">
         <is>
-          <t>보통주 희석주당이익 (단위 : 원)</t>
-        </is>
-      </c>
-      <c r="D34" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E34" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F34" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G34" s="1" t="n">
-        <v>45703</v>
-      </c>
-      <c r="H34" s="1" t="n">
-        <v>28521</v>
-      </c>
-      <c r="I34" s="1" t="n">
-        <v>18979</v>
+          <t>1우선주 희석주당이익 (단위 : 원)</t>
+        </is>
+      </c>
+      <c r="D34" s="1" t="n">
+        <v>45535</v>
+      </c>
+      <c r="E34" s="1" t="n">
+        <v>28207</v>
+      </c>
+      <c r="F34" s="1" t="n">
+        <v>19002</v>
+      </c>
+      <c r="G34" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H34" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I34" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="J34" s="1" t="n">
-        <v>45703</v>
+        <v>45535</v>
       </c>
       <c r="K34" s="1" t="n">
-        <v>28521</v>
+        <v>28207</v>
       </c>
       <c r="L34" s="1" t="n">
-        <v>18979</v>
+        <v>19002</v>
       </c>
       <c r="M34" s="1" t="n">
-        <v>45703</v>
+        <v>45535</v>
       </c>
       <c r="N34" s="1" t="n">
-        <v>28521</v>
+        <v>28207</v>
       </c>
       <c r="O34" s="1" t="n">
-        <v>18979</v>
+        <v>19002</v>
       </c>
     </row>
     <row r="35">
@@ -2315,14 +2315,10 @@
       </c>
       <c r="B35" s="1" t="inlineStr">
         <is>
-          <t>희석주당이익(손실)(단위 : 원)</t>
-        </is>
-      </c>
-      <c r="C35" s="1" t="inlineStr">
-        <is>
-          <t>1우선주 희석주당이익 (단위 : 원)</t>
-        </is>
-      </c>
+          <t>기본주당이익(손실) (단위 : 원)</t>
+        </is>
+      </c>
+      <c r="C35" s="1" t="n"/>
       <c r="D35" s="7" t="inlineStr">
         <is>
           <t>-</t>
@@ -2339,40 +2335,44 @@
         </is>
       </c>
       <c r="G35" s="1" t="n">
-        <v>45535</v>
+        <v>2131</v>
       </c>
       <c r="H35" s="1" t="n">
-        <v>28207</v>
+        <v>8057</v>
       </c>
       <c r="I35" s="1" t="n">
-        <v>19002</v>
+        <v>5777</v>
       </c>
       <c r="J35" s="1" t="n">
-        <v>45535</v>
+        <v>2131</v>
       </c>
       <c r="K35" s="1" t="n">
-        <v>28207</v>
+        <v>8057</v>
       </c>
       <c r="L35" s="1" t="n">
-        <v>19002</v>
+        <v>5777</v>
       </c>
       <c r="M35" s="1" t="n">
-        <v>45535</v>
+        <v>2131</v>
       </c>
       <c r="N35" s="1" t="n">
-        <v>28207</v>
+        <v>8057</v>
       </c>
       <c r="O35" s="1" t="n">
-        <v>19002</v>
+        <v>5777</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>매출액</t>
-        </is>
-      </c>
-      <c r="B36" s="1" t="n"/>
+          <t>주당이익</t>
+        </is>
+      </c>
+      <c r="B36" s="1" t="inlineStr">
+        <is>
+          <t>희석주당이익(손실) (단위 : 원)</t>
+        </is>
+      </c>
       <c r="C36" s="1" t="n"/>
       <c r="D36" s="7" t="inlineStr">
         <is>
@@ -2390,37 +2390,37 @@
         </is>
       </c>
       <c r="G36" s="1" t="n">
-        <v>162663579</v>
+        <v>2131</v>
       </c>
       <c r="H36" s="1" t="n">
-        <v>142151469</v>
+        <v>8057</v>
       </c>
       <c r="I36" s="1" t="n">
-        <v>116448159</v>
+        <v>5777</v>
       </c>
       <c r="J36" s="1" t="n">
-        <v>162663579</v>
+        <v>2131</v>
       </c>
       <c r="K36" s="1" t="n">
-        <v>142151469</v>
+        <v>8057</v>
       </c>
       <c r="L36" s="1" t="n">
-        <v>116448159</v>
+        <v>5777</v>
       </c>
       <c r="M36" s="1" t="n">
-        <v>162663579</v>
+        <v>2131</v>
       </c>
       <c r="N36" s="1" t="n">
-        <v>142151469</v>
+        <v>8057</v>
       </c>
       <c r="O36" s="1" t="n">
-        <v>116448159</v>
+        <v>5777</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>공동기업및관계기업투자손익</t>
+          <t>영업수익</t>
         </is>
       </c>
       <c r="B37" s="1" t="n"/>
@@ -2441,37 +2441,37 @@
         </is>
       </c>
       <c r="G37" s="1" t="n">
-        <v>2470933</v>
+        <v>258935494</v>
       </c>
       <c r="H37" s="1" t="n">
-        <v>1557630</v>
+        <v>302231360</v>
       </c>
       <c r="I37" s="1" t="n">
-        <v>1302150</v>
+        <v>279604799</v>
       </c>
       <c r="J37" s="1" t="n">
-        <v>2470933</v>
+        <v>258935494</v>
       </c>
       <c r="K37" s="1" t="n">
-        <v>1557630</v>
+        <v>302231360</v>
       </c>
       <c r="L37" s="1" t="n">
-        <v>1302150</v>
+        <v>279604799</v>
       </c>
       <c r="M37" s="1" t="n">
-        <v>2470933</v>
+        <v>258935494</v>
       </c>
       <c r="N37" s="1" t="n">
-        <v>1557630</v>
+        <v>302231360</v>
       </c>
       <c r="O37" s="1" t="n">
-        <v>1302150</v>
+        <v>279604799</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>기타수익</t>
+          <t>기타이익</t>
         </is>
       </c>
       <c r="B38" s="1" t="n"/>
@@ -2492,37 +2492,37 @@
         </is>
       </c>
       <c r="G38" s="1" t="n">
-        <v>1782333</v>
+        <v>1180448</v>
       </c>
       <c r="H38" s="1" t="n">
-        <v>1930914</v>
+        <v>1962071</v>
       </c>
       <c r="I38" s="1" t="n">
-        <v>1377997</v>
+        <v>2205695</v>
       </c>
       <c r="J38" s="1" t="n">
-        <v>1782333</v>
+        <v>1180448</v>
       </c>
       <c r="K38" s="1" t="n">
-        <v>1930914</v>
+        <v>1962071</v>
       </c>
       <c r="L38" s="1" t="n">
-        <v>1377997</v>
+        <v>2205695</v>
       </c>
       <c r="M38" s="1" t="n">
-        <v>1782333</v>
+        <v>1180448</v>
       </c>
       <c r="N38" s="1" t="n">
-        <v>1930914</v>
+        <v>1962071</v>
       </c>
       <c r="O38" s="1" t="n">
-        <v>1377997</v>
+        <v>2205695</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>기타비용</t>
+          <t>기타손실</t>
         </is>
       </c>
       <c r="B39" s="1" t="n"/>
@@ -2543,37 +2543,37 @@
         </is>
       </c>
       <c r="G39" s="1" t="n">
-        <v>2350343</v>
+        <v>1083327</v>
       </c>
       <c r="H39" s="1" t="n">
-        <v>2238256</v>
+        <v>1790176</v>
       </c>
       <c r="I39" s="1" t="n">
-        <v>1745985</v>
+        <v>2055971</v>
       </c>
       <c r="J39" s="1" t="n">
-        <v>2350343</v>
+        <v>1083327</v>
       </c>
       <c r="K39" s="1" t="n">
-        <v>2238256</v>
+        <v>1790176</v>
       </c>
       <c r="L39" s="1" t="n">
-        <v>1745985</v>
+        <v>2055971</v>
       </c>
       <c r="M39" s="1" t="n">
-        <v>2350343</v>
+        <v>1083327</v>
       </c>
       <c r="N39" s="1" t="n">
-        <v>2238256</v>
+        <v>1790176</v>
       </c>
       <c r="O39" s="1" t="n">
-        <v>1745985</v>
+        <v>2055971</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>법인세비용차감전순이익</t>
+          <t>지분법이익</t>
         </is>
       </c>
       <c r="B40" s="1" t="n"/>
@@ -2594,37 +2594,37 @@
         </is>
       </c>
       <c r="G40" s="1" t="n">
-        <v>17618662</v>
+        <v>887550</v>
       </c>
       <c r="H40" s="1" t="n">
-        <v>11181471</v>
+        <v>1090643</v>
       </c>
       <c r="I40" s="1" t="n">
-        <v>7789043</v>
+        <v>729614</v>
       </c>
       <c r="J40" s="1" t="n">
-        <v>17618662</v>
+        <v>887550</v>
       </c>
       <c r="K40" s="1" t="n">
-        <v>11181471</v>
+        <v>1090643</v>
       </c>
       <c r="L40" s="1" t="n">
-        <v>7789043</v>
+        <v>729614</v>
       </c>
       <c r="M40" s="1" t="n">
-        <v>17618662</v>
+        <v>887550</v>
       </c>
       <c r="N40" s="1" t="n">
-        <v>11181471</v>
+        <v>1090643</v>
       </c>
       <c r="O40" s="1" t="n">
-        <v>7789043</v>
+        <v>729614</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>계속영업연결당기순이익</t>
+          <t>법인세비용차감전순이익(손실)</t>
         </is>
       </c>
       <c r="B41" s="1" t="n"/>
@@ -2645,37 +2645,37 @@
         </is>
       </c>
       <c r="G41" s="1" t="n">
-        <v>12992022</v>
+        <v>11006265</v>
       </c>
       <c r="H41" s="1" t="n">
-        <v>8202303</v>
+        <v>46440474</v>
       </c>
       <c r="I41" s="1" t="n">
-        <v>5522220</v>
+        <v>53351827</v>
       </c>
       <c r="J41" s="1" t="n">
-        <v>12992022</v>
+        <v>11006265</v>
       </c>
       <c r="K41" s="1" t="n">
-        <v>8202303</v>
+        <v>46440474</v>
       </c>
       <c r="L41" s="1" t="n">
-        <v>5522220</v>
+        <v>53351827</v>
       </c>
       <c r="M41" s="1" t="n">
-        <v>12992022</v>
+        <v>11006265</v>
       </c>
       <c r="N41" s="1" t="n">
-        <v>8202303</v>
+        <v>46440474</v>
       </c>
       <c r="O41" s="1" t="n">
-        <v>5522220</v>
+        <v>53351827</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>중단영업당기순이익(손실)</t>
+          <t>계속영업이익(손실)</t>
         </is>
       </c>
       <c r="B42" s="1" t="n"/>
@@ -2696,37 +2696,37 @@
         </is>
       </c>
       <c r="G42" s="1" t="n">
-        <v>-719721</v>
+        <v>15487100</v>
       </c>
       <c r="H42" s="1" t="n">
-        <v>-218689</v>
+        <v>55654077</v>
       </c>
       <c r="I42" s="1" t="n">
-        <v>170857</v>
+        <v>39907450</v>
       </c>
       <c r="J42" s="1" t="n">
-        <v>-719721</v>
+        <v>15487100</v>
       </c>
       <c r="K42" s="1" t="n">
-        <v>-218689</v>
+        <v>55654077</v>
       </c>
       <c r="L42" s="1" t="n">
-        <v>170857</v>
+        <v>39907450</v>
       </c>
       <c r="M42" s="1" t="n">
-        <v>-719721</v>
+        <v>15487100</v>
       </c>
       <c r="N42" s="1" t="n">
-        <v>-218689</v>
+        <v>55654077</v>
       </c>
       <c r="O42" s="1" t="n">
-        <v>170857</v>
+        <v>39907450</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>연결당기순이익</t>
+          <t>당기순이익(손실)</t>
         </is>
       </c>
       <c r="B43" s="1" t="n"/>
@@ -2747,31 +2747,31 @@
         </is>
       </c>
       <c r="G43" s="1" t="n">
-        <v>12272301</v>
+        <v>15487100</v>
       </c>
       <c r="H43" s="1" t="n">
-        <v>7983614</v>
+        <v>55654077</v>
       </c>
       <c r="I43" s="1" t="n">
-        <v>5693077</v>
+        <v>39907450</v>
       </c>
       <c r="J43" s="1" t="n">
-        <v>12272301</v>
+        <v>15487100</v>
       </c>
       <c r="K43" s="1" t="n">
-        <v>7983614</v>
+        <v>55654077</v>
       </c>
       <c r="L43" s="1" t="n">
-        <v>5693077</v>
+        <v>39907450</v>
       </c>
       <c r="M43" s="1" t="n">
-        <v>12272301</v>
+        <v>15487100</v>
       </c>
       <c r="N43" s="1" t="n">
-        <v>7983614</v>
+        <v>55654077</v>
       </c>
       <c r="O43" s="1" t="n">
-        <v>5693077</v>
+        <v>39907450</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
disable .xlsx download buttons when db is not matched
폴더내에 쓸데없어진 메모나 배치파일 등등 들도 다 정리함.
</commit_message>
<xml_diff>
--- a/data/output/연결 손익계산서.xlsx
+++ b/data/output/연결 손익계산서.xlsx
@@ -499,14 +499,14 @@
       <c r="C1" s="3" t="n"/>
       <c r="D1" s="4" t="inlineStr">
         <is>
-          <t>Hyundai</t>
+          <t>Samsung</t>
         </is>
       </c>
       <c r="E1" s="1" t="n"/>
       <c r="F1" s="1" t="n"/>
       <c r="G1" s="4" t="inlineStr">
         <is>
-          <t>Samsung</t>
+          <t>Hyundai</t>
         </is>
       </c>
       <c r="H1" s="1" t="n"/>
@@ -611,19 +611,19 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>매출액</t>
+          <t>영업수익</t>
         </is>
       </c>
       <c r="B4" s="1" t="n"/>
       <c r="C4" s="1" t="n"/>
       <c r="D4" s="1" t="n">
-        <v>162663579</v>
+        <v>258935494</v>
       </c>
       <c r="E4" s="1" t="n">
-        <v>142151469</v>
+        <v>302231360</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>116448159</v>
+        <v>279604799</v>
       </c>
       <c r="G4" s="7" t="inlineStr">
         <is>
@@ -641,22 +641,22 @@
         </is>
       </c>
       <c r="J4" s="1" t="n">
-        <v>162663579</v>
+        <v>258935494</v>
       </c>
       <c r="K4" s="1" t="n">
-        <v>142151469</v>
+        <v>302231360</v>
       </c>
       <c r="L4" s="1" t="n">
-        <v>116448159</v>
+        <v>279604799</v>
       </c>
       <c r="M4" s="1" t="n">
-        <v>162663579</v>
+        <v>258935494</v>
       </c>
       <c r="N4" s="1" t="n">
-        <v>142151469</v>
+        <v>302231360</v>
       </c>
       <c r="O4" s="1" t="n">
-        <v>116448159</v>
+        <v>279604799</v>
       </c>
     </row>
     <row r="5">
@@ -668,22 +668,22 @@
       <c r="B5" s="1" t="n"/>
       <c r="C5" s="1" t="n"/>
       <c r="D5" s="1" t="n">
+        <v>180388580</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>190041770</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>166411342</v>
+      </c>
+      <c r="G5" s="1" t="n">
         <v>129179183</v>
       </c>
-      <c r="E5" s="1" t="n">
+      <c r="H5" s="1" t="n">
         <v>113879569</v>
       </c>
-      <c r="F5" s="1" t="n">
+      <c r="I5" s="1" t="n">
         <v>94721313</v>
-      </c>
-      <c r="G5" s="1" t="n">
-        <v>180388580</v>
-      </c>
-      <c r="H5" s="1" t="n">
-        <v>190041770</v>
-      </c>
-      <c r="I5" s="1" t="n">
-        <v>166411342</v>
       </c>
       <c r="J5" s="1" t="n">
         <v>309567763</v>
@@ -713,22 +713,22 @@
       <c r="B6" s="1" t="n"/>
       <c r="C6" s="1" t="n"/>
       <c r="D6" s="1" t="n">
+        <v>78546914</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>112189590</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>113193457</v>
+      </c>
+      <c r="G6" s="1" t="n">
         <v>33484396</v>
       </c>
-      <c r="E6" s="1" t="n">
+      <c r="H6" s="1" t="n">
         <v>28271900</v>
       </c>
-      <c r="F6" s="1" t="n">
+      <c r="I6" s="1" t="n">
         <v>21726846</v>
-      </c>
-      <c r="G6" s="1" t="n">
-        <v>78546914</v>
-      </c>
-      <c r="H6" s="1" t="n">
-        <v>112189590</v>
-      </c>
-      <c r="I6" s="1" t="n">
-        <v>113193457</v>
       </c>
       <c r="J6" s="1" t="n">
         <v>112031310</v>
@@ -758,22 +758,22 @@
       <c r="B7" s="1" t="n"/>
       <c r="C7" s="1" t="n"/>
       <c r="D7" s="1" t="n">
+        <v>71979938</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>68812960</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>61559601</v>
+      </c>
+      <c r="G7" s="1" t="n">
         <v>18357495</v>
       </c>
-      <c r="E7" s="1" t="n">
+      <c r="H7" s="1" t="n">
         <v>18446972</v>
       </c>
-      <c r="F7" s="1" t="n">
+      <c r="I7" s="1" t="n">
         <v>15200325</v>
-      </c>
-      <c r="G7" s="1" t="n">
-        <v>71979938</v>
-      </c>
-      <c r="H7" s="1" t="n">
-        <v>68812960</v>
-      </c>
-      <c r="I7" s="1" t="n">
-        <v>61559601</v>
       </c>
       <c r="J7" s="1" t="n">
         <v>90337433</v>
@@ -803,22 +803,22 @@
       <c r="B8" s="1" t="n"/>
       <c r="C8" s="1" t="n"/>
       <c r="D8" s="1" t="n">
+        <v>6566976</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>43376630</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>51633856</v>
+      </c>
+      <c r="G8" s="1" t="n">
         <v>15126901</v>
       </c>
-      <c r="E8" s="1" t="n">
+      <c r="H8" s="1" t="n">
         <v>9824928</v>
       </c>
-      <c r="F8" s="1" t="n">
+      <c r="I8" s="1" t="n">
         <v>6526521</v>
-      </c>
-      <c r="G8" s="1" t="n">
-        <v>6566976</v>
-      </c>
-      <c r="H8" s="1" t="n">
-        <v>43376630</v>
-      </c>
-      <c r="I8" s="1" t="n">
-        <v>51633856</v>
       </c>
       <c r="J8" s="1" t="n">
         <v>21693877</v>
@@ -842,19 +842,19 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>공동기업및관계기업투자손익</t>
+          <t>기타이익</t>
         </is>
       </c>
       <c r="B9" s="1" t="n"/>
       <c r="C9" s="1" t="n"/>
       <c r="D9" s="1" t="n">
-        <v>2470933</v>
+        <v>1180448</v>
       </c>
       <c r="E9" s="1" t="n">
-        <v>1557630</v>
+        <v>1962071</v>
       </c>
       <c r="F9" s="1" t="n">
-        <v>1302150</v>
+        <v>2205695</v>
       </c>
       <c r="G9" s="7" t="inlineStr">
         <is>
@@ -872,232 +872,232 @@
         </is>
       </c>
       <c r="J9" s="1" t="n">
-        <v>2470933</v>
+        <v>1180448</v>
       </c>
       <c r="K9" s="1" t="n">
-        <v>1557630</v>
+        <v>1962071</v>
       </c>
       <c r="L9" s="1" t="n">
-        <v>1302150</v>
+        <v>2205695</v>
       </c>
       <c r="M9" s="1" t="n">
-        <v>2470933</v>
+        <v>1180448</v>
       </c>
       <c r="N9" s="1" t="n">
-        <v>1557630</v>
+        <v>1962071</v>
       </c>
       <c r="O9" s="1" t="n">
-        <v>1302150</v>
+        <v>2205695</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>금융수익</t>
+          <t>기타손실</t>
         </is>
       </c>
       <c r="B10" s="1" t="n"/>
       <c r="C10" s="1" t="n"/>
       <c r="D10" s="1" t="n">
-        <v>1559538</v>
+        <v>1083327</v>
       </c>
       <c r="E10" s="1" t="n">
-        <v>985893</v>
+        <v>1790176</v>
       </c>
       <c r="F10" s="1" t="n">
-        <v>841196</v>
-      </c>
-      <c r="G10" s="1" t="n">
-        <v>16100148</v>
-      </c>
-      <c r="H10" s="1" t="n">
-        <v>20828995</v>
-      </c>
-      <c r="I10" s="1" t="n">
-        <v>8543187</v>
+        <v>2055971</v>
+      </c>
+      <c r="G10" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H10" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I10" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="J10" s="1" t="n">
-        <v>17659686</v>
+        <v>1083327</v>
       </c>
       <c r="K10" s="1" t="n">
-        <v>21814888</v>
+        <v>1790176</v>
       </c>
       <c r="L10" s="1" t="n">
-        <v>9384383</v>
+        <v>2055971</v>
       </c>
       <c r="M10" s="1" t="n">
-        <v>8829843</v>
+        <v>1083327</v>
       </c>
       <c r="N10" s="1" t="n">
-        <v>10907444</v>
+        <v>1790176</v>
       </c>
       <c r="O10" s="1" t="n">
-        <v>4692191.5</v>
+        <v>2055971</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>금융비용</t>
+          <t>지분법이익</t>
         </is>
       </c>
       <c r="B11" s="1" t="n"/>
       <c r="C11" s="1" t="n"/>
       <c r="D11" s="1" t="n">
-        <v>970700</v>
+        <v>887550</v>
       </c>
       <c r="E11" s="1" t="n">
-        <v>879638</v>
+        <v>1090643</v>
       </c>
       <c r="F11" s="1" t="n">
-        <v>512836</v>
-      </c>
-      <c r="G11" s="1" t="n">
-        <v>12645530</v>
-      </c>
-      <c r="H11" s="1" t="n">
-        <v>19027689</v>
-      </c>
-      <c r="I11" s="1" t="n">
-        <v>7704554</v>
+        <v>729614</v>
+      </c>
+      <c r="G11" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H11" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I11" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="J11" s="1" t="n">
-        <v>13616230</v>
+        <v>887550</v>
       </c>
       <c r="K11" s="1" t="n">
-        <v>19907327</v>
+        <v>1090643</v>
       </c>
       <c r="L11" s="1" t="n">
-        <v>8217390</v>
+        <v>729614</v>
       </c>
       <c r="M11" s="1" t="n">
-        <v>6808115</v>
+        <v>887550</v>
       </c>
       <c r="N11" s="1" t="n">
-        <v>9953663.5</v>
+        <v>1090643</v>
       </c>
       <c r="O11" s="1" t="n">
-        <v>4108695</v>
+        <v>729614</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>기타수익</t>
+          <t>금융수익</t>
         </is>
       </c>
       <c r="B12" s="1" t="n"/>
       <c r="C12" s="1" t="n"/>
       <c r="D12" s="1" t="n">
-        <v>1782333</v>
+        <v>16100148</v>
       </c>
       <c r="E12" s="1" t="n">
-        <v>1930914</v>
+        <v>20828995</v>
       </c>
       <c r="F12" s="1" t="n">
-        <v>1377997</v>
-      </c>
-      <c r="G12" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H12" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I12" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>8543187</v>
+      </c>
+      <c r="G12" s="1" t="n">
+        <v>1559538</v>
+      </c>
+      <c r="H12" s="1" t="n">
+        <v>985893</v>
+      </c>
+      <c r="I12" s="1" t="n">
+        <v>841196</v>
       </c>
       <c r="J12" s="1" t="n">
-        <v>1782333</v>
+        <v>17659686</v>
       </c>
       <c r="K12" s="1" t="n">
-        <v>1930914</v>
+        <v>21814888</v>
       </c>
       <c r="L12" s="1" t="n">
-        <v>1377997</v>
+        <v>9384383</v>
       </c>
       <c r="M12" s="1" t="n">
-        <v>1782333</v>
+        <v>8829843</v>
       </c>
       <c r="N12" s="1" t="n">
-        <v>1930914</v>
+        <v>10907444</v>
       </c>
       <c r="O12" s="1" t="n">
-        <v>1377997</v>
+        <v>4692191.5</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>기타비용</t>
+          <t>금융비용</t>
         </is>
       </c>
       <c r="B13" s="1" t="n"/>
       <c r="C13" s="1" t="n"/>
       <c r="D13" s="1" t="n">
-        <v>2350343</v>
+        <v>12645530</v>
       </c>
       <c r="E13" s="1" t="n">
-        <v>2238256</v>
+        <v>19027689</v>
       </c>
       <c r="F13" s="1" t="n">
-        <v>1745985</v>
-      </c>
-      <c r="G13" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H13" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I13" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>7704554</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <v>970700</v>
+      </c>
+      <c r="H13" s="1" t="n">
+        <v>879638</v>
+      </c>
+      <c r="I13" s="1" t="n">
+        <v>512836</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>2350343</v>
+        <v>13616230</v>
       </c>
       <c r="K13" s="1" t="n">
-        <v>2238256</v>
+        <v>19907327</v>
       </c>
       <c r="L13" s="1" t="n">
-        <v>1745985</v>
+        <v>8217390</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>2350343</v>
+        <v>6808115</v>
       </c>
       <c r="N13" s="1" t="n">
-        <v>2238256</v>
+        <v>9953663.5</v>
       </c>
       <c r="O13" s="1" t="n">
-        <v>1745985</v>
+        <v>4108695</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>법인세비용차감전순이익</t>
+          <t>법인세비용차감전순이익(손실)</t>
         </is>
       </c>
       <c r="B14" s="1" t="n"/>
       <c r="C14" s="1" t="n"/>
       <c r="D14" s="1" t="n">
-        <v>17618662</v>
+        <v>11006265</v>
       </c>
       <c r="E14" s="1" t="n">
-        <v>11181471</v>
+        <v>46440474</v>
       </c>
       <c r="F14" s="1" t="n">
-        <v>7789043</v>
+        <v>53351827</v>
       </c>
       <c r="G14" s="7" t="inlineStr">
         <is>
@@ -1115,22 +1115,22 @@
         </is>
       </c>
       <c r="J14" s="1" t="n">
-        <v>17618662</v>
+        <v>11006265</v>
       </c>
       <c r="K14" s="1" t="n">
-        <v>11181471</v>
+        <v>46440474</v>
       </c>
       <c r="L14" s="1" t="n">
-        <v>7789043</v>
+        <v>53351827</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>17618662</v>
+        <v>11006265</v>
       </c>
       <c r="N14" s="1" t="n">
-        <v>11181471</v>
+        <v>46440474</v>
       </c>
       <c r="O14" s="1" t="n">
-        <v>7789043</v>
+        <v>53351827</v>
       </c>
     </row>
     <row r="15">
@@ -1142,22 +1142,22 @@
       <c r="B15" s="1" t="n"/>
       <c r="C15" s="1" t="n"/>
       <c r="D15" s="1" t="n">
+        <v>-4480835</v>
+      </c>
+      <c r="E15" s="1" t="n">
+        <v>-9213603</v>
+      </c>
+      <c r="F15" s="1" t="n">
+        <v>13444377</v>
+      </c>
+      <c r="G15" s="1" t="n">
         <v>4626640</v>
       </c>
-      <c r="E15" s="1" t="n">
+      <c r="H15" s="1" t="n">
         <v>2979168</v>
       </c>
-      <c r="F15" s="1" t="n">
+      <c r="I15" s="1" t="n">
         <v>2266823</v>
-      </c>
-      <c r="G15" s="1" t="n">
-        <v>-4480835</v>
-      </c>
-      <c r="H15" s="1" t="n">
-        <v>-9213603</v>
-      </c>
-      <c r="I15" s="1" t="n">
-        <v>13444377</v>
       </c>
       <c r="J15" s="1" t="n">
         <v>145805</v>
@@ -1181,19 +1181,19 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>계속영업연결당기순이익</t>
+          <t>계속영업이익(손실)</t>
         </is>
       </c>
       <c r="B16" s="1" t="n"/>
       <c r="C16" s="1" t="n"/>
       <c r="D16" s="1" t="n">
-        <v>12992022</v>
+        <v>15487100</v>
       </c>
       <c r="E16" s="1" t="n">
-        <v>8202303</v>
+        <v>55654077</v>
       </c>
       <c r="F16" s="1" t="n">
-        <v>5522220</v>
+        <v>39907450</v>
       </c>
       <c r="G16" s="7" t="inlineStr">
         <is>
@@ -1211,40 +1211,40 @@
         </is>
       </c>
       <c r="J16" s="1" t="n">
-        <v>12992022</v>
+        <v>15487100</v>
       </c>
       <c r="K16" s="1" t="n">
-        <v>8202303</v>
+        <v>55654077</v>
       </c>
       <c r="L16" s="1" t="n">
-        <v>5522220</v>
+        <v>39907450</v>
       </c>
       <c r="M16" s="1" t="n">
-        <v>12992022</v>
+        <v>15487100</v>
       </c>
       <c r="N16" s="1" t="n">
-        <v>8202303</v>
+        <v>55654077</v>
       </c>
       <c r="O16" s="1" t="n">
-        <v>5522220</v>
+        <v>39907450</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>중단영업당기순이익(손실)</t>
+          <t>당기순이익(손실)</t>
         </is>
       </c>
       <c r="B17" s="1" t="n"/>
       <c r="C17" s="1" t="n"/>
       <c r="D17" s="1" t="n">
-        <v>-719721</v>
+        <v>15487100</v>
       </c>
       <c r="E17" s="1" t="n">
-        <v>-218689</v>
+        <v>55654077</v>
       </c>
       <c r="F17" s="1" t="n">
-        <v>170857</v>
+        <v>39907450</v>
       </c>
       <c r="G17" s="7" t="inlineStr">
         <is>
@@ -1262,40 +1262,46 @@
         </is>
       </c>
       <c r="J17" s="1" t="n">
-        <v>-719721</v>
+        <v>15487100</v>
       </c>
       <c r="K17" s="1" t="n">
-        <v>-218689</v>
+        <v>55654077</v>
       </c>
       <c r="L17" s="1" t="n">
-        <v>170857</v>
+        <v>39907450</v>
       </c>
       <c r="M17" s="1" t="n">
-        <v>-719721</v>
+        <v>15487100</v>
       </c>
       <c r="N17" s="1" t="n">
-        <v>-218689</v>
+        <v>55654077</v>
       </c>
       <c r="O17" s="1" t="n">
-        <v>170857</v>
+        <v>39907450</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>연결당기순이익</t>
+          <t>당기순이익(손실)의 귀속</t>
         </is>
       </c>
       <c r="B18" s="1" t="n"/>
       <c r="C18" s="1" t="n"/>
-      <c r="D18" s="1" t="n">
-        <v>12272301</v>
-      </c>
-      <c r="E18" s="1" t="n">
-        <v>7983614</v>
-      </c>
-      <c r="F18" s="1" t="n">
-        <v>5693077</v>
+      <c r="D18" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E18" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F18" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="G18" s="7" t="inlineStr">
         <is>
@@ -1312,23 +1318,35 @@
           <t>-</t>
         </is>
       </c>
-      <c r="J18" s="1" t="n">
-        <v>12272301</v>
-      </c>
-      <c r="K18" s="1" t="n">
-        <v>7983614</v>
-      </c>
-      <c r="L18" s="1" t="n">
-        <v>5693077</v>
-      </c>
-      <c r="M18" s="1" t="n">
-        <v>12272301</v>
-      </c>
-      <c r="N18" s="1" t="n">
-        <v>7983614</v>
-      </c>
-      <c r="O18" s="1" t="n">
-        <v>5693077</v>
+      <c r="J18" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K18" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L18" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M18" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N18" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O18" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
     </row>
     <row r="19">
@@ -1337,22 +1355,20 @@
           <t>당기순이익(손실)의 귀속</t>
         </is>
       </c>
-      <c r="B19" s="1" t="n"/>
+      <c r="B19" s="1" t="inlineStr">
+        <is>
+          <t>지배기업의 소유주에게 귀속되는 당기순이익(손실)</t>
+        </is>
+      </c>
       <c r="C19" s="1" t="n"/>
-      <c r="D19" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E19" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F19" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D19" s="1" t="n">
+        <v>14473401</v>
+      </c>
+      <c r="E19" s="1" t="n">
+        <v>54730018</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <v>39243791</v>
       </c>
       <c r="G19" s="7" t="inlineStr">
         <is>
@@ -1369,35 +1385,23 @@
           <t>-</t>
         </is>
       </c>
-      <c r="J19" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K19" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L19" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M19" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N19" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O19" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="J19" s="1" t="n">
+        <v>14473401</v>
+      </c>
+      <c r="K19" s="1" t="n">
+        <v>54730018</v>
+      </c>
+      <c r="L19" s="1" t="n">
+        <v>39243791</v>
+      </c>
+      <c r="M19" s="1" t="n">
+        <v>14473401</v>
+      </c>
+      <c r="N19" s="1" t="n">
+        <v>54730018</v>
+      </c>
+      <c r="O19" s="1" t="n">
+        <v>39243791</v>
       </c>
     </row>
     <row r="20">
@@ -1408,18 +1412,18 @@
       </c>
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>지배기업소유주지분</t>
+          <t>비지배지분에 귀속되는 당기순이익(손실)</t>
         </is>
       </c>
       <c r="C20" s="1" t="n"/>
       <c r="D20" s="1" t="n">
-        <v>11961717</v>
+        <v>1013699</v>
       </c>
       <c r="E20" s="1" t="n">
-        <v>7364364</v>
+        <v>924059</v>
       </c>
       <c r="F20" s="1" t="n">
-        <v>4942356</v>
+        <v>663659</v>
       </c>
       <c r="G20" s="7" t="inlineStr">
         <is>
@@ -1437,22 +1441,22 @@
         </is>
       </c>
       <c r="J20" s="1" t="n">
-        <v>11961717</v>
+        <v>1013699</v>
       </c>
       <c r="K20" s="1" t="n">
-        <v>7364364</v>
+        <v>924059</v>
       </c>
       <c r="L20" s="1" t="n">
-        <v>4942356</v>
+        <v>663659</v>
       </c>
       <c r="M20" s="1" t="n">
-        <v>11961717</v>
+        <v>1013699</v>
       </c>
       <c r="N20" s="1" t="n">
-        <v>7364364</v>
+        <v>924059</v>
       </c>
       <c r="O20" s="1" t="n">
-        <v>4942356</v>
+        <v>663659</v>
       </c>
     </row>
     <row r="21">
@@ -1463,51 +1467,51 @@
       </c>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>비지배지분</t>
+          <t>지배기업소유주지분</t>
         </is>
       </c>
       <c r="C21" s="1" t="n"/>
-      <c r="D21" s="1" t="n">
-        <v>310584</v>
-      </c>
-      <c r="E21" s="1" t="n">
-        <v>619250</v>
-      </c>
-      <c r="F21" s="1" t="n">
-        <v>750721</v>
-      </c>
-      <c r="G21" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H21" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I21" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D21" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E21" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F21" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G21" s="1" t="n">
+        <v>11961717</v>
+      </c>
+      <c r="H21" s="1" t="n">
+        <v>7364364</v>
+      </c>
+      <c r="I21" s="1" t="n">
+        <v>4942356</v>
       </c>
       <c r="J21" s="1" t="n">
-        <v>310584</v>
+        <v>11961717</v>
       </c>
       <c r="K21" s="1" t="n">
-        <v>619250</v>
+        <v>7364364</v>
       </c>
       <c r="L21" s="1" t="n">
-        <v>750721</v>
+        <v>4942356</v>
       </c>
       <c r="M21" s="1" t="n">
-        <v>310584</v>
+        <v>11961717</v>
       </c>
       <c r="N21" s="1" t="n">
-        <v>619250</v>
+        <v>7364364</v>
       </c>
       <c r="O21" s="1" t="n">
-        <v>750721</v>
+        <v>4942356</v>
       </c>
     </row>
     <row r="22">
@@ -1518,7 +1522,7 @@
       </c>
       <c r="B22" s="1" t="inlineStr">
         <is>
-          <t>지배기업의 소유주에게 귀속되는 당기순이익(손실)</t>
+          <t>비지배지분</t>
         </is>
       </c>
       <c r="C22" s="1" t="n"/>
@@ -1538,44 +1542,40 @@
         </is>
       </c>
       <c r="G22" s="1" t="n">
-        <v>14473401</v>
+        <v>310584</v>
       </c>
       <c r="H22" s="1" t="n">
-        <v>54730018</v>
+        <v>619250</v>
       </c>
       <c r="I22" s="1" t="n">
-        <v>39243791</v>
+        <v>750721</v>
       </c>
       <c r="J22" s="1" t="n">
-        <v>14473401</v>
+        <v>310584</v>
       </c>
       <c r="K22" s="1" t="n">
-        <v>54730018</v>
+        <v>619250</v>
       </c>
       <c r="L22" s="1" t="n">
-        <v>39243791</v>
+        <v>750721</v>
       </c>
       <c r="M22" s="1" t="n">
-        <v>14473401</v>
+        <v>310584</v>
       </c>
       <c r="N22" s="1" t="n">
-        <v>54730018</v>
+        <v>619250</v>
       </c>
       <c r="O22" s="1" t="n">
-        <v>39243791</v>
+        <v>750721</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>당기순이익(손실)의 귀속</t>
-        </is>
-      </c>
-      <c r="B23" s="1" t="inlineStr">
-        <is>
-          <t>비지배지분에 귀속되는 당기순이익(손실)</t>
-        </is>
-      </c>
+          <t>주당이익</t>
+        </is>
+      </c>
+      <c r="B23" s="1" t="n"/>
       <c r="C23" s="1" t="n"/>
       <c r="D23" s="7" t="inlineStr">
         <is>
@@ -1592,32 +1592,50 @@
           <t>-</t>
         </is>
       </c>
-      <c r="G23" s="1" t="n">
-        <v>1013699</v>
-      </c>
-      <c r="H23" s="1" t="n">
-        <v>924059</v>
-      </c>
-      <c r="I23" s="1" t="n">
-        <v>663659</v>
-      </c>
-      <c r="J23" s="1" t="n">
-        <v>1013699</v>
-      </c>
-      <c r="K23" s="1" t="n">
-        <v>924059</v>
-      </c>
-      <c r="L23" s="1" t="n">
-        <v>663659</v>
-      </c>
-      <c r="M23" s="1" t="n">
-        <v>1013699</v>
-      </c>
-      <c r="N23" s="1" t="n">
-        <v>924059</v>
-      </c>
-      <c r="O23" s="1" t="n">
-        <v>663659</v>
+      <c r="G23" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H23" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I23" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J23" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K23" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L23" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M23" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N23" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O23" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
     </row>
     <row r="24">
@@ -1626,22 +1644,20 @@
           <t>주당이익</t>
         </is>
       </c>
-      <c r="B24" s="1" t="n"/>
+      <c r="B24" s="1" t="inlineStr">
+        <is>
+          <t>기본주당이익(손실) (단위 : 원)</t>
+        </is>
+      </c>
       <c r="C24" s="1" t="n"/>
-      <c r="D24" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E24" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F24" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D24" s="1" t="n">
+        <v>2131</v>
+      </c>
+      <c r="E24" s="1" t="n">
+        <v>8057</v>
+      </c>
+      <c r="F24" s="1" t="n">
+        <v>5777</v>
       </c>
       <c r="G24" s="7" t="inlineStr">
         <is>
@@ -1658,35 +1674,23 @@
           <t>-</t>
         </is>
       </c>
-      <c r="J24" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K24" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L24" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M24" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N24" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O24" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="J24" s="1" t="n">
+        <v>2131</v>
+      </c>
+      <c r="K24" s="1" t="n">
+        <v>8057</v>
+      </c>
+      <c r="L24" s="1" t="n">
+        <v>5777</v>
+      </c>
+      <c r="M24" s="1" t="n">
+        <v>2131</v>
+      </c>
+      <c r="N24" s="1" t="n">
+        <v>8057</v>
+      </c>
+      <c r="O24" s="1" t="n">
+        <v>5777</v>
       </c>
     </row>
     <row r="25">
@@ -1697,24 +1701,18 @@
       </c>
       <c r="B25" s="1" t="inlineStr">
         <is>
-          <t>기본주당이익 (단위 :원)</t>
+          <t>희석주당이익(손실) (단위 : 원)</t>
         </is>
       </c>
       <c r="C25" s="1" t="n"/>
-      <c r="D25" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E25" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F25" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D25" s="1" t="n">
+        <v>2131</v>
+      </c>
+      <c r="E25" s="1" t="n">
+        <v>8057</v>
+      </c>
+      <c r="F25" s="1" t="n">
+        <v>5777</v>
       </c>
       <c r="G25" s="7" t="inlineStr">
         <is>
@@ -1731,35 +1729,23 @@
           <t>-</t>
         </is>
       </c>
-      <c r="J25" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K25" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L25" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M25" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N25" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O25" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="J25" s="1" t="n">
+        <v>2131</v>
+      </c>
+      <c r="K25" s="1" t="n">
+        <v>8057</v>
+      </c>
+      <c r="L25" s="1" t="n">
+        <v>5777</v>
+      </c>
+      <c r="M25" s="1" t="n">
+        <v>2131</v>
+      </c>
+      <c r="N25" s="1" t="n">
+        <v>8057</v>
+      </c>
+      <c r="O25" s="1" t="n">
+        <v>5777</v>
       </c>
     </row>
     <row r="26">
@@ -1773,19 +1759,21 @@
           <t>기본주당이익 (단위 :원)</t>
         </is>
       </c>
-      <c r="C26" s="1" t="inlineStr">
-        <is>
-          <t>보통주기본주당이익(손실) (단위 : 원)</t>
-        </is>
-      </c>
-      <c r="D26" s="1" t="n">
-        <v>45703</v>
-      </c>
-      <c r="E26" s="1" t="n">
-        <v>28521</v>
-      </c>
-      <c r="F26" s="1" t="n">
-        <v>18979</v>
+      <c r="C26" s="1" t="n"/>
+      <c r="D26" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E26" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F26" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="G26" s="7" t="inlineStr">
         <is>
@@ -1802,23 +1790,35 @@
           <t>-</t>
         </is>
       </c>
-      <c r="J26" s="1" t="n">
-        <v>45703</v>
-      </c>
-      <c r="K26" s="1" t="n">
-        <v>28521</v>
-      </c>
-      <c r="L26" s="1" t="n">
-        <v>18979</v>
-      </c>
-      <c r="M26" s="1" t="n">
-        <v>45703</v>
-      </c>
-      <c r="N26" s="1" t="n">
-        <v>28521</v>
-      </c>
-      <c r="O26" s="1" t="n">
-        <v>18979</v>
+      <c r="J26" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K26" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L26" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M26" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N26" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O26" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
     </row>
     <row r="27">
@@ -1834,50 +1834,50 @@
       </c>
       <c r="C27" s="1" t="inlineStr">
         <is>
-          <t>계속영업 보통주기본주당이익(손실) (단위: 원)</t>
-        </is>
-      </c>
-      <c r="D27" s="1" t="n">
-        <v>47622</v>
-      </c>
-      <c r="E27" s="1" t="n">
-        <v>29105</v>
-      </c>
-      <c r="F27" s="1" t="n">
-        <v>18521</v>
-      </c>
-      <c r="G27" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H27" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I27" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>보통주기본주당이익(손실) (단위 : 원)</t>
+        </is>
+      </c>
+      <c r="D27" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E27" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F27" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G27" s="1" t="n">
+        <v>45703</v>
+      </c>
+      <c r="H27" s="1" t="n">
+        <v>28521</v>
+      </c>
+      <c r="I27" s="1" t="n">
+        <v>18979</v>
       </c>
       <c r="J27" s="1" t="n">
-        <v>47622</v>
+        <v>45703</v>
       </c>
       <c r="K27" s="1" t="n">
-        <v>29105</v>
+        <v>28521</v>
       </c>
       <c r="L27" s="1" t="n">
-        <v>18521</v>
+        <v>18979</v>
       </c>
       <c r="M27" s="1" t="n">
-        <v>47622</v>
+        <v>45703</v>
       </c>
       <c r="N27" s="1" t="n">
-        <v>29105</v>
+        <v>28521</v>
       </c>
       <c r="O27" s="1" t="n">
-        <v>18521</v>
+        <v>18979</v>
       </c>
     </row>
     <row r="28">
@@ -1893,50 +1893,50 @@
       </c>
       <c r="C28" s="1" t="inlineStr">
         <is>
-          <t>중단영업 보통주기본주당이익(손실) (단위: 원)</t>
-        </is>
-      </c>
-      <c r="D28" s="1" t="n">
-        <v>-1919</v>
-      </c>
-      <c r="E28" s="1" t="n">
-        <v>-584</v>
-      </c>
-      <c r="F28" s="1" t="n">
-        <v>458</v>
-      </c>
-      <c r="G28" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H28" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I28" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>계속영업 보통주기본주당이익(손실) (단위: 원)</t>
+        </is>
+      </c>
+      <c r="D28" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E28" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F28" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G28" s="1" t="n">
+        <v>47622</v>
+      </c>
+      <c r="H28" s="1" t="n">
+        <v>29105</v>
+      </c>
+      <c r="I28" s="1" t="n">
+        <v>18521</v>
       </c>
       <c r="J28" s="1" t="n">
-        <v>-1919</v>
+        <v>47622</v>
       </c>
       <c r="K28" s="1" t="n">
-        <v>-584</v>
+        <v>29105</v>
       </c>
       <c r="L28" s="1" t="n">
-        <v>458</v>
+        <v>18521</v>
       </c>
       <c r="M28" s="1" t="n">
-        <v>-1919</v>
+        <v>47622</v>
       </c>
       <c r="N28" s="1" t="n">
-        <v>-584</v>
+        <v>29105</v>
       </c>
       <c r="O28" s="1" t="n">
-        <v>458</v>
+        <v>18521</v>
       </c>
     </row>
     <row r="29">
@@ -1952,50 +1952,50 @@
       </c>
       <c r="C29" s="1" t="inlineStr">
         <is>
-          <t>1우선주 기본주당이익(손실) (단위 : 원)</t>
-        </is>
-      </c>
-      <c r="D29" s="1" t="n">
-        <v>45535</v>
-      </c>
-      <c r="E29" s="1" t="n">
-        <v>28207</v>
-      </c>
-      <c r="F29" s="1" t="n">
-        <v>19002</v>
-      </c>
-      <c r="G29" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H29" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I29" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>중단영업 보통주기본주당이익(손실) (단위: 원)</t>
+        </is>
+      </c>
+      <c r="D29" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E29" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F29" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G29" s="1" t="n">
+        <v>-1919</v>
+      </c>
+      <c r="H29" s="1" t="n">
+        <v>-584</v>
+      </c>
+      <c r="I29" s="1" t="n">
+        <v>458</v>
       </c>
       <c r="J29" s="1" t="n">
-        <v>45535</v>
+        <v>-1919</v>
       </c>
       <c r="K29" s="1" t="n">
-        <v>28207</v>
+        <v>-584</v>
       </c>
       <c r="L29" s="1" t="n">
-        <v>19002</v>
+        <v>458</v>
       </c>
       <c r="M29" s="1" t="n">
-        <v>45535</v>
+        <v>-1919</v>
       </c>
       <c r="N29" s="1" t="n">
-        <v>28207</v>
+        <v>-584</v>
       </c>
       <c r="O29" s="1" t="n">
-        <v>19002</v>
+        <v>458</v>
       </c>
     </row>
     <row r="30">
@@ -2011,50 +2011,50 @@
       </c>
       <c r="C30" s="1" t="inlineStr">
         <is>
-          <t>계속영업 1우선주기본주당이익(손실) (단위 : 원)</t>
-        </is>
-      </c>
-      <c r="D30" s="1" t="n">
-        <v>47445</v>
-      </c>
-      <c r="E30" s="1" t="n">
-        <v>28783</v>
-      </c>
-      <c r="F30" s="1" t="n">
-        <v>18545</v>
-      </c>
-      <c r="G30" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H30" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I30" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>1우선주 기본주당이익(손실) (단위 : 원)</t>
+        </is>
+      </c>
+      <c r="D30" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E30" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F30" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G30" s="1" t="n">
+        <v>45535</v>
+      </c>
+      <c r="H30" s="1" t="n">
+        <v>28207</v>
+      </c>
+      <c r="I30" s="1" t="n">
+        <v>19002</v>
       </c>
       <c r="J30" s="1" t="n">
-        <v>47445</v>
+        <v>45535</v>
       </c>
       <c r="K30" s="1" t="n">
-        <v>28783</v>
+        <v>28207</v>
       </c>
       <c r="L30" s="1" t="n">
-        <v>18545</v>
+        <v>19002</v>
       </c>
       <c r="M30" s="1" t="n">
-        <v>47445</v>
+        <v>45535</v>
       </c>
       <c r="N30" s="1" t="n">
-        <v>28783</v>
+        <v>28207</v>
       </c>
       <c r="O30" s="1" t="n">
-        <v>18545</v>
+        <v>19002</v>
       </c>
     </row>
     <row r="31">
@@ -2070,50 +2070,50 @@
       </c>
       <c r="C31" s="1" t="inlineStr">
         <is>
-          <t>중단영업 1우선주기본주당이익(손실) (단위 : 원)</t>
-        </is>
-      </c>
-      <c r="D31" s="1" t="n">
-        <v>-1910</v>
-      </c>
-      <c r="E31" s="1" t="n">
-        <v>-576</v>
-      </c>
-      <c r="F31" s="1" t="n">
-        <v>457</v>
-      </c>
-      <c r="G31" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H31" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I31" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>계속영업 1우선주기본주당이익(손실) (단위 : 원)</t>
+        </is>
+      </c>
+      <c r="D31" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E31" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F31" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G31" s="1" t="n">
+        <v>47445</v>
+      </c>
+      <c r="H31" s="1" t="n">
+        <v>28783</v>
+      </c>
+      <c r="I31" s="1" t="n">
+        <v>18545</v>
       </c>
       <c r="J31" s="1" t="n">
-        <v>-1910</v>
+        <v>47445</v>
       </c>
       <c r="K31" s="1" t="n">
-        <v>-576</v>
+        <v>28783</v>
       </c>
       <c r="L31" s="1" t="n">
-        <v>457</v>
+        <v>18545</v>
       </c>
       <c r="M31" s="1" t="n">
-        <v>-1910</v>
+        <v>47445</v>
       </c>
       <c r="N31" s="1" t="n">
-        <v>-576</v>
+        <v>28783</v>
       </c>
       <c r="O31" s="1" t="n">
-        <v>457</v>
+        <v>18545</v>
       </c>
     </row>
     <row r="32">
@@ -2124,10 +2124,14 @@
       </c>
       <c r="B32" s="1" t="inlineStr">
         <is>
-          <t>희석주당이익(손실)(단위 : 원)</t>
-        </is>
-      </c>
-      <c r="C32" s="1" t="n"/>
+          <t>기본주당이익 (단위 :원)</t>
+        </is>
+      </c>
+      <c r="C32" s="1" t="inlineStr">
+        <is>
+          <t>중단영업 1우선주기본주당이익(손실) (단위 : 원)</t>
+        </is>
+      </c>
       <c r="D32" s="7" t="inlineStr">
         <is>
           <t>-</t>
@@ -2143,50 +2147,32 @@
           <t>-</t>
         </is>
       </c>
-      <c r="G32" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H32" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I32" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J32" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K32" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L32" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M32" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N32" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O32" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="G32" s="1" t="n">
+        <v>-1910</v>
+      </c>
+      <c r="H32" s="1" t="n">
+        <v>-576</v>
+      </c>
+      <c r="I32" s="1" t="n">
+        <v>457</v>
+      </c>
+      <c r="J32" s="1" t="n">
+        <v>-1910</v>
+      </c>
+      <c r="K32" s="1" t="n">
+        <v>-576</v>
+      </c>
+      <c r="L32" s="1" t="n">
+        <v>457</v>
+      </c>
+      <c r="M32" s="1" t="n">
+        <v>-1910</v>
+      </c>
+      <c r="N32" s="1" t="n">
+        <v>-576</v>
+      </c>
+      <c r="O32" s="1" t="n">
+        <v>457</v>
       </c>
     </row>
     <row r="33">
@@ -2200,19 +2186,21 @@
           <t>희석주당이익(손실)(단위 : 원)</t>
         </is>
       </c>
-      <c r="C33" s="1" t="inlineStr">
-        <is>
-          <t>보통주 희석주당이익 (단위 : 원)</t>
-        </is>
-      </c>
-      <c r="D33" s="1" t="n">
-        <v>45703</v>
-      </c>
-      <c r="E33" s="1" t="n">
-        <v>28521</v>
-      </c>
-      <c r="F33" s="1" t="n">
-        <v>18979</v>
+      <c r="C33" s="1" t="n"/>
+      <c r="D33" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E33" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F33" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="G33" s="7" t="inlineStr">
         <is>
@@ -2229,23 +2217,35 @@
           <t>-</t>
         </is>
       </c>
-      <c r="J33" s="1" t="n">
-        <v>45703</v>
-      </c>
-      <c r="K33" s="1" t="n">
-        <v>28521</v>
-      </c>
-      <c r="L33" s="1" t="n">
-        <v>18979</v>
-      </c>
-      <c r="M33" s="1" t="n">
-        <v>45703</v>
-      </c>
-      <c r="N33" s="1" t="n">
-        <v>28521</v>
-      </c>
-      <c r="O33" s="1" t="n">
-        <v>18979</v>
+      <c r="J33" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K33" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L33" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M33" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N33" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O33" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
     </row>
     <row r="34">
@@ -2261,50 +2261,50 @@
       </c>
       <c r="C34" s="1" t="inlineStr">
         <is>
-          <t>1우선주 희석주당이익 (단위 : 원)</t>
-        </is>
-      </c>
-      <c r="D34" s="1" t="n">
-        <v>45535</v>
-      </c>
-      <c r="E34" s="1" t="n">
-        <v>28207</v>
-      </c>
-      <c r="F34" s="1" t="n">
-        <v>19002</v>
-      </c>
-      <c r="G34" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H34" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I34" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>보통주 희석주당이익 (단위 : 원)</t>
+        </is>
+      </c>
+      <c r="D34" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E34" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F34" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G34" s="1" t="n">
+        <v>45703</v>
+      </c>
+      <c r="H34" s="1" t="n">
+        <v>28521</v>
+      </c>
+      <c r="I34" s="1" t="n">
+        <v>18979</v>
       </c>
       <c r="J34" s="1" t="n">
-        <v>45535</v>
+        <v>45703</v>
       </c>
       <c r="K34" s="1" t="n">
-        <v>28207</v>
+        <v>28521</v>
       </c>
       <c r="L34" s="1" t="n">
-        <v>19002</v>
+        <v>18979</v>
       </c>
       <c r="M34" s="1" t="n">
-        <v>45535</v>
+        <v>45703</v>
       </c>
       <c r="N34" s="1" t="n">
-        <v>28207</v>
+        <v>28521</v>
       </c>
       <c r="O34" s="1" t="n">
-        <v>19002</v>
+        <v>18979</v>
       </c>
     </row>
     <row r="35">
@@ -2315,10 +2315,14 @@
       </c>
       <c r="B35" s="1" t="inlineStr">
         <is>
-          <t>기본주당이익(손실) (단위 : 원)</t>
-        </is>
-      </c>
-      <c r="C35" s="1" t="n"/>
+          <t>희석주당이익(손실)(단위 : 원)</t>
+        </is>
+      </c>
+      <c r="C35" s="1" t="inlineStr">
+        <is>
+          <t>1우선주 희석주당이익 (단위 : 원)</t>
+        </is>
+      </c>
       <c r="D35" s="7" t="inlineStr">
         <is>
           <t>-</t>
@@ -2335,44 +2339,40 @@
         </is>
       </c>
       <c r="G35" s="1" t="n">
-        <v>2131</v>
+        <v>45535</v>
       </c>
       <c r="H35" s="1" t="n">
-        <v>8057</v>
+        <v>28207</v>
       </c>
       <c r="I35" s="1" t="n">
-        <v>5777</v>
+        <v>19002</v>
       </c>
       <c r="J35" s="1" t="n">
-        <v>2131</v>
+        <v>45535</v>
       </c>
       <c r="K35" s="1" t="n">
-        <v>8057</v>
+        <v>28207</v>
       </c>
       <c r="L35" s="1" t="n">
-        <v>5777</v>
+        <v>19002</v>
       </c>
       <c r="M35" s="1" t="n">
-        <v>2131</v>
+        <v>45535</v>
       </c>
       <c r="N35" s="1" t="n">
-        <v>8057</v>
+        <v>28207</v>
       </c>
       <c r="O35" s="1" t="n">
-        <v>5777</v>
+        <v>19002</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>주당이익</t>
-        </is>
-      </c>
-      <c r="B36" s="1" t="inlineStr">
-        <is>
-          <t>희석주당이익(손실) (단위 : 원)</t>
-        </is>
-      </c>
+          <t>매출액</t>
+        </is>
+      </c>
+      <c r="B36" s="1" t="n"/>
       <c r="C36" s="1" t="n"/>
       <c r="D36" s="7" t="inlineStr">
         <is>
@@ -2390,37 +2390,37 @@
         </is>
       </c>
       <c r="G36" s="1" t="n">
-        <v>2131</v>
+        <v>162663579</v>
       </c>
       <c r="H36" s="1" t="n">
-        <v>8057</v>
+        <v>142151469</v>
       </c>
       <c r="I36" s="1" t="n">
-        <v>5777</v>
+        <v>116448159</v>
       </c>
       <c r="J36" s="1" t="n">
-        <v>2131</v>
+        <v>162663579</v>
       </c>
       <c r="K36" s="1" t="n">
-        <v>8057</v>
+        <v>142151469</v>
       </c>
       <c r="L36" s="1" t="n">
-        <v>5777</v>
+        <v>116448159</v>
       </c>
       <c r="M36" s="1" t="n">
-        <v>2131</v>
+        <v>162663579</v>
       </c>
       <c r="N36" s="1" t="n">
-        <v>8057</v>
+        <v>142151469</v>
       </c>
       <c r="O36" s="1" t="n">
-        <v>5777</v>
+        <v>116448159</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>영업수익</t>
+          <t>공동기업및관계기업투자손익</t>
         </is>
       </c>
       <c r="B37" s="1" t="n"/>
@@ -2441,37 +2441,37 @@
         </is>
       </c>
       <c r="G37" s="1" t="n">
-        <v>258935494</v>
+        <v>2470933</v>
       </c>
       <c r="H37" s="1" t="n">
-        <v>302231360</v>
+        <v>1557630</v>
       </c>
       <c r="I37" s="1" t="n">
-        <v>279604799</v>
+        <v>1302150</v>
       </c>
       <c r="J37" s="1" t="n">
-        <v>258935494</v>
+        <v>2470933</v>
       </c>
       <c r="K37" s="1" t="n">
-        <v>302231360</v>
+        <v>1557630</v>
       </c>
       <c r="L37" s="1" t="n">
-        <v>279604799</v>
+        <v>1302150</v>
       </c>
       <c r="M37" s="1" t="n">
-        <v>258935494</v>
+        <v>2470933</v>
       </c>
       <c r="N37" s="1" t="n">
-        <v>302231360</v>
+        <v>1557630</v>
       </c>
       <c r="O37" s="1" t="n">
-        <v>279604799</v>
+        <v>1302150</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>기타이익</t>
+          <t>기타수익</t>
         </is>
       </c>
       <c r="B38" s="1" t="n"/>
@@ -2492,37 +2492,37 @@
         </is>
       </c>
       <c r="G38" s="1" t="n">
-        <v>1180448</v>
+        <v>1782333</v>
       </c>
       <c r="H38" s="1" t="n">
-        <v>1962071</v>
+        <v>1930914</v>
       </c>
       <c r="I38" s="1" t="n">
-        <v>2205695</v>
+        <v>1377997</v>
       </c>
       <c r="J38" s="1" t="n">
-        <v>1180448</v>
+        <v>1782333</v>
       </c>
       <c r="K38" s="1" t="n">
-        <v>1962071</v>
+        <v>1930914</v>
       </c>
       <c r="L38" s="1" t="n">
-        <v>2205695</v>
+        <v>1377997</v>
       </c>
       <c r="M38" s="1" t="n">
-        <v>1180448</v>
+        <v>1782333</v>
       </c>
       <c r="N38" s="1" t="n">
-        <v>1962071</v>
+        <v>1930914</v>
       </c>
       <c r="O38" s="1" t="n">
-        <v>2205695</v>
+        <v>1377997</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>기타손실</t>
+          <t>기타비용</t>
         </is>
       </c>
       <c r="B39" s="1" t="n"/>
@@ -2543,37 +2543,37 @@
         </is>
       </c>
       <c r="G39" s="1" t="n">
-        <v>1083327</v>
+        <v>2350343</v>
       </c>
       <c r="H39" s="1" t="n">
-        <v>1790176</v>
+        <v>2238256</v>
       </c>
       <c r="I39" s="1" t="n">
-        <v>2055971</v>
+        <v>1745985</v>
       </c>
       <c r="J39" s="1" t="n">
-        <v>1083327</v>
+        <v>2350343</v>
       </c>
       <c r="K39" s="1" t="n">
-        <v>1790176</v>
+        <v>2238256</v>
       </c>
       <c r="L39" s="1" t="n">
-        <v>2055971</v>
+        <v>1745985</v>
       </c>
       <c r="M39" s="1" t="n">
-        <v>1083327</v>
+        <v>2350343</v>
       </c>
       <c r="N39" s="1" t="n">
-        <v>1790176</v>
+        <v>2238256</v>
       </c>
       <c r="O39" s="1" t="n">
-        <v>2055971</v>
+        <v>1745985</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>지분법이익</t>
+          <t>법인세비용차감전순이익</t>
         </is>
       </c>
       <c r="B40" s="1" t="n"/>
@@ -2594,37 +2594,37 @@
         </is>
       </c>
       <c r="G40" s="1" t="n">
-        <v>887550</v>
+        <v>17618662</v>
       </c>
       <c r="H40" s="1" t="n">
-        <v>1090643</v>
+        <v>11181471</v>
       </c>
       <c r="I40" s="1" t="n">
-        <v>729614</v>
+        <v>7789043</v>
       </c>
       <c r="J40" s="1" t="n">
-        <v>887550</v>
+        <v>17618662</v>
       </c>
       <c r="K40" s="1" t="n">
-        <v>1090643</v>
+        <v>11181471</v>
       </c>
       <c r="L40" s="1" t="n">
-        <v>729614</v>
+        <v>7789043</v>
       </c>
       <c r="M40" s="1" t="n">
-        <v>887550</v>
+        <v>17618662</v>
       </c>
       <c r="N40" s="1" t="n">
-        <v>1090643</v>
+        <v>11181471</v>
       </c>
       <c r="O40" s="1" t="n">
-        <v>729614</v>
+        <v>7789043</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>법인세비용차감전순이익(손실)</t>
+          <t>계속영업연결당기순이익</t>
         </is>
       </c>
       <c r="B41" s="1" t="n"/>
@@ -2645,37 +2645,37 @@
         </is>
       </c>
       <c r="G41" s="1" t="n">
-        <v>11006265</v>
+        <v>12992022</v>
       </c>
       <c r="H41" s="1" t="n">
-        <v>46440474</v>
+        <v>8202303</v>
       </c>
       <c r="I41" s="1" t="n">
-        <v>53351827</v>
+        <v>5522220</v>
       </c>
       <c r="J41" s="1" t="n">
-        <v>11006265</v>
+        <v>12992022</v>
       </c>
       <c r="K41" s="1" t="n">
-        <v>46440474</v>
+        <v>8202303</v>
       </c>
       <c r="L41" s="1" t="n">
-        <v>53351827</v>
+        <v>5522220</v>
       </c>
       <c r="M41" s="1" t="n">
-        <v>11006265</v>
+        <v>12992022</v>
       </c>
       <c r="N41" s="1" t="n">
-        <v>46440474</v>
+        <v>8202303</v>
       </c>
       <c r="O41" s="1" t="n">
-        <v>53351827</v>
+        <v>5522220</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>계속영업이익(손실)</t>
+          <t>중단영업당기순이익(손실)</t>
         </is>
       </c>
       <c r="B42" s="1" t="n"/>
@@ -2696,37 +2696,37 @@
         </is>
       </c>
       <c r="G42" s="1" t="n">
-        <v>15487100</v>
+        <v>-719721</v>
       </c>
       <c r="H42" s="1" t="n">
-        <v>55654077</v>
+        <v>-218689</v>
       </c>
       <c r="I42" s="1" t="n">
-        <v>39907450</v>
+        <v>170857</v>
       </c>
       <c r="J42" s="1" t="n">
-        <v>15487100</v>
+        <v>-719721</v>
       </c>
       <c r="K42" s="1" t="n">
-        <v>55654077</v>
+        <v>-218689</v>
       </c>
       <c r="L42" s="1" t="n">
-        <v>39907450</v>
+        <v>170857</v>
       </c>
       <c r="M42" s="1" t="n">
-        <v>15487100</v>
+        <v>-719721</v>
       </c>
       <c r="N42" s="1" t="n">
-        <v>55654077</v>
+        <v>-218689</v>
       </c>
       <c r="O42" s="1" t="n">
-        <v>39907450</v>
+        <v>170857</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>당기순이익(손실)</t>
+          <t>연결당기순이익</t>
         </is>
       </c>
       <c r="B43" s="1" t="n"/>
@@ -2747,31 +2747,31 @@
         </is>
       </c>
       <c r="G43" s="1" t="n">
-        <v>15487100</v>
+        <v>12272301</v>
       </c>
       <c r="H43" s="1" t="n">
-        <v>55654077</v>
+        <v>7983614</v>
       </c>
       <c r="I43" s="1" t="n">
-        <v>39907450</v>
+        <v>5693077</v>
       </c>
       <c r="J43" s="1" t="n">
-        <v>15487100</v>
+        <v>12272301</v>
       </c>
       <c r="K43" s="1" t="n">
-        <v>55654077</v>
+        <v>7983614</v>
       </c>
       <c r="L43" s="1" t="n">
-        <v>39907450</v>
+        <v>5693077</v>
       </c>
       <c r="M43" s="1" t="n">
-        <v>15487100</v>
+        <v>12272301</v>
       </c>
       <c r="N43" s="1" t="n">
-        <v>55654077</v>
+        <v>7983614</v>
       </c>
       <c r="O43" s="1" t="n">
-        <v>39907450</v>
+        <v>5693077</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
saved initial state of db
이거 먼저 저장해놓고...
세션분리작업 시작해야겠다
</commit_message>
<xml_diff>
--- a/data/output/연결 손익계산서.xlsx
+++ b/data/output/연결 손익계산서.xlsx
@@ -468,7 +468,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:O43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,8 +476,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="25.4" customWidth="1" min="1" max="1"/>
-    <col width="34.4" customWidth="1" min="2" max="2"/>
+    <col width="29" customWidth="1" min="1" max="1"/>
+    <col width="48.8" customWidth="1" min="2" max="2"/>
     <col width="52.4" customWidth="1" min="3" max="3"/>
     <col width="11" customWidth="1" min="4" max="4"/>
     <col width="11" customWidth="1" min="5" max="5"/>
@@ -485,9 +485,12 @@
     <col width="11" customWidth="1" min="7" max="7"/>
     <col width="11" customWidth="1" min="8" max="8"/>
     <col width="11" customWidth="1" min="9" max="9"/>
-    <col width="13" customWidth="1" min="10" max="10"/>
-    <col width="13" customWidth="1" min="11" max="11"/>
-    <col width="13" customWidth="1" min="12" max="12"/>
+    <col width="11" customWidth="1" min="10" max="10"/>
+    <col width="11" customWidth="1" min="11" max="11"/>
+    <col width="11" customWidth="1" min="12" max="12"/>
+    <col width="13" customWidth="1" min="13" max="13"/>
+    <col width="13" customWidth="1" min="14" max="14"/>
+    <col width="13" customWidth="1" min="15" max="15"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -496,25 +499,32 @@
       <c r="C1" s="3" t="n"/>
       <c r="D1" s="4" t="inlineStr">
         <is>
-          <t>Hyundai</t>
+          <t>Samsung</t>
         </is>
       </c>
       <c r="E1" s="1" t="n"/>
       <c r="F1" s="1" t="n"/>
       <c r="G1" s="4" t="inlineStr">
         <is>
-          <t>Sum</t>
+          <t>Hyundai</t>
         </is>
       </c>
       <c r="H1" s="1" t="n"/>
       <c r="I1" s="1" t="n"/>
       <c r="J1" s="4" t="inlineStr">
         <is>
-          <t>Average</t>
+          <t>Sum</t>
         </is>
       </c>
       <c r="K1" s="1" t="n"/>
       <c r="L1" s="1" t="n"/>
+      <c r="M1" s="4" t="inlineStr">
+        <is>
+          <t>Average</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="n"/>
+      <c r="O1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n"/>
@@ -561,6 +571,21 @@
         </is>
       </c>
       <c r="L2" s="5" t="inlineStr">
+        <is>
+          <t>2021년</t>
+        </is>
+      </c>
+      <c r="M2" s="5" t="inlineStr">
+        <is>
+          <t>2023년</t>
+        </is>
+      </c>
+      <c r="N2" s="5" t="inlineStr">
+        <is>
+          <t>2022년</t>
+        </is>
+      </c>
+      <c r="O2" s="5" t="inlineStr">
         <is>
           <t>2021년</t>
         </is>
@@ -579,41 +604,59 @@
       <c r="J3" s="6" t="n"/>
       <c r="K3" s="6" t="n"/>
       <c r="L3" s="6" t="n"/>
+      <c r="M3" s="6" t="n"/>
+      <c r="N3" s="6" t="n"/>
+      <c r="O3" s="6" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>매출액</t>
+          <t>영업수익</t>
         </is>
       </c>
       <c r="B4" s="1" t="n"/>
       <c r="C4" s="1" t="n"/>
       <c r="D4" s="1" t="n">
-        <v>162663579</v>
+        <v>258935494</v>
       </c>
       <c r="E4" s="1" t="n">
-        <v>142151469</v>
+        <v>302231360</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>116448159</v>
-      </c>
-      <c r="G4" s="1" t="n">
-        <v>162663579</v>
-      </c>
-      <c r="H4" s="1" t="n">
-        <v>142151469</v>
-      </c>
-      <c r="I4" s="1" t="n">
-        <v>116448159</v>
+        <v>279604799</v>
+      </c>
+      <c r="G4" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H4" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I4" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="J4" s="1" t="n">
-        <v>162663579</v>
+        <v>258935494</v>
       </c>
       <c r="K4" s="1" t="n">
-        <v>142151469</v>
+        <v>302231360</v>
       </c>
       <c r="L4" s="1" t="n">
-        <v>116448159</v>
+        <v>279604799</v>
+      </c>
+      <c r="M4" s="1" t="n">
+        <v>258935494</v>
+      </c>
+      <c r="N4" s="1" t="n">
+        <v>302231360</v>
+      </c>
+      <c r="O4" s="1" t="n">
+        <v>279604799</v>
       </c>
     </row>
     <row r="5">
@@ -625,13 +668,13 @@
       <c r="B5" s="1" t="n"/>
       <c r="C5" s="1" t="n"/>
       <c r="D5" s="1" t="n">
-        <v>129179183</v>
+        <v>180388580</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>113879569</v>
+        <v>190041770</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>94721313</v>
+        <v>166411342</v>
       </c>
       <c r="G5" s="1" t="n">
         <v>129179183</v>
@@ -643,13 +686,22 @@
         <v>94721313</v>
       </c>
       <c r="J5" s="1" t="n">
-        <v>129179183</v>
+        <v>309567763</v>
       </c>
       <c r="K5" s="1" t="n">
-        <v>113879569</v>
+        <v>303921339</v>
       </c>
       <c r="L5" s="1" t="n">
-        <v>94721313</v>
+        <v>261132655</v>
+      </c>
+      <c r="M5" s="1" t="n">
+        <v>154783881.5</v>
+      </c>
+      <c r="N5" s="1" t="n">
+        <v>151960669.5</v>
+      </c>
+      <c r="O5" s="1" t="n">
+        <v>130566327.5</v>
       </c>
     </row>
     <row r="6">
@@ -661,13 +713,13 @@
       <c r="B6" s="1" t="n"/>
       <c r="C6" s="1" t="n"/>
       <c r="D6" s="1" t="n">
-        <v>33484396</v>
+        <v>78546914</v>
       </c>
       <c r="E6" s="1" t="n">
-        <v>28271900</v>
+        <v>112189590</v>
       </c>
       <c r="F6" s="1" t="n">
-        <v>21726846</v>
+        <v>113193457</v>
       </c>
       <c r="G6" s="1" t="n">
         <v>33484396</v>
@@ -679,13 +731,22 @@
         <v>21726846</v>
       </c>
       <c r="J6" s="1" t="n">
-        <v>33484396</v>
+        <v>112031310</v>
       </c>
       <c r="K6" s="1" t="n">
-        <v>28271900</v>
+        <v>140461490</v>
       </c>
       <c r="L6" s="1" t="n">
-        <v>21726846</v>
+        <v>134920303</v>
+      </c>
+      <c r="M6" s="1" t="n">
+        <v>56015655</v>
+      </c>
+      <c r="N6" s="1" t="n">
+        <v>70230745</v>
+      </c>
+      <c r="O6" s="1" t="n">
+        <v>67460151.5</v>
       </c>
     </row>
     <row r="7">
@@ -697,13 +758,13 @@
       <c r="B7" s="1" t="n"/>
       <c r="C7" s="1" t="n"/>
       <c r="D7" s="1" t="n">
-        <v>18357495</v>
+        <v>71979938</v>
       </c>
       <c r="E7" s="1" t="n">
-        <v>18446972</v>
+        <v>68812960</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>15200325</v>
+        <v>61559601</v>
       </c>
       <c r="G7" s="1" t="n">
         <v>18357495</v>
@@ -715,13 +776,22 @@
         <v>15200325</v>
       </c>
       <c r="J7" s="1" t="n">
-        <v>18357495</v>
+        <v>90337433</v>
       </c>
       <c r="K7" s="1" t="n">
-        <v>18446972</v>
+        <v>87259932</v>
       </c>
       <c r="L7" s="1" t="n">
-        <v>15200325</v>
+        <v>76759926</v>
+      </c>
+      <c r="M7" s="1" t="n">
+        <v>45168716.5</v>
+      </c>
+      <c r="N7" s="1" t="n">
+        <v>43629966</v>
+      </c>
+      <c r="O7" s="1" t="n">
+        <v>38379963</v>
       </c>
     </row>
     <row r="8">
@@ -733,13 +803,13 @@
       <c r="B8" s="1" t="n"/>
       <c r="C8" s="1" t="n"/>
       <c r="D8" s="1" t="n">
-        <v>15126901</v>
+        <v>6566976</v>
       </c>
       <c r="E8" s="1" t="n">
-        <v>9824928</v>
+        <v>43376630</v>
       </c>
       <c r="F8" s="1" t="n">
-        <v>6526521</v>
+        <v>51633856</v>
       </c>
       <c r="G8" s="1" t="n">
         <v>15126901</v>
@@ -751,229 +821,316 @@
         <v>6526521</v>
       </c>
       <c r="J8" s="1" t="n">
-        <v>15126901</v>
+        <v>21693877</v>
       </c>
       <c r="K8" s="1" t="n">
-        <v>9824928</v>
+        <v>53201558</v>
       </c>
       <c r="L8" s="1" t="n">
-        <v>6526521</v>
+        <v>58160377</v>
+      </c>
+      <c r="M8" s="1" t="n">
+        <v>10846938.5</v>
+      </c>
+      <c r="N8" s="1" t="n">
+        <v>26600779</v>
+      </c>
+      <c r="O8" s="1" t="n">
+        <v>29080188.5</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>공동기업및관계기업투자손익</t>
+          <t>기타이익</t>
         </is>
       </c>
       <c r="B9" s="1" t="n"/>
       <c r="C9" s="1" t="n"/>
       <c r="D9" s="1" t="n">
-        <v>2470933</v>
+        <v>1180448</v>
       </c>
       <c r="E9" s="1" t="n">
-        <v>1557630</v>
+        <v>1962071</v>
       </c>
       <c r="F9" s="1" t="n">
-        <v>1302150</v>
-      </c>
-      <c r="G9" s="1" t="n">
-        <v>2470933</v>
-      </c>
-      <c r="H9" s="1" t="n">
-        <v>1557630</v>
-      </c>
-      <c r="I9" s="1" t="n">
-        <v>1302150</v>
+        <v>2205695</v>
+      </c>
+      <c r="G9" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H9" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I9" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="J9" s="1" t="n">
-        <v>2470933</v>
+        <v>1180448</v>
       </c>
       <c r="K9" s="1" t="n">
-        <v>1557630</v>
+        <v>1962071</v>
       </c>
       <c r="L9" s="1" t="n">
-        <v>1302150</v>
+        <v>2205695</v>
+      </c>
+      <c r="M9" s="1" t="n">
+        <v>1180448</v>
+      </c>
+      <c r="N9" s="1" t="n">
+        <v>1962071</v>
+      </c>
+      <c r="O9" s="1" t="n">
+        <v>2205695</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>금융수익</t>
+          <t>기타손실</t>
         </is>
       </c>
       <c r="B10" s="1" t="n"/>
       <c r="C10" s="1" t="n"/>
       <c r="D10" s="1" t="n">
-        <v>1559538</v>
+        <v>1083327</v>
       </c>
       <c r="E10" s="1" t="n">
-        <v>985893</v>
+        <v>1790176</v>
       </c>
       <c r="F10" s="1" t="n">
-        <v>841196</v>
-      </c>
-      <c r="G10" s="1" t="n">
-        <v>1559538</v>
-      </c>
-      <c r="H10" s="1" t="n">
-        <v>985893</v>
-      </c>
-      <c r="I10" s="1" t="n">
-        <v>841196</v>
+        <v>2055971</v>
+      </c>
+      <c r="G10" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H10" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I10" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="J10" s="1" t="n">
-        <v>1559538</v>
+        <v>1083327</v>
       </c>
       <c r="K10" s="1" t="n">
-        <v>985893</v>
+        <v>1790176</v>
       </c>
       <c r="L10" s="1" t="n">
-        <v>841196</v>
+        <v>2055971</v>
+      </c>
+      <c r="M10" s="1" t="n">
+        <v>1083327</v>
+      </c>
+      <c r="N10" s="1" t="n">
+        <v>1790176</v>
+      </c>
+      <c r="O10" s="1" t="n">
+        <v>2055971</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>금융비용</t>
+          <t>지분법이익</t>
         </is>
       </c>
       <c r="B11" s="1" t="n"/>
       <c r="C11" s="1" t="n"/>
       <c r="D11" s="1" t="n">
-        <v>970700</v>
+        <v>887550</v>
       </c>
       <c r="E11" s="1" t="n">
-        <v>879638</v>
+        <v>1090643</v>
       </c>
       <c r="F11" s="1" t="n">
-        <v>512836</v>
-      </c>
-      <c r="G11" s="1" t="n">
-        <v>970700</v>
-      </c>
-      <c r="H11" s="1" t="n">
-        <v>879638</v>
-      </c>
-      <c r="I11" s="1" t="n">
-        <v>512836</v>
+        <v>729614</v>
+      </c>
+      <c r="G11" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H11" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I11" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="J11" s="1" t="n">
-        <v>970700</v>
+        <v>887550</v>
       </c>
       <c r="K11" s="1" t="n">
-        <v>879638</v>
+        <v>1090643</v>
       </c>
       <c r="L11" s="1" t="n">
-        <v>512836</v>
+        <v>729614</v>
+      </c>
+      <c r="M11" s="1" t="n">
+        <v>887550</v>
+      </c>
+      <c r="N11" s="1" t="n">
+        <v>1090643</v>
+      </c>
+      <c r="O11" s="1" t="n">
+        <v>729614</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>기타수익</t>
+          <t>금융수익</t>
         </is>
       </c>
       <c r="B12" s="1" t="n"/>
       <c r="C12" s="1" t="n"/>
       <c r="D12" s="1" t="n">
-        <v>1782333</v>
+        <v>16100148</v>
       </c>
       <c r="E12" s="1" t="n">
-        <v>1930914</v>
+        <v>20828995</v>
       </c>
       <c r="F12" s="1" t="n">
-        <v>1377997</v>
+        <v>8543187</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>1782333</v>
+        <v>1559538</v>
       </c>
       <c r="H12" s="1" t="n">
-        <v>1930914</v>
+        <v>985893</v>
       </c>
       <c r="I12" s="1" t="n">
-        <v>1377997</v>
+        <v>841196</v>
       </c>
       <c r="J12" s="1" t="n">
-        <v>1782333</v>
+        <v>17659686</v>
       </c>
       <c r="K12" s="1" t="n">
-        <v>1930914</v>
+        <v>21814888</v>
       </c>
       <c r="L12" s="1" t="n">
-        <v>1377997</v>
+        <v>9384383</v>
+      </c>
+      <c r="M12" s="1" t="n">
+        <v>8829843</v>
+      </c>
+      <c r="N12" s="1" t="n">
+        <v>10907444</v>
+      </c>
+      <c r="O12" s="1" t="n">
+        <v>4692191.5</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>기타비용</t>
+          <t>금융비용</t>
         </is>
       </c>
       <c r="B13" s="1" t="n"/>
       <c r="C13" s="1" t="n"/>
       <c r="D13" s="1" t="n">
-        <v>2350343</v>
+        <v>12645530</v>
       </c>
       <c r="E13" s="1" t="n">
-        <v>2238256</v>
+        <v>19027689</v>
       </c>
       <c r="F13" s="1" t="n">
-        <v>1745985</v>
+        <v>7704554</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>2350343</v>
+        <v>970700</v>
       </c>
       <c r="H13" s="1" t="n">
-        <v>2238256</v>
+        <v>879638</v>
       </c>
       <c r="I13" s="1" t="n">
-        <v>1745985</v>
+        <v>512836</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>2350343</v>
+        <v>13616230</v>
       </c>
       <c r="K13" s="1" t="n">
-        <v>2238256</v>
+        <v>19907327</v>
       </c>
       <c r="L13" s="1" t="n">
-        <v>1745985</v>
+        <v>8217390</v>
+      </c>
+      <c r="M13" s="1" t="n">
+        <v>6808115</v>
+      </c>
+      <c r="N13" s="1" t="n">
+        <v>9953663.5</v>
+      </c>
+      <c r="O13" s="1" t="n">
+        <v>4108695</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>법인세비용차감전순이익</t>
+          <t>법인세비용차감전순이익(손실)</t>
         </is>
       </c>
       <c r="B14" s="1" t="n"/>
       <c r="C14" s="1" t="n"/>
       <c r="D14" s="1" t="n">
-        <v>17618662</v>
+        <v>11006265</v>
       </c>
       <c r="E14" s="1" t="n">
-        <v>11181471</v>
+        <v>46440474</v>
       </c>
       <c r="F14" s="1" t="n">
-        <v>7789043</v>
-      </c>
-      <c r="G14" s="1" t="n">
-        <v>17618662</v>
-      </c>
-      <c r="H14" s="1" t="n">
-        <v>11181471</v>
-      </c>
-      <c r="I14" s="1" t="n">
-        <v>7789043</v>
+        <v>53351827</v>
+      </c>
+      <c r="G14" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H14" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I14" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="J14" s="1" t="n">
-        <v>17618662</v>
+        <v>11006265</v>
       </c>
       <c r="K14" s="1" t="n">
-        <v>11181471</v>
+        <v>46440474</v>
       </c>
       <c r="L14" s="1" t="n">
-        <v>7789043</v>
+        <v>53351827</v>
+      </c>
+      <c r="M14" s="1" t="n">
+        <v>11006265</v>
+      </c>
+      <c r="N14" s="1" t="n">
+        <v>46440474</v>
+      </c>
+      <c r="O14" s="1" t="n">
+        <v>53351827</v>
       </c>
     </row>
     <row r="15">
@@ -985,13 +1142,13 @@
       <c r="B15" s="1" t="n"/>
       <c r="C15" s="1" t="n"/>
       <c r="D15" s="1" t="n">
-        <v>4626640</v>
+        <v>-4480835</v>
       </c>
       <c r="E15" s="1" t="n">
-        <v>2979168</v>
+        <v>-9213603</v>
       </c>
       <c r="F15" s="1" t="n">
-        <v>2266823</v>
+        <v>13444377</v>
       </c>
       <c r="G15" s="1" t="n">
         <v>4626640</v>
@@ -1003,121 +1160,193 @@
         <v>2266823</v>
       </c>
       <c r="J15" s="1" t="n">
-        <v>4626640</v>
+        <v>145805</v>
       </c>
       <c r="K15" s="1" t="n">
-        <v>2979168</v>
+        <v>-6234435</v>
       </c>
       <c r="L15" s="1" t="n">
-        <v>2266823</v>
+        <v>15711200</v>
+      </c>
+      <c r="M15" s="1" t="n">
+        <v>72902.5</v>
+      </c>
+      <c r="N15" s="1" t="n">
+        <v>-3117217.5</v>
+      </c>
+      <c r="O15" s="1" t="n">
+        <v>7855600</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>계속영업연결당기순이익</t>
+          <t>계속영업이익(손실)</t>
         </is>
       </c>
       <c r="B16" s="1" t="n"/>
       <c r="C16" s="1" t="n"/>
       <c r="D16" s="1" t="n">
-        <v>12992022</v>
+        <v>15487100</v>
       </c>
       <c r="E16" s="1" t="n">
-        <v>8202303</v>
+        <v>55654077</v>
       </c>
       <c r="F16" s="1" t="n">
-        <v>5522220</v>
-      </c>
-      <c r="G16" s="1" t="n">
-        <v>12992022</v>
-      </c>
-      <c r="H16" s="1" t="n">
-        <v>8202303</v>
-      </c>
-      <c r="I16" s="1" t="n">
-        <v>5522220</v>
+        <v>39907450</v>
+      </c>
+      <c r="G16" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H16" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I16" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="J16" s="1" t="n">
-        <v>12992022</v>
+        <v>15487100</v>
       </c>
       <c r="K16" s="1" t="n">
-        <v>8202303</v>
+        <v>55654077</v>
       </c>
       <c r="L16" s="1" t="n">
-        <v>5522220</v>
+        <v>39907450</v>
+      </c>
+      <c r="M16" s="1" t="n">
+        <v>15487100</v>
+      </c>
+      <c r="N16" s="1" t="n">
+        <v>55654077</v>
+      </c>
+      <c r="O16" s="1" t="n">
+        <v>39907450</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>중단영업당기순이익(손실)</t>
+          <t>당기순이익(손실)</t>
         </is>
       </c>
       <c r="B17" s="1" t="n"/>
       <c r="C17" s="1" t="n"/>
       <c r="D17" s="1" t="n">
-        <v>-719721</v>
+        <v>15487100</v>
       </c>
       <c r="E17" s="1" t="n">
-        <v>-218689</v>
+        <v>55654077</v>
       </c>
       <c r="F17" s="1" t="n">
-        <v>170857</v>
-      </c>
-      <c r="G17" s="1" t="n">
-        <v>-719721</v>
-      </c>
-      <c r="H17" s="1" t="n">
-        <v>-218689</v>
-      </c>
-      <c r="I17" s="1" t="n">
-        <v>170857</v>
+        <v>39907450</v>
+      </c>
+      <c r="G17" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H17" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I17" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="J17" s="1" t="n">
-        <v>-719721</v>
+        <v>15487100</v>
       </c>
       <c r="K17" s="1" t="n">
-        <v>-218689</v>
+        <v>55654077</v>
       </c>
       <c r="L17" s="1" t="n">
-        <v>170857</v>
+        <v>39907450</v>
+      </c>
+      <c r="M17" s="1" t="n">
+        <v>15487100</v>
+      </c>
+      <c r="N17" s="1" t="n">
+        <v>55654077</v>
+      </c>
+      <c r="O17" s="1" t="n">
+        <v>39907450</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>연결당기순이익</t>
+          <t>당기순이익(손실)의 귀속</t>
         </is>
       </c>
       <c r="B18" s="1" t="n"/>
       <c r="C18" s="1" t="n"/>
-      <c r="D18" s="1" t="n">
-        <v>12272301</v>
-      </c>
-      <c r="E18" s="1" t="n">
-        <v>7983614</v>
-      </c>
-      <c r="F18" s="1" t="n">
-        <v>5693077</v>
-      </c>
-      <c r="G18" s="1" t="n">
-        <v>12272301</v>
-      </c>
-      <c r="H18" s="1" t="n">
-        <v>7983614</v>
-      </c>
-      <c r="I18" s="1" t="n">
-        <v>5693077</v>
-      </c>
-      <c r="J18" s="1" t="n">
-        <v>12272301</v>
-      </c>
-      <c r="K18" s="1" t="n">
-        <v>7983614</v>
-      </c>
-      <c r="L18" s="1" t="n">
-        <v>5693077</v>
+      <c r="D18" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E18" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F18" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G18" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H18" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I18" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J18" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K18" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L18" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M18" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N18" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O18" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
     </row>
     <row r="19">
@@ -1126,22 +1355,20 @@
           <t>당기순이익(손실)의 귀속</t>
         </is>
       </c>
-      <c r="B19" s="1" t="n"/>
+      <c r="B19" s="1" t="inlineStr">
+        <is>
+          <t>지배기업의 소유주에게 귀속되는 당기순이익(손실)</t>
+        </is>
+      </c>
       <c r="C19" s="1" t="n"/>
-      <c r="D19" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E19" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F19" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D19" s="1" t="n">
+        <v>14473401</v>
+      </c>
+      <c r="E19" s="1" t="n">
+        <v>54730018</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <v>39243791</v>
       </c>
       <c r="G19" s="7" t="inlineStr">
         <is>
@@ -1158,20 +1385,23 @@
           <t>-</t>
         </is>
       </c>
-      <c r="J19" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K19" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L19" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="J19" s="1" t="n">
+        <v>14473401</v>
+      </c>
+      <c r="K19" s="1" t="n">
+        <v>54730018</v>
+      </c>
+      <c r="L19" s="1" t="n">
+        <v>39243791</v>
+      </c>
+      <c r="M19" s="1" t="n">
+        <v>14473401</v>
+      </c>
+      <c r="N19" s="1" t="n">
+        <v>54730018</v>
+      </c>
+      <c r="O19" s="1" t="n">
+        <v>39243791</v>
       </c>
     </row>
     <row r="20">
@@ -1182,36 +1412,51 @@
       </c>
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>지배기업소유주지분</t>
+          <t>비지배지분에 귀속되는 당기순이익(손실)</t>
         </is>
       </c>
       <c r="C20" s="1" t="n"/>
       <c r="D20" s="1" t="n">
-        <v>11961717</v>
+        <v>1013699</v>
       </c>
       <c r="E20" s="1" t="n">
-        <v>7364364</v>
+        <v>924059</v>
       </c>
       <c r="F20" s="1" t="n">
-        <v>4942356</v>
-      </c>
-      <c r="G20" s="1" t="n">
-        <v>11961717</v>
-      </c>
-      <c r="H20" s="1" t="n">
-        <v>7364364</v>
-      </c>
-      <c r="I20" s="1" t="n">
-        <v>4942356</v>
+        <v>663659</v>
+      </c>
+      <c r="G20" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H20" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I20" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="J20" s="1" t="n">
-        <v>11961717</v>
+        <v>1013699</v>
       </c>
       <c r="K20" s="1" t="n">
-        <v>7364364</v>
+        <v>924059</v>
       </c>
       <c r="L20" s="1" t="n">
-        <v>4942356</v>
+        <v>663659</v>
+      </c>
+      <c r="M20" s="1" t="n">
+        <v>1013699</v>
+      </c>
+      <c r="N20" s="1" t="n">
+        <v>924059</v>
+      </c>
+      <c r="O20" s="1" t="n">
+        <v>663659</v>
       </c>
     </row>
     <row r="21">
@@ -1222,45 +1467,64 @@
       </c>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>비지배지분</t>
+          <t>지배기업소유주지분</t>
         </is>
       </c>
       <c r="C21" s="1" t="n"/>
-      <c r="D21" s="1" t="n">
-        <v>310584</v>
-      </c>
-      <c r="E21" s="1" t="n">
-        <v>619250</v>
-      </c>
-      <c r="F21" s="1" t="n">
-        <v>750721</v>
+      <c r="D21" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E21" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F21" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="G21" s="1" t="n">
-        <v>310584</v>
+        <v>11961717</v>
       </c>
       <c r="H21" s="1" t="n">
-        <v>619250</v>
+        <v>7364364</v>
       </c>
       <c r="I21" s="1" t="n">
-        <v>750721</v>
+        <v>4942356</v>
       </c>
       <c r="J21" s="1" t="n">
-        <v>310584</v>
+        <v>11961717</v>
       </c>
       <c r="K21" s="1" t="n">
-        <v>619250</v>
+        <v>7364364</v>
       </c>
       <c r="L21" s="1" t="n">
-        <v>750721</v>
+        <v>4942356</v>
+      </c>
+      <c r="M21" s="1" t="n">
+        <v>11961717</v>
+      </c>
+      <c r="N21" s="1" t="n">
+        <v>7364364</v>
+      </c>
+      <c r="O21" s="1" t="n">
+        <v>4942356</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>주당이익</t>
-        </is>
-      </c>
-      <c r="B22" s="1" t="n"/>
+          <t>당기순이익(손실)의 귀속</t>
+        </is>
+      </c>
+      <c r="B22" s="1" t="inlineStr">
+        <is>
+          <t>비지배지분</t>
+        </is>
+      </c>
       <c r="C22" s="1" t="n"/>
       <c r="D22" s="7" t="inlineStr">
         <is>
@@ -1277,35 +1541,32 @@
           <t>-</t>
         </is>
       </c>
-      <c r="G22" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H22" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I22" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J22" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K22" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L22" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="G22" s="1" t="n">
+        <v>310584</v>
+      </c>
+      <c r="H22" s="1" t="n">
+        <v>619250</v>
+      </c>
+      <c r="I22" s="1" t="n">
+        <v>750721</v>
+      </c>
+      <c r="J22" s="1" t="n">
+        <v>310584</v>
+      </c>
+      <c r="K22" s="1" t="n">
+        <v>619250</v>
+      </c>
+      <c r="L22" s="1" t="n">
+        <v>750721</v>
+      </c>
+      <c r="M22" s="1" t="n">
+        <v>310584</v>
+      </c>
+      <c r="N22" s="1" t="n">
+        <v>619250</v>
+      </c>
+      <c r="O22" s="1" t="n">
+        <v>750721</v>
       </c>
     </row>
     <row r="23">
@@ -1314,11 +1575,7 @@
           <t>주당이익</t>
         </is>
       </c>
-      <c r="B23" s="1" t="inlineStr">
-        <is>
-          <t>기본주당이익 (단위 :원)</t>
-        </is>
-      </c>
+      <c r="B23" s="1" t="n"/>
       <c r="C23" s="1" t="n"/>
       <c r="D23" s="7" t="inlineStr">
         <is>
@@ -1365,6 +1622,21 @@
           <t>-</t>
         </is>
       </c>
+      <c r="M23" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N23" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O23" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
@@ -1374,40 +1646,51 @@
       </c>
       <c r="B24" s="1" t="inlineStr">
         <is>
-          <t>기본주당이익 (단위 :원)</t>
-        </is>
-      </c>
-      <c r="C24" s="1" t="inlineStr">
-        <is>
-          <t>보통주기본주당이익(손실) (단위 : 원)</t>
-        </is>
-      </c>
+          <t>기본주당이익(손실) (단위 : 원)</t>
+        </is>
+      </c>
+      <c r="C24" s="1" t="n"/>
       <c r="D24" s="1" t="n">
-        <v>45703</v>
+        <v>2131</v>
       </c>
       <c r="E24" s="1" t="n">
-        <v>28521</v>
+        <v>8057</v>
       </c>
       <c r="F24" s="1" t="n">
-        <v>18979</v>
-      </c>
-      <c r="G24" s="1" t="n">
-        <v>45703</v>
-      </c>
-      <c r="H24" s="1" t="n">
-        <v>28521</v>
-      </c>
-      <c r="I24" s="1" t="n">
-        <v>18979</v>
+        <v>5777</v>
+      </c>
+      <c r="G24" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H24" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I24" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="J24" s="1" t="n">
-        <v>45703</v>
+        <v>2131</v>
       </c>
       <c r="K24" s="1" t="n">
-        <v>28521</v>
+        <v>8057</v>
       </c>
       <c r="L24" s="1" t="n">
-        <v>18979</v>
+        <v>5777</v>
+      </c>
+      <c r="M24" s="1" t="n">
+        <v>2131</v>
+      </c>
+      <c r="N24" s="1" t="n">
+        <v>8057</v>
+      </c>
+      <c r="O24" s="1" t="n">
+        <v>5777</v>
       </c>
     </row>
     <row r="25">
@@ -1418,40 +1701,51 @@
       </c>
       <c r="B25" s="1" t="inlineStr">
         <is>
-          <t>기본주당이익 (단위 :원)</t>
-        </is>
-      </c>
-      <c r="C25" s="1" t="inlineStr">
-        <is>
-          <t>계속영업 보통주기본주당이익(손실) (단위: 원)</t>
-        </is>
-      </c>
+          <t>희석주당이익(손실) (단위 : 원)</t>
+        </is>
+      </c>
+      <c r="C25" s="1" t="n"/>
       <c r="D25" s="1" t="n">
-        <v>47622</v>
+        <v>2131</v>
       </c>
       <c r="E25" s="1" t="n">
-        <v>29105</v>
+        <v>8057</v>
       </c>
       <c r="F25" s="1" t="n">
-        <v>18521</v>
-      </c>
-      <c r="G25" s="1" t="n">
-        <v>47622</v>
-      </c>
-      <c r="H25" s="1" t="n">
-        <v>29105</v>
-      </c>
-      <c r="I25" s="1" t="n">
-        <v>18521</v>
+        <v>5777</v>
+      </c>
+      <c r="G25" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H25" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I25" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="J25" s="1" t="n">
-        <v>47622</v>
+        <v>2131</v>
       </c>
       <c r="K25" s="1" t="n">
-        <v>29105</v>
+        <v>8057</v>
       </c>
       <c r="L25" s="1" t="n">
-        <v>18521</v>
+        <v>5777</v>
+      </c>
+      <c r="M25" s="1" t="n">
+        <v>2131</v>
+      </c>
+      <c r="N25" s="1" t="n">
+        <v>8057</v>
+      </c>
+      <c r="O25" s="1" t="n">
+        <v>5777</v>
       </c>
     </row>
     <row r="26">
@@ -1465,37 +1759,66 @@
           <t>기본주당이익 (단위 :원)</t>
         </is>
       </c>
-      <c r="C26" s="1" t="inlineStr">
-        <is>
-          <t>중단영업 보통주기본주당이익(손실) (단위: 원)</t>
-        </is>
-      </c>
-      <c r="D26" s="1" t="n">
-        <v>-1919</v>
-      </c>
-      <c r="E26" s="1" t="n">
-        <v>-584</v>
-      </c>
-      <c r="F26" s="1" t="n">
-        <v>458</v>
-      </c>
-      <c r="G26" s="1" t="n">
-        <v>-1919</v>
-      </c>
-      <c r="H26" s="1" t="n">
-        <v>-584</v>
-      </c>
-      <c r="I26" s="1" t="n">
-        <v>458</v>
-      </c>
-      <c r="J26" s="1" t="n">
-        <v>-1919</v>
-      </c>
-      <c r="K26" s="1" t="n">
-        <v>-584</v>
-      </c>
-      <c r="L26" s="1" t="n">
-        <v>458</v>
+      <c r="C26" s="1" t="n"/>
+      <c r="D26" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E26" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F26" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G26" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H26" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I26" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J26" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K26" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L26" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M26" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N26" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O26" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
     </row>
     <row r="27">
@@ -1511,35 +1834,50 @@
       </c>
       <c r="C27" s="1" t="inlineStr">
         <is>
-          <t>1우선주 기본주당이익(손실) (단위 : 원)</t>
-        </is>
-      </c>
-      <c r="D27" s="1" t="n">
-        <v>45535</v>
-      </c>
-      <c r="E27" s="1" t="n">
-        <v>28207</v>
-      </c>
-      <c r="F27" s="1" t="n">
-        <v>19002</v>
+          <t>보통주기본주당이익(손실) (단위 : 원)</t>
+        </is>
+      </c>
+      <c r="D27" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E27" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F27" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="G27" s="1" t="n">
-        <v>45535</v>
+        <v>45703</v>
       </c>
       <c r="H27" s="1" t="n">
-        <v>28207</v>
+        <v>28521</v>
       </c>
       <c r="I27" s="1" t="n">
-        <v>19002</v>
+        <v>18979</v>
       </c>
       <c r="J27" s="1" t="n">
-        <v>45535</v>
+        <v>45703</v>
       </c>
       <c r="K27" s="1" t="n">
-        <v>28207</v>
+        <v>28521</v>
       </c>
       <c r="L27" s="1" t="n">
-        <v>19002</v>
+        <v>18979</v>
+      </c>
+      <c r="M27" s="1" t="n">
+        <v>45703</v>
+      </c>
+      <c r="N27" s="1" t="n">
+        <v>28521</v>
+      </c>
+      <c r="O27" s="1" t="n">
+        <v>18979</v>
       </c>
     </row>
     <row r="28">
@@ -1555,35 +1893,50 @@
       </c>
       <c r="C28" s="1" t="inlineStr">
         <is>
-          <t>계속영업 1우선주기본주당이익(손실) (단위 : 원)</t>
-        </is>
-      </c>
-      <c r="D28" s="1" t="n">
-        <v>47445</v>
-      </c>
-      <c r="E28" s="1" t="n">
-        <v>28783</v>
-      </c>
-      <c r="F28" s="1" t="n">
-        <v>18545</v>
+          <t>계속영업 보통주기본주당이익(손실) (단위: 원)</t>
+        </is>
+      </c>
+      <c r="D28" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E28" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F28" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="G28" s="1" t="n">
-        <v>47445</v>
+        <v>47622</v>
       </c>
       <c r="H28" s="1" t="n">
-        <v>28783</v>
+        <v>29105</v>
       </c>
       <c r="I28" s="1" t="n">
-        <v>18545</v>
+        <v>18521</v>
       </c>
       <c r="J28" s="1" t="n">
-        <v>47445</v>
+        <v>47622</v>
       </c>
       <c r="K28" s="1" t="n">
-        <v>28783</v>
+        <v>29105</v>
       </c>
       <c r="L28" s="1" t="n">
-        <v>18545</v>
+        <v>18521</v>
+      </c>
+      <c r="M28" s="1" t="n">
+        <v>47622</v>
+      </c>
+      <c r="N28" s="1" t="n">
+        <v>29105</v>
+      </c>
+      <c r="O28" s="1" t="n">
+        <v>18521</v>
       </c>
     </row>
     <row r="29">
@@ -1599,35 +1952,50 @@
       </c>
       <c r="C29" s="1" t="inlineStr">
         <is>
-          <t>중단영업 1우선주기본주당이익(손실) (단위 : 원)</t>
-        </is>
-      </c>
-      <c r="D29" s="1" t="n">
-        <v>-1910</v>
-      </c>
-      <c r="E29" s="1" t="n">
-        <v>-576</v>
-      </c>
-      <c r="F29" s="1" t="n">
-        <v>457</v>
+          <t>중단영업 보통주기본주당이익(손실) (단위: 원)</t>
+        </is>
+      </c>
+      <c r="D29" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E29" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F29" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="G29" s="1" t="n">
-        <v>-1910</v>
+        <v>-1919</v>
       </c>
       <c r="H29" s="1" t="n">
-        <v>-576</v>
+        <v>-584</v>
       </c>
       <c r="I29" s="1" t="n">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="J29" s="1" t="n">
-        <v>-1910</v>
+        <v>-1919</v>
       </c>
       <c r="K29" s="1" t="n">
-        <v>-576</v>
+        <v>-584</v>
       </c>
       <c r="L29" s="1" t="n">
-        <v>457</v>
+        <v>458</v>
+      </c>
+      <c r="M29" s="1" t="n">
+        <v>-1919</v>
+      </c>
+      <c r="N29" s="1" t="n">
+        <v>-584</v>
+      </c>
+      <c r="O29" s="1" t="n">
+        <v>458</v>
       </c>
     </row>
     <row r="30">
@@ -1638,10 +2006,14 @@
       </c>
       <c r="B30" s="1" t="inlineStr">
         <is>
-          <t>희석주당이익(손실)(단위 : 원)</t>
-        </is>
-      </c>
-      <c r="C30" s="1" t="n"/>
+          <t>기본주당이익 (단위 :원)</t>
+        </is>
+      </c>
+      <c r="C30" s="1" t="inlineStr">
+        <is>
+          <t>1우선주 기본주당이익(손실) (단위 : 원)</t>
+        </is>
+      </c>
       <c r="D30" s="7" t="inlineStr">
         <is>
           <t>-</t>
@@ -1657,35 +2029,32 @@
           <t>-</t>
         </is>
       </c>
-      <c r="G30" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H30" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I30" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J30" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K30" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L30" s="7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="G30" s="1" t="n">
+        <v>45535</v>
+      </c>
+      <c r="H30" s="1" t="n">
+        <v>28207</v>
+      </c>
+      <c r="I30" s="1" t="n">
+        <v>19002</v>
+      </c>
+      <c r="J30" s="1" t="n">
+        <v>45535</v>
+      </c>
+      <c r="K30" s="1" t="n">
+        <v>28207</v>
+      </c>
+      <c r="L30" s="1" t="n">
+        <v>19002</v>
+      </c>
+      <c r="M30" s="1" t="n">
+        <v>45535</v>
+      </c>
+      <c r="N30" s="1" t="n">
+        <v>28207</v>
+      </c>
+      <c r="O30" s="1" t="n">
+        <v>19002</v>
       </c>
     </row>
     <row r="31">
@@ -1696,40 +2065,55 @@
       </c>
       <c r="B31" s="1" t="inlineStr">
         <is>
-          <t>희석주당이익(손실)(단위 : 원)</t>
+          <t>기본주당이익 (단위 :원)</t>
         </is>
       </c>
       <c r="C31" s="1" t="inlineStr">
         <is>
-          <t>보통주 희석주당이익 (단위 : 원)</t>
-        </is>
-      </c>
-      <c r="D31" s="1" t="n">
-        <v>45703</v>
-      </c>
-      <c r="E31" s="1" t="n">
-        <v>28521</v>
-      </c>
-      <c r="F31" s="1" t="n">
-        <v>18979</v>
+          <t>계속영업 1우선주기본주당이익(손실) (단위 : 원)</t>
+        </is>
+      </c>
+      <c r="D31" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E31" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F31" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="G31" s="1" t="n">
-        <v>45703</v>
+        <v>47445</v>
       </c>
       <c r="H31" s="1" t="n">
-        <v>28521</v>
+        <v>28783</v>
       </c>
       <c r="I31" s="1" t="n">
-        <v>18979</v>
+        <v>18545</v>
       </c>
       <c r="J31" s="1" t="n">
-        <v>45703</v>
+        <v>47445</v>
       </c>
       <c r="K31" s="1" t="n">
-        <v>28521</v>
+        <v>28783</v>
       </c>
       <c r="L31" s="1" t="n">
-        <v>18979</v>
+        <v>18545</v>
+      </c>
+      <c r="M31" s="1" t="n">
+        <v>47445</v>
+      </c>
+      <c r="N31" s="1" t="n">
+        <v>28783</v>
+      </c>
+      <c r="O31" s="1" t="n">
+        <v>18545</v>
       </c>
     </row>
     <row r="32">
@@ -1740,49 +2124,664 @@
       </c>
       <c r="B32" s="1" t="inlineStr">
         <is>
+          <t>기본주당이익 (단위 :원)</t>
+        </is>
+      </c>
+      <c r="C32" s="1" t="inlineStr">
+        <is>
+          <t>중단영업 1우선주기본주당이익(손실) (단위 : 원)</t>
+        </is>
+      </c>
+      <c r="D32" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E32" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F32" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G32" s="1" t="n">
+        <v>-1910</v>
+      </c>
+      <c r="H32" s="1" t="n">
+        <v>-576</v>
+      </c>
+      <c r="I32" s="1" t="n">
+        <v>457</v>
+      </c>
+      <c r="J32" s="1" t="n">
+        <v>-1910</v>
+      </c>
+      <c r="K32" s="1" t="n">
+        <v>-576</v>
+      </c>
+      <c r="L32" s="1" t="n">
+        <v>457</v>
+      </c>
+      <c r="M32" s="1" t="n">
+        <v>-1910</v>
+      </c>
+      <c r="N32" s="1" t="n">
+        <v>-576</v>
+      </c>
+      <c r="O32" s="1" t="n">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>주당이익</t>
+        </is>
+      </c>
+      <c r="B33" s="1" t="inlineStr">
+        <is>
           <t>희석주당이익(손실)(단위 : 원)</t>
         </is>
       </c>
-      <c r="C32" s="1" t="inlineStr">
+      <c r="C33" s="1" t="n"/>
+      <c r="D33" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E33" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F33" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G33" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H33" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I33" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J33" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K33" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L33" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M33" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N33" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O33" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>주당이익</t>
+        </is>
+      </c>
+      <c r="B34" s="1" t="inlineStr">
+        <is>
+          <t>희석주당이익(손실)(단위 : 원)</t>
+        </is>
+      </c>
+      <c r="C34" s="1" t="inlineStr">
+        <is>
+          <t>보통주 희석주당이익 (단위 : 원)</t>
+        </is>
+      </c>
+      <c r="D34" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E34" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F34" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G34" s="1" t="n">
+        <v>45703</v>
+      </c>
+      <c r="H34" s="1" t="n">
+        <v>28521</v>
+      </c>
+      <c r="I34" s="1" t="n">
+        <v>18979</v>
+      </c>
+      <c r="J34" s="1" t="n">
+        <v>45703</v>
+      </c>
+      <c r="K34" s="1" t="n">
+        <v>28521</v>
+      </c>
+      <c r="L34" s="1" t="n">
+        <v>18979</v>
+      </c>
+      <c r="M34" s="1" t="n">
+        <v>45703</v>
+      </c>
+      <c r="N34" s="1" t="n">
+        <v>28521</v>
+      </c>
+      <c r="O34" s="1" t="n">
+        <v>18979</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>주당이익</t>
+        </is>
+      </c>
+      <c r="B35" s="1" t="inlineStr">
+        <is>
+          <t>희석주당이익(손실)(단위 : 원)</t>
+        </is>
+      </c>
+      <c r="C35" s="1" t="inlineStr">
         <is>
           <t>1우선주 희석주당이익 (단위 : 원)</t>
         </is>
       </c>
-      <c r="D32" s="1" t="n">
+      <c r="D35" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E35" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F35" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G35" s="1" t="n">
         <v>45535</v>
       </c>
-      <c r="E32" s="1" t="n">
+      <c r="H35" s="1" t="n">
         <v>28207</v>
       </c>
-      <c r="F32" s="1" t="n">
+      <c r="I35" s="1" t="n">
         <v>19002</v>
       </c>
-      <c r="G32" s="1" t="n">
+      <c r="J35" s="1" t="n">
         <v>45535</v>
       </c>
-      <c r="H32" s="1" t="n">
+      <c r="K35" s="1" t="n">
         <v>28207</v>
       </c>
-      <c r="I32" s="1" t="n">
+      <c r="L35" s="1" t="n">
         <v>19002</v>
       </c>
-      <c r="J32" s="1" t="n">
+      <c r="M35" s="1" t="n">
         <v>45535</v>
       </c>
-      <c r="K32" s="1" t="n">
+      <c r="N35" s="1" t="n">
         <v>28207</v>
       </c>
-      <c r="L32" s="1" t="n">
+      <c r="O35" s="1" t="n">
         <v>19002</v>
       </c>
     </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>매출액</t>
+        </is>
+      </c>
+      <c r="B36" s="1" t="n"/>
+      <c r="C36" s="1" t="n"/>
+      <c r="D36" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E36" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F36" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G36" s="1" t="n">
+        <v>162663579</v>
+      </c>
+      <c r="H36" s="1" t="n">
+        <v>142151469</v>
+      </c>
+      <c r="I36" s="1" t="n">
+        <v>116448159</v>
+      </c>
+      <c r="J36" s="1" t="n">
+        <v>162663579</v>
+      </c>
+      <c r="K36" s="1" t="n">
+        <v>142151469</v>
+      </c>
+      <c r="L36" s="1" t="n">
+        <v>116448159</v>
+      </c>
+      <c r="M36" s="1" t="n">
+        <v>162663579</v>
+      </c>
+      <c r="N36" s="1" t="n">
+        <v>142151469</v>
+      </c>
+      <c r="O36" s="1" t="n">
+        <v>116448159</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>공동기업및관계기업투자손익</t>
+        </is>
+      </c>
+      <c r="B37" s="1" t="n"/>
+      <c r="C37" s="1" t="n"/>
+      <c r="D37" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E37" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F37" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G37" s="1" t="n">
+        <v>2470933</v>
+      </c>
+      <c r="H37" s="1" t="n">
+        <v>1557630</v>
+      </c>
+      <c r="I37" s="1" t="n">
+        <v>1302150</v>
+      </c>
+      <c r="J37" s="1" t="n">
+        <v>2470933</v>
+      </c>
+      <c r="K37" s="1" t="n">
+        <v>1557630</v>
+      </c>
+      <c r="L37" s="1" t="n">
+        <v>1302150</v>
+      </c>
+      <c r="M37" s="1" t="n">
+        <v>2470933</v>
+      </c>
+      <c r="N37" s="1" t="n">
+        <v>1557630</v>
+      </c>
+      <c r="O37" s="1" t="n">
+        <v>1302150</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>기타수익</t>
+        </is>
+      </c>
+      <c r="B38" s="1" t="n"/>
+      <c r="C38" s="1" t="n"/>
+      <c r="D38" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E38" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F38" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G38" s="1" t="n">
+        <v>1782333</v>
+      </c>
+      <c r="H38" s="1" t="n">
+        <v>1930914</v>
+      </c>
+      <c r="I38" s="1" t="n">
+        <v>1377997</v>
+      </c>
+      <c r="J38" s="1" t="n">
+        <v>1782333</v>
+      </c>
+      <c r="K38" s="1" t="n">
+        <v>1930914</v>
+      </c>
+      <c r="L38" s="1" t="n">
+        <v>1377997</v>
+      </c>
+      <c r="M38" s="1" t="n">
+        <v>1782333</v>
+      </c>
+      <c r="N38" s="1" t="n">
+        <v>1930914</v>
+      </c>
+      <c r="O38" s="1" t="n">
+        <v>1377997</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>기타비용</t>
+        </is>
+      </c>
+      <c r="B39" s="1" t="n"/>
+      <c r="C39" s="1" t="n"/>
+      <c r="D39" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E39" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F39" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G39" s="1" t="n">
+        <v>2350343</v>
+      </c>
+      <c r="H39" s="1" t="n">
+        <v>2238256</v>
+      </c>
+      <c r="I39" s="1" t="n">
+        <v>1745985</v>
+      </c>
+      <c r="J39" s="1" t="n">
+        <v>2350343</v>
+      </c>
+      <c r="K39" s="1" t="n">
+        <v>2238256</v>
+      </c>
+      <c r="L39" s="1" t="n">
+        <v>1745985</v>
+      </c>
+      <c r="M39" s="1" t="n">
+        <v>2350343</v>
+      </c>
+      <c r="N39" s="1" t="n">
+        <v>2238256</v>
+      </c>
+      <c r="O39" s="1" t="n">
+        <v>1745985</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>법인세비용차감전순이익</t>
+        </is>
+      </c>
+      <c r="B40" s="1" t="n"/>
+      <c r="C40" s="1" t="n"/>
+      <c r="D40" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E40" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F40" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G40" s="1" t="n">
+        <v>17618662</v>
+      </c>
+      <c r="H40" s="1" t="n">
+        <v>11181471</v>
+      </c>
+      <c r="I40" s="1" t="n">
+        <v>7789043</v>
+      </c>
+      <c r="J40" s="1" t="n">
+        <v>17618662</v>
+      </c>
+      <c r="K40" s="1" t="n">
+        <v>11181471</v>
+      </c>
+      <c r="L40" s="1" t="n">
+        <v>7789043</v>
+      </c>
+      <c r="M40" s="1" t="n">
+        <v>17618662</v>
+      </c>
+      <c r="N40" s="1" t="n">
+        <v>11181471</v>
+      </c>
+      <c r="O40" s="1" t="n">
+        <v>7789043</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>계속영업연결당기순이익</t>
+        </is>
+      </c>
+      <c r="B41" s="1" t="n"/>
+      <c r="C41" s="1" t="n"/>
+      <c r="D41" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E41" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F41" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G41" s="1" t="n">
+        <v>12992022</v>
+      </c>
+      <c r="H41" s="1" t="n">
+        <v>8202303</v>
+      </c>
+      <c r="I41" s="1" t="n">
+        <v>5522220</v>
+      </c>
+      <c r="J41" s="1" t="n">
+        <v>12992022</v>
+      </c>
+      <c r="K41" s="1" t="n">
+        <v>8202303</v>
+      </c>
+      <c r="L41" s="1" t="n">
+        <v>5522220</v>
+      </c>
+      <c r="M41" s="1" t="n">
+        <v>12992022</v>
+      </c>
+      <c r="N41" s="1" t="n">
+        <v>8202303</v>
+      </c>
+      <c r="O41" s="1" t="n">
+        <v>5522220</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>중단영업당기순이익(손실)</t>
+        </is>
+      </c>
+      <c r="B42" s="1" t="n"/>
+      <c r="C42" s="1" t="n"/>
+      <c r="D42" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E42" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F42" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G42" s="1" t="n">
+        <v>-719721</v>
+      </c>
+      <c r="H42" s="1" t="n">
+        <v>-218689</v>
+      </c>
+      <c r="I42" s="1" t="n">
+        <v>170857</v>
+      </c>
+      <c r="J42" s="1" t="n">
+        <v>-719721</v>
+      </c>
+      <c r="K42" s="1" t="n">
+        <v>-218689</v>
+      </c>
+      <c r="L42" s="1" t="n">
+        <v>170857</v>
+      </c>
+      <c r="M42" s="1" t="n">
+        <v>-719721</v>
+      </c>
+      <c r="N42" s="1" t="n">
+        <v>-218689</v>
+      </c>
+      <c r="O42" s="1" t="n">
+        <v>170857</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>연결당기순이익</t>
+        </is>
+      </c>
+      <c r="B43" s="1" t="n"/>
+      <c r="C43" s="1" t="n"/>
+      <c r="D43" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E43" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F43" s="7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G43" s="1" t="n">
+        <v>12272301</v>
+      </c>
+      <c r="H43" s="1" t="n">
+        <v>7983614</v>
+      </c>
+      <c r="I43" s="1" t="n">
+        <v>5693077</v>
+      </c>
+      <c r="J43" s="1" t="n">
+        <v>12272301</v>
+      </c>
+      <c r="K43" s="1" t="n">
+        <v>7983614</v>
+      </c>
+      <c r="L43" s="1" t="n">
+        <v>5693077</v>
+      </c>
+      <c r="M43" s="1" t="n">
+        <v>12272301</v>
+      </c>
+      <c r="N43" s="1" t="n">
+        <v>7983614</v>
+      </c>
+      <c r="O43" s="1" t="n">
+        <v>5693077</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="J1:L1"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="D1:F1"/>
     <mergeCell ref="G1:I1"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="A2:C2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>